<commit_message>
Added code for Powers
</commit_message>
<xml_diff>
--- a/DND4eCharacterGenerator/Assets/ScrapeData.xlsx
+++ b/DND4eCharacterGenerator/Assets/ScrapeData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="9510" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="9510" firstSheet="6" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Referencer" sheetId="10" r:id="rId1"/>
@@ -190,7 +190,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3967" uniqueCount="2070">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4064" uniqueCount="2130">
   <si>
     <t>Source</t>
   </si>
@@ -6961,6 +6961,191 @@
       </rPr>
       <t>", a property that makes the worlds collective primal energy resist entry into the world by the cosmos most powerful beings. The gods then had no choice but to try to influence the world indirectly through their believers and servants. Great weapons and monsters created during the Dawn War still remains, scattered throughout the planes, and are the center of many a plot.</t>
     </r>
+  </si>
+  <si>
+    <t>Abberrant-Bane Strike</t>
+  </si>
+  <si>
+    <t>You strike at your horrid enemy, using your knowledge of its strengths and weaknesses to twist the knife just a bit more.</t>
+  </si>
+  <si>
+    <t>Power Type</t>
+  </si>
+  <si>
+    <t>Source Types</t>
+  </si>
+  <si>
+    <t>Martial|Weapon</t>
+  </si>
+  <si>
+    <t>Action Type</t>
+  </si>
+  <si>
+    <t>Standard Action</t>
+  </si>
+  <si>
+    <t>Weapon Type</t>
+  </si>
+  <si>
+    <t>Weapon Types</t>
+  </si>
+  <si>
+    <t>Prerequisites</t>
+  </si>
+  <si>
+    <t>Prerequisite Type</t>
+  </si>
+  <si>
+    <t>Prereq Def</t>
+  </si>
+  <si>
+    <t>You must be trained in Dungeoneering</t>
+  </si>
+  <si>
+    <t>Target #</t>
+  </si>
+  <si>
+    <t>One</t>
+  </si>
+  <si>
+    <t>Target Type</t>
+  </si>
+  <si>
+    <t>Creature</t>
+  </si>
+  <si>
+    <t>Attack Type</t>
+  </si>
+  <si>
+    <t>Dex</t>
+  </si>
+  <si>
+    <t>Attack vs type</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>Hit</t>
+  </si>
+  <si>
+    <t>1[W] + Dexterity modifier damage. If the target is aberrant and has resistance or vulnerability to your attack, you gain a bonus to damage equal to your Wisdom modifier.
+Level 21: 2[W] + Dexterity modifier damage.</t>
+  </si>
+  <si>
+    <t>Acid Orb</t>
+  </si>
+  <si>
+    <t>Class level</t>
+  </si>
+  <si>
+    <t>Acid|Arcane|Implement</t>
+  </si>
+  <si>
+    <t>Ranged 20</t>
+  </si>
+  <si>
+    <t>Cha</t>
+  </si>
+  <si>
+    <t>1d10 + Charisma modifier acid damage.
+Level 21: "2d10 + Charisma modifier acid damage.</t>
+  </si>
+  <si>
+    <t>Acrobat's Trick</t>
+  </si>
+  <si>
+    <t>You must have the selected Acrobat's trick as part of the Rogue's Trick class feature.</t>
+  </si>
+  <si>
+    <t>Move Action</t>
+  </si>
+  <si>
+    <t>Personal</t>
+  </si>
+  <si>
+    <t>You move up to your speed -2. During this move, you have a climb speed equal to your speed -2. You also gain a +2 power bonus to your next damage roll with a basic attack during this turn.
+Level 11: +4 power bonus.
+Level 21: +6 power bonus.</t>
+  </si>
+  <si>
+    <t>Acrobatic Strike</t>
+  </si>
+  <si>
+    <t>MP2</t>
+  </si>
+  <si>
+    <t>Utility</t>
+  </si>
+  <si>
+    <t>Power usage</t>
+  </si>
+  <si>
+    <t>Light Blade</t>
+  </si>
+  <si>
+    <t>Requirement</t>
+  </si>
+  <si>
+    <t>Acrobatics</t>
+  </si>
+  <si>
+    <t>You must be trained in Acrobatics</t>
+  </si>
+  <si>
+    <t>Requirement Type</t>
+  </si>
+  <si>
+    <t>Requirement Def</t>
+  </si>
+  <si>
+    <t>You must be wielding a light blade in order to use.</t>
+  </si>
+  <si>
+    <t>Melee Weapon</t>
+  </si>
+  <si>
+    <t>Melee Weapon|Ranged Weapon</t>
+  </si>
+  <si>
+    <t>1[W] + Dexterity modifier ([DexMod]). If the target is aberrant and has resistance or vulnerability to your attack, you gain a bonus to damage equal to your Wisdom modifier ([WisMod]).
+Level 21: 2[W] + Dexterity modifier ([DexMod]).</t>
+  </si>
+  <si>
+    <t>Hit Description</t>
+  </si>
+  <si>
+    <t>Effect Description</t>
+  </si>
+  <si>
+    <t>Hit1</t>
+  </si>
+  <si>
+    <t>Hi1 level</t>
+  </si>
+  <si>
+    <t>1W|DexMod</t>
+  </si>
+  <si>
+    <t>2W|DexMod</t>
+  </si>
+  <si>
+    <t>1d10|ChaMod</t>
+  </si>
+  <si>
+    <t>2d10|ChaMod</t>
+  </si>
+  <si>
+    <t>Before or after the attack, you shift 1 square.</t>
+  </si>
+  <si>
+    <t>Rituals</t>
+  </si>
+  <si>
+    <t>Ritual</t>
+  </si>
+  <si>
+    <t>End Column</t>
   </si>
 </sst>
 </file>
@@ -8403,10 +8588,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8414,33 +8599,45 @@
     <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>676</v>
       </c>
       <c r="B1" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>2129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1600</v>
       </c>
       <c r="B2" s="3">
-        <f t="shared" ref="B2:B6" ca="1" si="0">COUNTA(INDIRECT(A2&amp;"!A:A"))-1</f>
+        <f ca="1">COUNTA(INDIRECT(A2&amp;"!A:A"))-1</f>
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="3" t="str">
+        <f ca="1">SUBSTITUTE(ADDRESS(1,COUNTA(INDIRECT(A2&amp;"!A1:ZZ1")),4),1,"")</f>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1595</v>
       </c>
       <c r="B3" s="3">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ref="B3:B6" ca="1" si="0">COUNTA(INDIRECT(A3&amp;"!A:A"))-1</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" s="3" t="str">
+        <f t="shared" ref="C3:C18" ca="1" si="1">SUBSTITUTE(ADDRESS(1,COUNTA(INDIRECT(A3&amp;"!A1:ZZ1")),4),1,"")</f>
+        <v>D</v>
+      </c>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1108</v>
       </c>
@@ -8448,8 +8645,13 @@
         <f t="shared" ca="1" si="0"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>E</v>
+      </c>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>848</v>
       </c>
@@ -8457,8 +8659,13 @@
         <f t="shared" ca="1" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>C</v>
+      </c>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>679</v>
       </c>
@@ -8466,17 +8673,27 @@
         <f t="shared" ca="1" si="0"/>
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>G</v>
+      </c>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>1107</v>
       </c>
       <c r="B7" s="3">
-        <f t="shared" ref="B7" ca="1" si="1">COUNTA(INDIRECT(A7&amp;"!A:A"))-1</f>
+        <f t="shared" ref="B7" ca="1" si="2">COUNTA(INDIRECT(A7&amp;"!A:A"))-1</f>
         <v>47</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>BG</v>
+      </c>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1080</v>
       </c>
@@ -8484,8 +8701,13 @@
         <f ca="1">COUNTA(INDIRECT(A8&amp;"!A:A"))-1</f>
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>J</v>
+      </c>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1106</v>
       </c>
@@ -8493,26 +8715,40 @@
         <f ca="1">COUNTA(INDIRECT(A9&amp;"!A:A"))-1</f>
         <v>85</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>H</v>
+      </c>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>680</v>
       </c>
       <c r="B10" s="3">
-        <f t="shared" ref="B10:B17" ca="1" si="2">COUNTA(INDIRECT(A10&amp;"!A:A"))-1</f>
+        <f t="shared" ref="B10:B17" ca="1" si="3">COUNTA(INDIRECT(A10&amp;"!A:A"))-1</f>
         <v>46</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>AE</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>837</v>
       </c>
       <c r="B11" s="3">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>D</v>
+      </c>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>686</v>
       </c>
@@ -8520,51 +8756,95 @@
         <f ca="1">COUNTA(INDIRECT(A12&amp;"!A:A"))-1</f>
         <v>112</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>D</v>
+      </c>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>681</v>
       </c>
       <c r="B13" s="3">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>A</v>
+      </c>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>682</v>
       </c>
       <c r="B14" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="C14" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>A</v>
+      </c>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>683</v>
       </c>
       <c r="B15" s="3">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>105</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>F</v>
+      </c>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>684</v>
       </c>
       <c r="B16" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="C16" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Y</v>
+      </c>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>685</v>
       </c>
       <c r="B17" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
-      </c>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="C17" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>A</v>
+      </c>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>2127</v>
+      </c>
+      <c r="B18">
+        <f ca="1">COUNTA(INDIRECT(A18&amp;"!A:A"))-1</f>
+        <v>0</v>
+      </c>
+      <c r="C18" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>A</v>
+      </c>
+      <c r="D18" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8577,10 +8857,10 @@
   <dimension ref="A1:AK49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AB22" sqref="AB22"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11644,9 +11924,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11914,9 +12192,7 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:D113"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -13004,9 +13280,7 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:A24"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -15058,7 +15332,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15078,9 +15352,7 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:F106"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -16274,21 +16546,340 @@
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <sheetPr codeName="Sheet9"/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:Y5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="Y1" sqref="Y1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="9.140625" style="3"/>
+    <col min="21" max="23" width="9.140625" style="3"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>690</v>
       </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>687</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2094</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>2072</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2107</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2073</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2075</v>
+      </c>
+      <c r="J1" t="s">
+        <v>2078</v>
+      </c>
+      <c r="K1" t="s">
+        <v>2079</v>
+      </c>
+      <c r="L1" t="s">
+        <v>2080</v>
+      </c>
+      <c r="M1" t="s">
+        <v>2081</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>2109</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>2112</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>2113</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>2083</v>
+      </c>
+      <c r="R1" t="s">
+        <v>2085</v>
+      </c>
+      <c r="S1" t="s">
+        <v>2087</v>
+      </c>
+      <c r="T1" t="s">
+        <v>2089</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>2091</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>2120</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>2121</v>
+      </c>
+      <c r="X1" t="s">
+        <v>2118</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>2119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2070</v>
+      </c>
+      <c r="B2" t="s">
+        <v>700</v>
+      </c>
+      <c r="C2" t="s">
+        <v>731</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2071</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>754</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1084</v>
+      </c>
+      <c r="H2" t="s">
+        <v>2074</v>
+      </c>
+      <c r="I2" t="s">
+        <v>2076</v>
+      </c>
+      <c r="J2" t="s">
+        <v>2116</v>
+      </c>
+      <c r="K2" t="s">
+        <v>390</v>
+      </c>
+      <c r="L2" t="s">
+        <v>1083</v>
+      </c>
+      <c r="M2" t="s">
+        <v>2082</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>2084</v>
+      </c>
+      <c r="R2" t="s">
+        <v>2086</v>
+      </c>
+      <c r="S2" t="s">
+        <v>2088</v>
+      </c>
+      <c r="T2" t="s">
+        <v>2090</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>2122</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>2123</v>
+      </c>
+      <c r="W2" s="3">
+        <v>21</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>2117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2093</v>
+      </c>
+      <c r="B3" t="s">
+        <v>746</v>
+      </c>
+      <c r="C3" t="s">
+        <v>738</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>754</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1084</v>
+      </c>
+      <c r="H3" t="s">
+        <v>2095</v>
+      </c>
+      <c r="I3" t="s">
+        <v>2076</v>
+      </c>
+      <c r="J3" t="s">
+        <v>2096</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>2084</v>
+      </c>
+      <c r="R3" t="s">
+        <v>2086</v>
+      </c>
+      <c r="S3" t="s">
+        <v>2097</v>
+      </c>
+      <c r="T3" t="s">
+        <v>752</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>2124</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>2125</v>
+      </c>
+      <c r="W3" s="3">
+        <v>21</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>2098</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2099</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>1774</v>
+      </c>
+      <c r="C4" t="s">
+        <v>731</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>2106</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1084</v>
+      </c>
+      <c r="H4" t="s">
+        <v>711</v>
+      </c>
+      <c r="I4" t="s">
+        <v>2101</v>
+      </c>
+      <c r="K4" t="s">
+        <v>2099</v>
+      </c>
+      <c r="L4" t="s">
+        <v>844</v>
+      </c>
+      <c r="M4" t="s">
+        <v>2100</v>
+      </c>
+      <c r="R4" t="s">
+        <v>2102</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>2103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2104</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2105</v>
+      </c>
+      <c r="C5" t="s">
+        <v>731</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2071</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>754</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1084</v>
+      </c>
+      <c r="H5" t="s">
+        <v>2074</v>
+      </c>
+      <c r="I5" t="s">
+        <v>2076</v>
+      </c>
+      <c r="J5" t="s">
+        <v>2115</v>
+      </c>
+      <c r="K5" t="s">
+        <v>2110</v>
+      </c>
+      <c r="L5" t="s">
+        <v>1083</v>
+      </c>
+      <c r="M5" t="s">
+        <v>2111</v>
+      </c>
+      <c r="N5" t="s">
+        <v>2108</v>
+      </c>
+      <c r="O5" t="s">
+        <v>2077</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>2114</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>2084</v>
+      </c>
+      <c r="R5" t="s">
+        <v>2086</v>
+      </c>
+      <c r="S5" t="s">
+        <v>2088</v>
+      </c>
+      <c r="T5" t="s">
+        <v>2090</v>
+      </c>
+      <c r="U5" s="3" t="s">
+        <v>2122</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>2123</v>
+      </c>
+      <c r="W5" s="3">
+        <v>21</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>2092</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>2126</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -16318,7 +16909,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16488,10 +17079,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE883B56-0E73-42B4-A478-5009BC784D1A}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2128</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -16502,7 +17101,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16595,8 +17194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16699,7 +17298,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16781,7 +17380,7 @@
   <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17450,10 +18049,10 @@
   <dimension ref="A1:BH49"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AK2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AZ12" sqref="AZ12"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25040,9 +25639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -25584,7 +26181,7 @@
   <dimension ref="A1:H86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25611,6 +26208,9 @@
       <c r="E1" t="s">
         <v>1027</v>
       </c>
+      <c r="F1" t="s">
+        <v>692</v>
+      </c>
       <c r="G1" t="s">
         <v>1028</v>
       </c>

</xml_diff>

<commit_message>
First build of Power Cards
</commit_message>
<xml_diff>
--- a/DND4eCharacterGenerator/Assets/ScrapeData.xlsx
+++ b/DND4eCharacterGenerator/Assets/ScrapeData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="9510" firstSheet="6" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="9510" firstSheet="14" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Referencer" sheetId="10" r:id="rId1"/>
@@ -27,14 +27,15 @@
     <sheet name="Traits" sheetId="8" r:id="rId13"/>
     <sheet name="Subraces" sheetId="9" r:id="rId14"/>
     <sheet name="Subracedatafix" sheetId="12" r:id="rId15"/>
-    <sheet name="Items" sheetId="4" r:id="rId16"/>
-    <sheet name="Feats" sheetId="5" r:id="rId17"/>
-    <sheet name="Powers" sheetId="6" r:id="rId18"/>
-    <sheet name="Spells" sheetId="7" r:id="rId19"/>
-    <sheet name="Rituals" sheetId="23" r:id="rId20"/>
+    <sheet name="Sheet1" sheetId="24" r:id="rId16"/>
+    <sheet name="Items" sheetId="4" r:id="rId17"/>
+    <sheet name="Feats" sheetId="5" r:id="rId18"/>
+    <sheet name="Powers" sheetId="6" r:id="rId19"/>
+    <sheet name="Spells" sheetId="7" r:id="rId20"/>
+    <sheet name="Rituals" sheetId="23" r:id="rId21"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId21"/>
+    <externalReference r:id="rId22"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Deities!$A$1:$E$86</definedName>
@@ -190,7 +191,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4064" uniqueCount="2130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4064" uniqueCount="2128">
   <si>
     <t>Source</t>
   </si>
@@ -7042,9 +7043,6 @@
     <t>Acid|Arcane|Implement</t>
   </si>
   <si>
-    <t>Ranged 20</t>
-  </si>
-  <si>
     <t>Cha</t>
   </si>
   <si>
@@ -7102,12 +7100,6 @@
     <t>You must be wielding a light blade in order to use.</t>
   </si>
   <si>
-    <t>Melee Weapon</t>
-  </si>
-  <si>
-    <t>Melee Weapon|Ranged Weapon</t>
-  </si>
-  <si>
     <t>1[W] + Dexterity modifier ([DexMod]). If the target is aberrant and has resistance or vulnerability to your attack, you gain a bonus to damage equal to your Wisdom modifier ([WisMod]).
 Level 21: 2[W] + Dexterity modifier ([DexMod]).</t>
   </si>
@@ -7146,6 +7138,9 @@
   </si>
   <si>
     <t>End Column</t>
+  </si>
+  <si>
+    <t>Melee|Ranged</t>
   </si>
 </sst>
 </file>
@@ -8607,7 +8602,7 @@
         <v>677</v>
       </c>
       <c r="C1" t="s">
-        <v>2129</v>
+        <v>2126</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -8834,7 +8829,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>2127</v>
+        <v>2124</v>
       </c>
       <c r="B18">
         <f ca="1">COUNTA(INDIRECT(A18&amp;"!A:A"))-1</f>
@@ -8860,7 +8855,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13496,7 +13491,7 @@
   <dimension ref="A1:E230"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15327,6 +15322,18 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5409F685-987D-421D-A06C-6C14318AD189}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1"/>
@@ -15347,7 +15354,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:F106"/>
@@ -16543,13 +16550,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:Y5"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="Y1" sqref="Y1"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16587,7 +16594,7 @@
         <v>2072</v>
       </c>
       <c r="G1" t="s">
-        <v>2107</v>
+        <v>2106</v>
       </c>
       <c r="H1" t="s">
         <v>2073</v>
@@ -16608,13 +16615,13 @@
         <v>2081</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>2109</v>
+        <v>2108</v>
       </c>
       <c r="O1" s="3" t="s">
+        <v>2111</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>2112</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>2113</v>
       </c>
       <c r="Q1" t="s">
         <v>2083</v>
@@ -16632,16 +16639,16 @@
         <v>2091</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>2120</v>
+        <v>2117</v>
       </c>
       <c r="W1" s="3" t="s">
-        <v>2121</v>
+        <v>2118</v>
       </c>
       <c r="X1" t="s">
-        <v>2118</v>
+        <v>2115</v>
       </c>
       <c r="Y1" t="s">
-        <v>2119</v>
+        <v>2116</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
@@ -16673,7 +16680,7 @@
         <v>2076</v>
       </c>
       <c r="J2" t="s">
-        <v>2116</v>
+        <v>2127</v>
       </c>
       <c r="K2" t="s">
         <v>390</v>
@@ -16697,16 +16704,16 @@
         <v>2090</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>2122</v>
+        <v>2119</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>2123</v>
+        <v>2120</v>
       </c>
       <c r="W2" s="3">
         <v>21</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>2117</v>
+        <v>2114</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -16735,7 +16742,7 @@
         <v>2076</v>
       </c>
       <c r="J3" t="s">
-        <v>2096</v>
+        <v>758</v>
       </c>
       <c r="Q3" t="s">
         <v>2084</v>
@@ -16744,27 +16751,27 @@
         <v>2086</v>
       </c>
       <c r="S3" t="s">
-        <v>2097</v>
+        <v>2096</v>
       </c>
       <c r="T3" t="s">
         <v>752</v>
       </c>
       <c r="U3" s="3" t="s">
-        <v>2124</v>
+        <v>2121</v>
       </c>
       <c r="V3" s="3" t="s">
-        <v>2125</v>
+        <v>2122</v>
       </c>
       <c r="W3" s="3">
         <v>21</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2099</v>
+        <v>2098</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>1774</v>
@@ -16773,7 +16780,7 @@
         <v>731</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>2106</v>
+        <v>2105</v>
       </c>
       <c r="G4" t="s">
         <v>1084</v>
@@ -16782,30 +16789,30 @@
         <v>711</v>
       </c>
       <c r="I4" t="s">
-        <v>2101</v>
+        <v>2100</v>
       </c>
       <c r="K4" t="s">
-        <v>2099</v>
+        <v>2098</v>
       </c>
       <c r="L4" t="s">
         <v>844</v>
       </c>
       <c r="M4" t="s">
-        <v>2100</v>
+        <v>2099</v>
       </c>
       <c r="R4" t="s">
+        <v>2101</v>
+      </c>
+      <c r="Y4" s="1" t="s">
         <v>2102</v>
-      </c>
-      <c r="Y4" s="1" t="s">
-        <v>2103</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>2103</v>
+      </c>
+      <c r="B5" t="s">
         <v>2104</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2105</v>
       </c>
       <c r="C5" t="s">
         <v>731</v>
@@ -16829,25 +16836,25 @@
         <v>2076</v>
       </c>
       <c r="J5" t="s">
-        <v>2115</v>
+        <v>757</v>
       </c>
       <c r="K5" t="s">
-        <v>2110</v>
+        <v>2109</v>
       </c>
       <c r="L5" t="s">
         <v>1083</v>
       </c>
       <c r="M5" t="s">
-        <v>2111</v>
+        <v>2110</v>
       </c>
       <c r="N5" t="s">
-        <v>2108</v>
+        <v>2107</v>
       </c>
       <c r="O5" t="s">
         <v>2077</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>2114</v>
+        <v>2113</v>
       </c>
       <c r="Q5" t="s">
         <v>2084</v>
@@ -16862,10 +16869,10 @@
         <v>2090</v>
       </c>
       <c r="U5" s="3" t="s">
-        <v>2122</v>
+        <v>2119</v>
       </c>
       <c r="V5" s="3" t="s">
-        <v>2123</v>
+        <v>2120</v>
       </c>
       <c r="W5" s="3">
         <v>21</v>
@@ -16874,33 +16881,12 @@
         <v>2092</v>
       </c>
       <c r="Y5" s="1" t="s">
-        <v>2126</v>
+        <v>2123</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <sheetPr codeName="Sheet10"/>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X26" sqref="X26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>691</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -17076,10 +17062,31 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+  <sheetPr codeName="Sheet10"/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="X26" sqref="X26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>691</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE883B56-0E73-42B4-A478-5009BC784D1A}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
@@ -17087,7 +17094,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2128</v>
+        <v>2125</v>
       </c>
     </row>
   </sheetData>
@@ -18052,7 +18059,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Autopopulate Power Card from Powers via binding
</commit_message>
<xml_diff>
--- a/DND4eCharacterGenerator/Assets/ScrapeData.xlsx
+++ b/DND4eCharacterGenerator/Assets/ScrapeData.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="9510" firstSheet="14" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="9510" firstSheet="4" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Referencer" sheetId="10" r:id="rId1"/>
@@ -27,15 +27,14 @@
     <sheet name="Traits" sheetId="8" r:id="rId13"/>
     <sheet name="Subraces" sheetId="9" r:id="rId14"/>
     <sheet name="Subracedatafix" sheetId="12" r:id="rId15"/>
-    <sheet name="Sheet1" sheetId="24" r:id="rId16"/>
-    <sheet name="Items" sheetId="4" r:id="rId17"/>
-    <sheet name="Feats" sheetId="5" r:id="rId18"/>
-    <sheet name="Powers" sheetId="6" r:id="rId19"/>
-    <sheet name="Spells" sheetId="7" r:id="rId20"/>
-    <sheet name="Rituals" sheetId="23" r:id="rId21"/>
+    <sheet name="Items" sheetId="4" r:id="rId16"/>
+    <sheet name="Feats" sheetId="5" r:id="rId17"/>
+    <sheet name="Powers" sheetId="6" r:id="rId18"/>
+    <sheet name="Spells" sheetId="7" r:id="rId19"/>
+    <sheet name="Rituals" sheetId="23" r:id="rId20"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId22"/>
+    <externalReference r:id="rId21"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Deities!$A$1:$E$86</definedName>
@@ -191,7 +190,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4064" uniqueCount="2128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4087" uniqueCount="2141">
   <si>
     <t>Source</t>
   </si>
@@ -6973,12 +6972,6 @@
     <t>Power Type</t>
   </si>
   <si>
-    <t>Source Types</t>
-  </si>
-  <si>
-    <t>Martial|Weapon</t>
-  </si>
-  <si>
     <t>Action Type</t>
   </si>
   <si>
@@ -6988,66 +6981,25 @@
     <t>Weapon Type</t>
   </si>
   <si>
-    <t>Weapon Types</t>
-  </si>
-  <si>
     <t>Prerequisites</t>
   </si>
   <si>
     <t>Prerequisite Type</t>
   </si>
   <si>
-    <t>Prereq Def</t>
-  </si>
-  <si>
     <t>You must be trained in Dungeoneering</t>
   </si>
   <si>
-    <t>Target #</t>
-  </si>
-  <si>
-    <t>One</t>
-  </si>
-  <si>
-    <t>Target Type</t>
-  </si>
-  <si>
-    <t>Creature</t>
-  </si>
-  <si>
     <t>Attack Type</t>
   </si>
   <si>
-    <t>Dex</t>
-  </si>
-  <si>
     <t>Attack vs type</t>
   </si>
   <si>
     <t>AC</t>
   </si>
   <si>
-    <t>Hit</t>
-  </si>
-  <si>
-    <t>1[W] + Dexterity modifier damage. If the target is aberrant and has resistance or vulnerability to your attack, you gain a bonus to damage equal to your Wisdom modifier.
-Level 21: 2[W] + Dexterity modifier damage.</t>
-  </si>
-  <si>
     <t>Acid Orb</t>
-  </si>
-  <si>
-    <t>Class level</t>
-  </si>
-  <si>
-    <t>Acid|Arcane|Implement</t>
-  </si>
-  <si>
-    <t>Cha</t>
-  </si>
-  <si>
-    <t>1d10 + Charisma modifier acid damage.
-Level 21: "2d10 + Charisma modifier acid damage.</t>
   </si>
   <si>
     <t>Acrobat's Trick</t>
@@ -7082,9 +7034,6 @@
     <t>Light Blade</t>
   </si>
   <si>
-    <t>Requirement</t>
-  </si>
-  <si>
     <t>Acrobatics</t>
   </si>
   <si>
@@ -7094,40 +7043,9 @@
     <t>Requirement Type</t>
   </si>
   <si>
-    <t>Requirement Def</t>
-  </si>
-  <si>
     <t>You must be wielding a light blade in order to use.</t>
   </si>
   <si>
-    <t>1[W] + Dexterity modifier ([DexMod]). If the target is aberrant and has resistance or vulnerability to your attack, you gain a bonus to damage equal to your Wisdom modifier ([WisMod]).
-Level 21: 2[W] + Dexterity modifier ([DexMod]).</t>
-  </si>
-  <si>
-    <t>Hit Description</t>
-  </si>
-  <si>
-    <t>Effect Description</t>
-  </si>
-  <si>
-    <t>Hit1</t>
-  </si>
-  <si>
-    <t>Hi1 level</t>
-  </si>
-  <si>
-    <t>1W|DexMod</t>
-  </si>
-  <si>
-    <t>2W|DexMod</t>
-  </si>
-  <si>
-    <t>1d10|ChaMod</t>
-  </si>
-  <si>
-    <t>2d10|ChaMod</t>
-  </si>
-  <si>
     <t>Before or after the attack, you shift 1 square.</t>
   </si>
   <si>
@@ -7141,6 +7059,126 @@
   </si>
   <si>
     <t>Melee|Ranged</t>
+  </si>
+  <si>
+    <t>One Creature</t>
+  </si>
+  <si>
+    <t>Dexterity vs AC</t>
+  </si>
+  <si>
+    <t>Charisma vs Reflexes</t>
+  </si>
+  <si>
+    <t>Augment</t>
+  </si>
+  <si>
+    <t>Origin</t>
+  </si>
+  <si>
+    <t>Origin Type</t>
+  </si>
+  <si>
+    <t>Weapon|Weapon</t>
+  </si>
+  <si>
+    <t>Method Ranges</t>
+  </si>
+  <si>
+    <t>Method Types</t>
+  </si>
+  <si>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>Flavor:</t>
+  </si>
+  <si>
+    <t>Prerequisite:</t>
+  </si>
+  <si>
+    <t>Special:</t>
+  </si>
+  <si>
+    <t>Requirement:</t>
+  </si>
+  <si>
+    <t>Requirements</t>
+  </si>
+  <si>
+    <t>Keywords:</t>
+  </si>
+  <si>
+    <t>Trigger:</t>
+  </si>
+  <si>
+    <t>Attack:</t>
+  </si>
+  <si>
+    <t>Hit:</t>
+  </si>
+  <si>
+    <t>First Failed Saving Throw:</t>
+  </si>
+  <si>
+    <t>Miss:</t>
+  </si>
+  <si>
+    <t>Second Failed Saving Throw:</t>
+  </si>
+  <si>
+    <t>Effect:</t>
+  </si>
+  <si>
+    <t>Target:</t>
+  </si>
+  <si>
+    <t>Additional Effect Name</t>
+  </si>
+  <si>
+    <t>Additional Effect Description</t>
+  </si>
+  <si>
+    <t>Acid, Arcane, Implement</t>
+  </si>
+  <si>
+    <t>Martial, Weapon</t>
+  </si>
+  <si>
+    <t>1[W] + Dexterity modifier (~DEXMod~). If the target is aberrant and has resistance or vulnerability to your attack, you gain a bonus to damage equal to your Wisdom modifier (~WISMod~).
+Level 21: 2[W] + Dexterity modifier (~DEXMod~).</t>
+  </si>
+  <si>
+    <t>1d10 + Charisma modifier (~CHAMod~) acid damage.
+Level 21: 2d10 + Charisma modifier (~CHAMod~) acid damage.</t>
+  </si>
+  <si>
+    <t>1[W] + Dexterity modifier (~DEXMod~) damage. If the target is aberrant and has resistance or vulnerability to your attack, you gain a bonus to damage equal to your Wisdom modifier (~WISMod~).
+Level 21: 2[W] + Dexterity modifier (~DEXMod~) damage.</t>
+  </si>
+  <si>
+    <t>DEX</t>
+  </si>
+  <si>
+    <t>CHA</t>
+  </si>
+  <si>
+    <t>Hits</t>
+  </si>
+  <si>
+    <t>Hit Levels</t>
+  </si>
+  <si>
+    <t>1[W] + (~DEXMod~)|2[W] + (~DEXMod~)</t>
+  </si>
+  <si>
+    <t>1|21</t>
+  </si>
+  <si>
+    <t>1d10 + (~CHAMod~)|2d10 + (~CHAMod~)</t>
+  </si>
+  <si>
+    <t>V</t>
   </si>
 </sst>
 </file>
@@ -8586,7 +8624,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8602,7 +8640,7 @@
         <v>677</v>
       </c>
       <c r="C1" t="s">
-        <v>2126</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -8766,7 +8804,7 @@
         <v>10</v>
       </c>
       <c r="C13" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">SUBSTITUTE(ADDRESS(1,COUNTA(INDIRECT(A13&amp;"!A1:ZZ1")),4),1,"")</f>
         <v>A</v>
       </c>
       <c r="D13" s="3"/>
@@ -8807,9 +8845,8 @@
         <f t="shared" ca="1" si="3"/>
         <v>4</v>
       </c>
-      <c r="C16" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Y</v>
+      <c r="C16" s="3" t="s">
+        <v>2140</v>
       </c>
       <c r="D16" s="3"/>
     </row>
@@ -8829,7 +8866,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>2124</v>
+        <v>2098</v>
       </c>
       <c r="B18">
         <f ca="1">COUNTA(INDIRECT(A18&amp;"!A:A"))-1</f>
@@ -15322,18 +15359,6 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5409F685-987D-421D-A06C-6C14318AD189}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1"/>
@@ -15354,7 +15379,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:F106"/>
@@ -16550,31 +16575,39 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <sheetPr codeName="Sheet9"/>
-  <dimension ref="A1:Y5"/>
+  <dimension ref="A1:AU50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="X2" sqref="X2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="9.140625" style="3"/>
-    <col min="21" max="23" width="9.140625" style="3"/>
+    <col min="5" max="5" width="15.5703125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="9.140625" style="3"/>
+    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" style="3" customWidth="1"/>
+    <col min="15" max="15" width="16" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.85546875" customWidth="1"/>
+    <col min="17" max="20" width="9.140625" style="3"/>
+    <col min="21" max="22" width="10.28515625" style="3" customWidth="1"/>
+    <col min="23" max="23" width="15.5703125" customWidth="1"/>
+    <col min="24" max="24" width="16" style="3" customWidth="1"/>
+    <col min="26" max="26" width="9.140625" style="3"/>
+    <col min="27" max="27" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.85546875" style="3" customWidth="1"/>
+    <col min="29" max="29" width="9.28515625" style="3" customWidth="1"/>
+    <col min="31" max="33" width="9.140625" style="3"/>
+    <col min="36" max="41" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>690</v>
       </c>
@@ -16582,76 +16615,136 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>687</v>
+        <v>2106</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>2094</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="3" t="s">
+        <v>2107</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>2072</v>
       </c>
+      <c r="F1" t="s">
+        <v>2091</v>
+      </c>
       <c r="G1" t="s">
-        <v>2106</v>
+        <v>2073</v>
       </c>
       <c r="H1" t="s">
-        <v>2073</v>
+        <v>2079</v>
       </c>
       <c r="I1" t="s">
-        <v>2075</v>
-      </c>
-      <c r="J1" t="s">
-        <v>2078</v>
-      </c>
-      <c r="K1" t="s">
-        <v>2079</v>
+        <v>2080</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>2135</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>2136</v>
       </c>
       <c r="L1" t="s">
-        <v>2080</v>
-      </c>
-      <c r="M1" t="s">
-        <v>2081</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>2108</v>
-      </c>
-      <c r="O1" s="3" t="s">
+        <v>2110</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>2109</v>
+      </c>
+      <c r="N1" t="s">
         <v>2111</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="O1" t="s">
+        <v>2076</v>
+      </c>
+      <c r="P1" t="s">
+        <v>2077</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>2116</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>2095</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>2126</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>2127</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>1479</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>1480</v>
+      </c>
+      <c r="W1" t="s">
         <v>2112</v>
       </c>
-      <c r="Q1" t="s">
-        <v>2083</v>
-      </c>
-      <c r="R1" t="s">
-        <v>2085</v>
-      </c>
-      <c r="S1" t="s">
-        <v>2087</v>
-      </c>
-      <c r="T1" t="s">
-        <v>2089</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>2091</v>
-      </c>
-      <c r="V1" s="3" t="s">
+      <c r="X1" s="3" t="s">
+        <v>2114</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>2113</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>2115</v>
+      </c>
+      <c r="AA1" t="s">
         <v>2117</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>2118</v>
       </c>
-      <c r="X1" t="s">
-        <v>2115</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>2116</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="AC1" s="3" t="s">
+        <v>2119</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>2120</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>2121</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>2123</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>2122</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>2124</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>2105</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
+        <v>2125</v>
+      </c>
+      <c r="AK1" s="3" t="s">
+        <v>2114</v>
+      </c>
+      <c r="AL1" s="3" t="s">
+        <v>2119</v>
+      </c>
+      <c r="AM1" s="3" t="s">
+        <v>2120</v>
+      </c>
+      <c r="AN1" s="3" t="s">
+        <v>2105</v>
+      </c>
+      <c r="AO1" s="3" t="s">
+        <v>2125</v>
+      </c>
+      <c r="AP1" s="3" t="s">
+        <v>2114</v>
+      </c>
+      <c r="AQ1" s="3" t="s">
+        <v>2119</v>
+      </c>
+      <c r="AR1" s="3" t="s">
+        <v>2120</v>
+      </c>
+      <c r="AS1" s="3"/>
+      <c r="AT1" s="3"/>
+      <c r="AU1" s="3"/>
+    </row>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2070</v>
       </c>
@@ -16664,61 +16757,79 @@
       <c r="D2" s="3">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="3" t="s">
+        <v>754</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1084</v>
+      </c>
+      <c r="G2" t="s">
+        <v>2074</v>
+      </c>
+      <c r="H2" t="s">
+        <v>2133</v>
+      </c>
+      <c r="I2" t="s">
+        <v>2081</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>2137</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>2138</v>
+      </c>
+      <c r="L2" t="s">
+        <v>2101</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>2108</v>
+      </c>
+      <c r="N2" t="s">
+        <v>2102</v>
+      </c>
+      <c r="O2" t="s">
+        <v>390</v>
+      </c>
+      <c r="P2" t="s">
+        <v>1083</v>
+      </c>
+      <c r="U2" s="3" t="str">
+        <f>IF(W2&lt;&gt;"",$W$1,"")&amp;IF(X2&lt;&gt;"","|"&amp;$X$1,"")&amp;IF(Y2&lt;&gt;"","|"&amp;$Y$1,"")&amp;IF(Z2&lt;&gt;"","|"&amp;$Z$1,"")&amp;IF(AA2&lt;&gt;"","|"&amp;$AA$1,"")&amp;IF(AB2&lt;&gt;"","|"&amp;$AB$1,"")&amp;IF(AC2&lt;&gt;"","|"&amp;$AC$1,"")&amp;IF(AD2&lt;&gt;"","|"&amp;$AD$1,"")&amp;IF(AE2&lt;&gt;"","|"&amp;$AE$1,"")&amp;IF(AF2&lt;&gt;"","|"&amp;$AF$1,"")&amp;IF(AG2&lt;&gt;"","|"&amp;$AG$1,"")&amp;IF(AH2&lt;&gt;"","|"&amp;$AH$1,"")&amp;IF(AI2&lt;&gt;"","|"&amp;$AI$1,"")&amp;IF(AJ2&lt;&gt;"","|"&amp;$AJ$1,"")&amp;IF(AK2&lt;&gt;"","|"&amp;$AK$1,"")&amp;IF(AL2&lt;&gt;"","|"&amp;$AL$1,"")&amp;IF(AM2&lt;&gt;"","|"&amp;$AM$1,"")&amp;IF(AN2&lt;&gt;"","|"&amp;$AN$1,"")&amp;IF(AO2&lt;&gt;"","|"&amp;$AO$1,"")&amp;IF(AP2&lt;&gt;"","|"&amp;$AP$1,"")&amp;IF(AQ2&lt;&gt;"","|"&amp;$AQ$1,"")&amp;IF(AR2&lt;&gt;"","|"&amp;$AR$1,"")&amp;IF(AS2&lt;&gt;"","|"&amp;$AS$1,"")&amp;IF(AT2&lt;&gt;"","|"&amp;$AT$1,"")&amp;IF(AU2&lt;&gt;"","|"&amp;$AU$1,"")&amp;IF(AV2&lt;&gt;"","|"&amp;$AV$1,"")&amp;IF(AW2&lt;&gt;"","|"&amp;$AW$1,"")&amp;IF(AX2&lt;&gt;"","|"&amp;$AX$1,"")&amp;IF(AY2&lt;&gt;"","|"&amp;$AY$1,"")&amp;IF(AZ2&lt;&gt;"","|"&amp;$AZ$1,"")&amp;IF(BA2&lt;&gt;"","|"&amp;$BA$1,"")&amp;IF(BB2&lt;&gt;"","|"&amp;$BB$1,"")&amp;IF(BC2&lt;&gt;"","|"&amp;$BC$1,"")&amp;IF(BD2&lt;&gt;"","|"&amp;$BD$1,"")&amp;IF(BE2&lt;&gt;"","|"&amp;$BE$1,"")&amp;IF(BF2&lt;&gt;"","|"&amp;$BF$1,"")&amp;IF(BG2&lt;&gt;"","|"&amp;$BG$1,"")&amp;IF(BH2&lt;&gt;"","|"&amp;$BH$1,"")</f>
+        <v>Flavor:|Prerequisite:|Keywords:|Attack:|Hit:</v>
+      </c>
+      <c r="V2" s="3" t="str">
+        <f>IF(W2&lt;&gt;"",W2,"")&amp;IF(X2&lt;&gt;"","|"&amp;X2,"")&amp;IF(Y2&lt;&gt;"","|"&amp;Y2,"")&amp;IF(Z2&lt;&gt;"","|"&amp;Z2,"")&amp;IF(AA2&lt;&gt;"","|"&amp;AA2,"")&amp;IF(AB2&lt;&gt;"","|"&amp;AB2,"")&amp;IF(AC2&lt;&gt;"","|"&amp;AC2,"")&amp;IF(AD2&lt;&gt;"","|"&amp;AD2,"")&amp;IF(AE2&lt;&gt;"","|"&amp;AE2,"")&amp;IF(AF2&lt;&gt;"","|"&amp;AF2,"")&amp;IF(AG2&lt;&gt;"","|"&amp;AG2,"")&amp;IF(AH2&lt;&gt;"","|"&amp;AH2,"")&amp;IF(AI2&lt;&gt;"","|"&amp;AI2,"")&amp;IF(AJ2&lt;&gt;"","|"&amp;AJ2,"")&amp;IF(AK2&lt;&gt;"","|"&amp;AK2,"")&amp;IF(AL2&lt;&gt;"","|"&amp;AL2,"")&amp;IF(AM2&lt;&gt;"","|"&amp;AM2,"")&amp;IF(AN2&lt;&gt;"","|"&amp;AN2,"")&amp;IF(AO2&lt;&gt;"","|"&amp;AO2,"")&amp;IF(AP2&lt;&gt;"","|"&amp;AP2,"")&amp;IF(AQ2&lt;&gt;"","|"&amp;AQ2,"")&amp;IF(AR2&lt;&gt;"","|"&amp;AR2,"")&amp;IF(AS2&lt;&gt;"","|"&amp;AS2,"")&amp;IF(AT2&lt;&gt;"","|"&amp;AT2,"")&amp;IF(AU2&lt;&gt;"","|"&amp;AU2,"")&amp;IF(AV2&lt;&gt;"","|"&amp;AV2,"")&amp;IF(AW2&lt;&gt;"","|"&amp;AW2,"")&amp;IF(AX2&lt;&gt;"","|"&amp;AX2,"")&amp;IF(AY2&lt;&gt;"","|"&amp;AY2,"")&amp;IF(AZ2&lt;&gt;"","|"&amp;AZ2,"")&amp;IF(BA2&lt;&gt;"","|"&amp;BA2,"")&amp;IF(BB2&lt;&gt;"","|"&amp;BB2,"")&amp;IF(BC2&lt;&gt;"","|"&amp;BC2,"")&amp;IF(BD2&lt;&gt;"","|"&amp;BD2,"")&amp;IF(BE2&lt;&gt;"","|"&amp;BE2,"")&amp;IF(BF2&lt;&gt;"","|"&amp;BF2,"")&amp;IF(BG2&lt;&gt;"","|"&amp;BG2,"")&amp;IF(BH2&lt;&gt;"","|"&amp;BH2,"")</f>
+        <v>You strike at your horrid enemy, using your knowledge of its strengths and weaknesses to twist the knife just a bit more.|You must be trained in Dungeoneering|Martial, Weapon|Dexterity vs AC|1[W] + Dexterity modifier (~DEXMod~). If the target is aberrant and has resistance or vulnerability to your attack, you gain a bonus to damage equal to your Wisdom modifier (~WISMod~).
+Level 21: 2[W] + Dexterity modifier (~DEXMod~).</v>
+      </c>
+      <c r="W2" t="s">
         <v>2071</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>754</v>
-      </c>
-      <c r="G2" t="s">
-        <v>1084</v>
-      </c>
-      <c r="H2" t="s">
-        <v>2074</v>
-      </c>
-      <c r="I2" t="s">
-        <v>2076</v>
-      </c>
-      <c r="J2" t="s">
-        <v>2127</v>
-      </c>
-      <c r="K2" t="s">
-        <v>390</v>
-      </c>
-      <c r="L2" t="s">
-        <v>1083</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="Y2" t="s">
+        <v>2078</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>2129</v>
+      </c>
+      <c r="AC2" s="3" t="s">
+        <v>2103</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>2130</v>
+      </c>
+      <c r="AE2" s="1"/>
+      <c r="AF2" s="1"/>
+      <c r="AG2" s="1"/>
+      <c r="AP2" s="3"/>
+      <c r="AQ2" s="3"/>
+      <c r="AR2" s="3"/>
+      <c r="AS2" s="3"/>
+      <c r="AT2" s="3"/>
+      <c r="AU2" s="3"/>
+    </row>
+    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>2082</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>2084</v>
-      </c>
-      <c r="R2" t="s">
-        <v>2086</v>
-      </c>
-      <c r="S2" t="s">
-        <v>2088</v>
-      </c>
-      <c r="T2" t="s">
-        <v>2090</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>2119</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>2120</v>
-      </c>
-      <c r="W2" s="3">
-        <v>21</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>2114</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2093</v>
       </c>
       <c r="B3" t="s">
         <v>746</v>
@@ -16729,49 +16840,67 @@
       <c r="D3" s="3">
         <v>1</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>754</v>
       </c>
+      <c r="F3" t="s">
+        <v>1084</v>
+      </c>
       <c r="G3" t="s">
-        <v>1084</v>
+        <v>2074</v>
       </c>
       <c r="H3" t="s">
-        <v>2095</v>
+        <v>2134</v>
       </c>
       <c r="I3" t="s">
-        <v>2076</v>
-      </c>
-      <c r="J3" t="s">
+        <v>752</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>2139</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>2138</v>
+      </c>
+      <c r="L3" t="s">
         <v>758</v>
       </c>
-      <c r="Q3" t="s">
-        <v>2084</v>
-      </c>
-      <c r="R3" t="s">
-        <v>2086</v>
-      </c>
-      <c r="S3" t="s">
-        <v>2096</v>
-      </c>
-      <c r="T3" t="s">
-        <v>752</v>
-      </c>
-      <c r="U3" s="3" t="s">
-        <v>2121</v>
-      </c>
-      <c r="V3" s="3" t="s">
-        <v>2122</v>
-      </c>
-      <c r="W3" s="3">
-        <v>21</v>
-      </c>
-      <c r="X3" s="1" t="s">
-        <v>2097</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="M3" s="3">
+        <v>20</v>
+      </c>
+      <c r="N3" t="s">
+        <v>2102</v>
+      </c>
+      <c r="U3" s="3" t="str">
+        <f>IF(W3&lt;&gt;"",$W$1,"")&amp;IF(X3&lt;&gt;"","|"&amp;$X$1,"")&amp;IF(Y3&lt;&gt;"","|"&amp;$Y$1,"")&amp;IF(Z3&lt;&gt;"","|"&amp;$Z$1,"")&amp;IF(AA3&lt;&gt;"","|"&amp;$AA$1,"")&amp;IF(AB3&lt;&gt;"","|"&amp;$AB$1,"")&amp;IF(AC3&lt;&gt;"","|"&amp;$AC$1,"")&amp;IF(AD3&lt;&gt;"","|"&amp;$AD$1,"")&amp;IF(AE3&lt;&gt;"","|"&amp;$AE$1,"")&amp;IF(AF3&lt;&gt;"","|"&amp;$AF$1,"")&amp;IF(AG3&lt;&gt;"","|"&amp;$AG$1,"")&amp;IF(AH3&lt;&gt;"","|"&amp;$AH$1,"")&amp;IF(AI3&lt;&gt;"","|"&amp;$AI$1,"")&amp;IF(AJ3&lt;&gt;"","|"&amp;$AJ$1,"")&amp;IF(AK3&lt;&gt;"","|"&amp;$AK$1,"")&amp;IF(AL3&lt;&gt;"","|"&amp;$AL$1,"")&amp;IF(AM3&lt;&gt;"","|"&amp;$AM$1,"")&amp;IF(AN3&lt;&gt;"","|"&amp;$AN$1,"")&amp;IF(AO3&lt;&gt;"","|"&amp;$AO$1,"")&amp;IF(AP3&lt;&gt;"","|"&amp;$AP$1,"")&amp;IF(AQ3&lt;&gt;"","|"&amp;$AQ$1,"")&amp;IF(AR3&lt;&gt;"","|"&amp;$AR$1,"")&amp;IF(AS3&lt;&gt;"","|"&amp;$AS$1,"")&amp;IF(AT3&lt;&gt;"","|"&amp;$AT$1,"")&amp;IF(AU3&lt;&gt;"","|"&amp;$AU$1,"")&amp;IF(AV3&lt;&gt;"","|"&amp;$AV$1,"")&amp;IF(AW3&lt;&gt;"","|"&amp;$AW$1,"")&amp;IF(AX3&lt;&gt;"","|"&amp;$AX$1,"")&amp;IF(AY3&lt;&gt;"","|"&amp;$AY$1,"")&amp;IF(AZ3&lt;&gt;"","|"&amp;$AZ$1,"")&amp;IF(BA3&lt;&gt;"","|"&amp;$BA$1,"")&amp;IF(BB3&lt;&gt;"","|"&amp;$BB$1,"")&amp;IF(BC3&lt;&gt;"","|"&amp;$BC$1,"")&amp;IF(BD3&lt;&gt;"","|"&amp;$BD$1,"")&amp;IF(BE3&lt;&gt;"","|"&amp;$BE$1,"")&amp;IF(BF3&lt;&gt;"","|"&amp;$BF$1,"")&amp;IF(BG3&lt;&gt;"","|"&amp;$BG$1,"")&amp;IF(BH3&lt;&gt;"","|"&amp;$BH$1,"")</f>
+        <v>|Keywords:|Attack:|Hit:</v>
+      </c>
+      <c r="V3" s="3" t="str">
+        <f>IF(W3&lt;&gt;"",W3,"")&amp;IF(X3&lt;&gt;"","|"&amp;X3,"")&amp;IF(Y3&lt;&gt;"","|"&amp;Y3,"")&amp;IF(Z3&lt;&gt;"","|"&amp;Z3,"")&amp;IF(AA3&lt;&gt;"","|"&amp;AA3,"")&amp;IF(AB3&lt;&gt;"","|"&amp;AB3,"")&amp;IF(AC3&lt;&gt;"","|"&amp;AC3,"")&amp;IF(AD3&lt;&gt;"","|"&amp;AD3,"")&amp;IF(AE3&lt;&gt;"","|"&amp;AE3,"")&amp;IF(AF3&lt;&gt;"","|"&amp;AF3,"")&amp;IF(AG3&lt;&gt;"","|"&amp;AG3,"")&amp;IF(AH3&lt;&gt;"","|"&amp;AH3,"")&amp;IF(AI3&lt;&gt;"","|"&amp;AI3,"")&amp;IF(AJ3&lt;&gt;"","|"&amp;AJ3,"")&amp;IF(AK3&lt;&gt;"","|"&amp;AK3,"")&amp;IF(AL3&lt;&gt;"","|"&amp;AL3,"")&amp;IF(AM3&lt;&gt;"","|"&amp;AM3,"")&amp;IF(AN3&lt;&gt;"","|"&amp;AN3,"")&amp;IF(AO3&lt;&gt;"","|"&amp;AO3,"")&amp;IF(AP3&lt;&gt;"","|"&amp;AP3,"")&amp;IF(AQ3&lt;&gt;"","|"&amp;AQ3,"")&amp;IF(AR3&lt;&gt;"","|"&amp;AR3,"")&amp;IF(AS3&lt;&gt;"","|"&amp;AS3,"")&amp;IF(AT3&lt;&gt;"","|"&amp;AT3,"")&amp;IF(AU3&lt;&gt;"","|"&amp;AU3,"")&amp;IF(AV3&lt;&gt;"","|"&amp;AV3,"")&amp;IF(AW3&lt;&gt;"","|"&amp;AW3,"")&amp;IF(AX3&lt;&gt;"","|"&amp;AX3,"")&amp;IF(AY3&lt;&gt;"","|"&amp;AY3,"")&amp;IF(AZ3&lt;&gt;"","|"&amp;AZ3,"")&amp;IF(BA3&lt;&gt;"","|"&amp;BA3,"")&amp;IF(BB3&lt;&gt;"","|"&amp;BB3,"")&amp;IF(BC3&lt;&gt;"","|"&amp;BC3,"")&amp;IF(BD3&lt;&gt;"","|"&amp;BD3,"")&amp;IF(BE3&lt;&gt;"","|"&amp;BE3,"")&amp;IF(BF3&lt;&gt;"","|"&amp;BF3,"")&amp;IF(BG3&lt;&gt;"","|"&amp;BG3,"")&amp;IF(BH3&lt;&gt;"","|"&amp;BH3,"")</f>
+        <v>|Acid, Arcane, Implement|Charisma vs Reflexes|1d10 + Charisma modifier (~CHAMod~) acid damage.
+Level 21: 2d10 + Charisma modifier (~CHAMod~) acid damage.</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>2128</v>
+      </c>
+      <c r="AC3" s="3" t="s">
+        <v>2104</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>2131</v>
+      </c>
+      <c r="AE3" s="1"/>
+      <c r="AF3" s="1"/>
+      <c r="AG3" s="1"/>
+      <c r="AP3" s="3"/>
+      <c r="AQ3" s="3"/>
+      <c r="AR3" s="3"/>
+      <c r="AS3" s="3"/>
+      <c r="AT3" s="3"/>
+      <c r="AU3" s="3"/>
+    </row>
+    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2098</v>
+        <v>2083</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>1774</v>
@@ -16779,40 +16908,59 @@
       <c r="C4" t="s">
         <v>731</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>2105</v>
+      <c r="D4" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>2090</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1084</v>
       </c>
       <c r="G4" t="s">
-        <v>1084</v>
-      </c>
-      <c r="H4" t="s">
+        <v>2085</v>
+      </c>
+      <c r="L4" t="s">
+        <v>2086</v>
+      </c>
+      <c r="O4" t="s">
+        <v>2083</v>
+      </c>
+      <c r="P4" t="s">
+        <v>265</v>
+      </c>
+      <c r="U4" s="3" t="str">
+        <f>IF(W4&lt;&gt;"",$W$1,"")&amp;IF(X4&lt;&gt;"","|"&amp;$X$1,"")&amp;IF(Y4&lt;&gt;"","|"&amp;$Y$1,"")&amp;IF(Z4&lt;&gt;"","|"&amp;$Z$1,"")&amp;IF(AA4&lt;&gt;"","|"&amp;$AA$1,"")&amp;IF(AB4&lt;&gt;"","|"&amp;$AB$1,"")&amp;IF(AC4&lt;&gt;"","|"&amp;$AC$1,"")&amp;IF(AD4&lt;&gt;"","|"&amp;$AD$1,"")&amp;IF(AE4&lt;&gt;"","|"&amp;$AE$1,"")&amp;IF(AF4&lt;&gt;"","|"&amp;$AF$1,"")&amp;IF(AG4&lt;&gt;"","|"&amp;$AG$1,"")&amp;IF(AH4&lt;&gt;"","|"&amp;$AH$1,"")&amp;IF(AI4&lt;&gt;"","|"&amp;$AI$1,"")&amp;IF(AJ4&lt;&gt;"","|"&amp;$AJ$1,"")&amp;IF(AK4&lt;&gt;"","|"&amp;$AK$1,"")&amp;IF(AL4&lt;&gt;"","|"&amp;$AL$1,"")&amp;IF(AM4&lt;&gt;"","|"&amp;$AM$1,"")&amp;IF(AN4&lt;&gt;"","|"&amp;$AN$1,"")&amp;IF(AO4&lt;&gt;"","|"&amp;$AO$1,"")&amp;IF(AP4&lt;&gt;"","|"&amp;$AP$1,"")&amp;IF(AQ4&lt;&gt;"","|"&amp;$AQ$1,"")&amp;IF(AR4&lt;&gt;"","|"&amp;$AR$1,"")&amp;IF(AS4&lt;&gt;"","|"&amp;$AS$1,"")&amp;IF(AT4&lt;&gt;"","|"&amp;$AT$1,"")&amp;IF(AU4&lt;&gt;"","|"&amp;$AU$1,"")&amp;IF(AV4&lt;&gt;"","|"&amp;$AV$1,"")&amp;IF(AW4&lt;&gt;"","|"&amp;$AW$1,"")&amp;IF(AX4&lt;&gt;"","|"&amp;$AX$1,"")&amp;IF(AY4&lt;&gt;"","|"&amp;$AY$1,"")&amp;IF(AZ4&lt;&gt;"","|"&amp;$AZ$1,"")&amp;IF(BA4&lt;&gt;"","|"&amp;$BA$1,"")&amp;IF(BB4&lt;&gt;"","|"&amp;$BB$1,"")&amp;IF(BC4&lt;&gt;"","|"&amp;$BC$1,"")&amp;IF(BD4&lt;&gt;"","|"&amp;$BD$1,"")&amp;IF(BE4&lt;&gt;"","|"&amp;$BE$1,"")&amp;IF(BF4&lt;&gt;"","|"&amp;$BF$1,"")&amp;IF(BG4&lt;&gt;"","|"&amp;$BG$1,"")&amp;IF(BH4&lt;&gt;"","|"&amp;$BH$1,"")</f>
+        <v>|Prerequisite:|Keywords:|Effect:</v>
+      </c>
+      <c r="V4" s="3" t="str">
+        <f>IF(W4&lt;&gt;"",W4,"")&amp;IF(X4&lt;&gt;"","|"&amp;X4,"")&amp;IF(Y4&lt;&gt;"","|"&amp;Y4,"")&amp;IF(Z4&lt;&gt;"","|"&amp;Z4,"")&amp;IF(AA4&lt;&gt;"","|"&amp;AA4,"")&amp;IF(AB4&lt;&gt;"","|"&amp;AB4,"")&amp;IF(AC4&lt;&gt;"","|"&amp;AC4,"")&amp;IF(AD4&lt;&gt;"","|"&amp;AD4,"")&amp;IF(AE4&lt;&gt;"","|"&amp;AE4,"")&amp;IF(AF4&lt;&gt;"","|"&amp;AF4,"")&amp;IF(AG4&lt;&gt;"","|"&amp;AG4,"")&amp;IF(AH4&lt;&gt;"","|"&amp;AH4,"")&amp;IF(AI4&lt;&gt;"","|"&amp;AI4,"")&amp;IF(AJ4&lt;&gt;"","|"&amp;AJ4,"")&amp;IF(AK4&lt;&gt;"","|"&amp;AK4,"")&amp;IF(AL4&lt;&gt;"","|"&amp;AL4,"")&amp;IF(AM4&lt;&gt;"","|"&amp;AM4,"")&amp;IF(AN4&lt;&gt;"","|"&amp;AN4,"")&amp;IF(AO4&lt;&gt;"","|"&amp;AO4,"")&amp;IF(AP4&lt;&gt;"","|"&amp;AP4,"")&amp;IF(AQ4&lt;&gt;"","|"&amp;AQ4,"")&amp;IF(AR4&lt;&gt;"","|"&amp;AR4,"")&amp;IF(AS4&lt;&gt;"","|"&amp;AS4,"")&amp;IF(AT4&lt;&gt;"","|"&amp;AT4,"")&amp;IF(AU4&lt;&gt;"","|"&amp;AU4,"")&amp;IF(AV4&lt;&gt;"","|"&amp;AV4,"")&amp;IF(AW4&lt;&gt;"","|"&amp;AW4,"")&amp;IF(AX4&lt;&gt;"","|"&amp;AX4,"")&amp;IF(AY4&lt;&gt;"","|"&amp;AY4,"")&amp;IF(AZ4&lt;&gt;"","|"&amp;AZ4,"")&amp;IF(BA4&lt;&gt;"","|"&amp;BA4,"")&amp;IF(BB4&lt;&gt;"","|"&amp;BB4,"")&amp;IF(BC4&lt;&gt;"","|"&amp;BC4,"")&amp;IF(BD4&lt;&gt;"","|"&amp;BD4,"")&amp;IF(BE4&lt;&gt;"","|"&amp;BE4,"")&amp;IF(BF4&lt;&gt;"","|"&amp;BF4,"")&amp;IF(BG4&lt;&gt;"","|"&amp;BG4,"")&amp;IF(BH4&lt;&gt;"","|"&amp;BH4,"")</f>
+        <v>|You must have the selected Acrobat's trick as part of the Rogue's Trick class feature.|Martial|You move up to your speed -2. During this move, you have a climb speed equal to your speed -2. You also gain a +2 power bonus to your next damage roll with a basic attack during this turn.
+Level 11: +4 power bonus.
+Level 21: +6 power bonus.</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>2084</v>
+      </c>
+      <c r="AA4" t="s">
         <v>711</v>
       </c>
-      <c r="I4" t="s">
-        <v>2100</v>
-      </c>
-      <c r="K4" t="s">
-        <v>2098</v>
-      </c>
-      <c r="L4" t="s">
-        <v>844</v>
-      </c>
-      <c r="M4" t="s">
-        <v>2099</v>
-      </c>
-      <c r="R4" t="s">
-        <v>2101</v>
-      </c>
-      <c r="Y4" s="1" t="s">
-        <v>2102</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="AH4" s="1" t="s">
+        <v>2087</v>
+      </c>
+      <c r="AP4" s="3"/>
+      <c r="AQ4" s="3"/>
+      <c r="AR4" s="3"/>
+      <c r="AS4" s="3"/>
+      <c r="AT4" s="3"/>
+      <c r="AU4" s="3"/>
+    </row>
+    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2103</v>
+        <v>2088</v>
       </c>
       <c r="B5" t="s">
-        <v>2104</v>
+        <v>2089</v>
       </c>
       <c r="C5" t="s">
         <v>731</v>
@@ -16820,69 +16968,623 @@
       <c r="D5" s="3">
         <v>1</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="3" t="s">
+        <v>754</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1084</v>
+      </c>
+      <c r="G5" t="s">
+        <v>2074</v>
+      </c>
+      <c r="H5" t="s">
+        <v>2133</v>
+      </c>
+      <c r="I5" t="s">
+        <v>2081</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>2137</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>2138</v>
+      </c>
+      <c r="L5" t="s">
+        <v>757</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>780</v>
+      </c>
+      <c r="N5" t="s">
+        <v>2102</v>
+      </c>
+      <c r="O5" t="s">
+        <v>2093</v>
+      </c>
+      <c r="P5" t="s">
+        <v>1083</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>2092</v>
+      </c>
+      <c r="R5" t="s">
+        <v>2075</v>
+      </c>
+      <c r="U5" s="3" t="str">
+        <f>IF(W5&lt;&gt;"",$W$1,"")&amp;IF(X5&lt;&gt;"","|"&amp;$X$1,"")&amp;IF(Y5&lt;&gt;"","|"&amp;$Y$1,"")&amp;IF(Z5&lt;&gt;"","|"&amp;$Z$1,"")&amp;IF(AA5&lt;&gt;"","|"&amp;$AA$1,"")&amp;IF(AB5&lt;&gt;"","|"&amp;$AB$1,"")&amp;IF(AC5&lt;&gt;"","|"&amp;$AC$1,"")&amp;IF(AD5&lt;&gt;"","|"&amp;$AD$1,"")&amp;IF(AE5&lt;&gt;"","|"&amp;$AE$1,"")&amp;IF(AF5&lt;&gt;"","|"&amp;$AF$1,"")&amp;IF(AG5&lt;&gt;"","|"&amp;$AG$1,"")&amp;IF(AH5&lt;&gt;"","|"&amp;$AH$1,"")&amp;IF(AI5&lt;&gt;"","|"&amp;$AI$1,"")&amp;IF(AJ5&lt;&gt;"","|"&amp;$AJ$1,"")&amp;IF(AK5&lt;&gt;"","|"&amp;$AK$1,"")&amp;IF(AL5&lt;&gt;"","|"&amp;$AL$1,"")&amp;IF(AM5&lt;&gt;"","|"&amp;$AM$1,"")&amp;IF(AN5&lt;&gt;"","|"&amp;$AN$1,"")&amp;IF(AO5&lt;&gt;"","|"&amp;$AO$1,"")&amp;IF(AP5&lt;&gt;"","|"&amp;$AP$1,"")&amp;IF(AQ5&lt;&gt;"","|"&amp;$AQ$1,"")&amp;IF(AR5&lt;&gt;"","|"&amp;$AR$1,"")&amp;IF(AS5&lt;&gt;"","|"&amp;$AS$1,"")&amp;IF(AT5&lt;&gt;"","|"&amp;$AT$1,"")&amp;IF(AU5&lt;&gt;"","|"&amp;$AU$1,"")&amp;IF(AV5&lt;&gt;"","|"&amp;$AV$1,"")&amp;IF(AW5&lt;&gt;"","|"&amp;$AW$1,"")&amp;IF(AX5&lt;&gt;"","|"&amp;$AX$1,"")&amp;IF(AY5&lt;&gt;"","|"&amp;$AY$1,"")&amp;IF(AZ5&lt;&gt;"","|"&amp;$AZ$1,"")&amp;IF(BA5&lt;&gt;"","|"&amp;$BA$1,"")&amp;IF(BB5&lt;&gt;"","|"&amp;$BB$1,"")&amp;IF(BC5&lt;&gt;"","|"&amp;$BC$1,"")&amp;IF(BD5&lt;&gt;"","|"&amp;$BD$1,"")&amp;IF(BE5&lt;&gt;"","|"&amp;$BE$1,"")&amp;IF(BF5&lt;&gt;"","|"&amp;$BF$1,"")&amp;IF(BG5&lt;&gt;"","|"&amp;$BG$1,"")&amp;IF(BH5&lt;&gt;"","|"&amp;$BH$1,"")</f>
+        <v>Flavor:|Prerequisite:|Requirement:|Keywords:|Attack:|Hit:|Effect:</v>
+      </c>
+      <c r="V5" s="3" t="str">
+        <f>IF(W5&lt;&gt;"",W5,"")&amp;IF(X5&lt;&gt;"","|"&amp;X5,"")&amp;IF(Y5&lt;&gt;"","|"&amp;Y5,"")&amp;IF(Z5&lt;&gt;"","|"&amp;Z5,"")&amp;IF(AA5&lt;&gt;"","|"&amp;AA5,"")&amp;IF(AB5&lt;&gt;"","|"&amp;AB5,"")&amp;IF(AC5&lt;&gt;"","|"&amp;AC5,"")&amp;IF(AD5&lt;&gt;"","|"&amp;AD5,"")&amp;IF(AE5&lt;&gt;"","|"&amp;AE5,"")&amp;IF(AF5&lt;&gt;"","|"&amp;AF5,"")&amp;IF(AG5&lt;&gt;"","|"&amp;AG5,"")&amp;IF(AH5&lt;&gt;"","|"&amp;AH5,"")&amp;IF(AI5&lt;&gt;"","|"&amp;AI5,"")&amp;IF(AJ5&lt;&gt;"","|"&amp;AJ5,"")&amp;IF(AK5&lt;&gt;"","|"&amp;AK5,"")&amp;IF(AL5&lt;&gt;"","|"&amp;AL5,"")&amp;IF(AM5&lt;&gt;"","|"&amp;AM5,"")&amp;IF(AN5&lt;&gt;"","|"&amp;AN5,"")&amp;IF(AO5&lt;&gt;"","|"&amp;AO5,"")&amp;IF(AP5&lt;&gt;"","|"&amp;AP5,"")&amp;IF(AQ5&lt;&gt;"","|"&amp;AQ5,"")&amp;IF(AR5&lt;&gt;"","|"&amp;AR5,"")&amp;IF(AS5&lt;&gt;"","|"&amp;AS5,"")&amp;IF(AT5&lt;&gt;"","|"&amp;AT5,"")&amp;IF(AU5&lt;&gt;"","|"&amp;AU5,"")&amp;IF(AV5&lt;&gt;"","|"&amp;AV5,"")&amp;IF(AW5&lt;&gt;"","|"&amp;AW5,"")&amp;IF(AX5&lt;&gt;"","|"&amp;AX5,"")&amp;IF(AY5&lt;&gt;"","|"&amp;AY5,"")&amp;IF(AZ5&lt;&gt;"","|"&amp;AZ5,"")&amp;IF(BA5&lt;&gt;"","|"&amp;BA5,"")&amp;IF(BB5&lt;&gt;"","|"&amp;BB5,"")&amp;IF(BC5&lt;&gt;"","|"&amp;BC5,"")&amp;IF(BD5&lt;&gt;"","|"&amp;BD5,"")&amp;IF(BE5&lt;&gt;"","|"&amp;BE5,"")&amp;IF(BF5&lt;&gt;"","|"&amp;BF5,"")&amp;IF(BG5&lt;&gt;"","|"&amp;BG5,"")&amp;IF(BH5&lt;&gt;"","|"&amp;BH5,"")</f>
+        <v>You strike at your horrid enemy, using your knowledge of its strengths and weaknesses to twist the knife just a bit more.|You must be trained in Acrobatics|You must be wielding a light blade in order to use.|Martial, Weapon|Dexterity vs AC|1[W] + Dexterity modifier (~DEXMod~) damage. If the target is aberrant and has resistance or vulnerability to your attack, you gain a bonus to damage equal to your Wisdom modifier (~WISMod~).
+Level 21: 2[W] + Dexterity modifier (~DEXMod~) damage.|Before or after the attack, you shift 1 square.</v>
+      </c>
+      <c r="W5" t="s">
         <v>2071</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>754</v>
-      </c>
-      <c r="G5" t="s">
-        <v>1084</v>
-      </c>
-      <c r="H5" t="s">
-        <v>2074</v>
-      </c>
-      <c r="I5" t="s">
-        <v>2076</v>
-      </c>
-      <c r="J5" t="s">
-        <v>757</v>
-      </c>
-      <c r="K5" t="s">
-        <v>2109</v>
-      </c>
-      <c r="L5" t="s">
-        <v>1083</v>
-      </c>
-      <c r="M5" t="s">
-        <v>2110</v>
-      </c>
-      <c r="N5" t="s">
-        <v>2107</v>
-      </c>
-      <c r="O5" t="s">
-        <v>2077</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>2113</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>2084</v>
-      </c>
-      <c r="R5" t="s">
-        <v>2086</v>
-      </c>
-      <c r="S5" t="s">
-        <v>2088</v>
-      </c>
-      <c r="T5" t="s">
-        <v>2090</v>
-      </c>
-      <c r="U5" s="3" t="s">
-        <v>2119</v>
-      </c>
-      <c r="V5" s="3" t="s">
-        <v>2120</v>
-      </c>
-      <c r="W5" s="3">
-        <v>21</v>
-      </c>
-      <c r="X5" s="1" t="s">
-        <v>2092</v>
-      </c>
-      <c r="Y5" s="1" t="s">
-        <v>2123</v>
-      </c>
+      <c r="Y5" t="s">
+        <v>2094</v>
+      </c>
+      <c r="Z5" s="3" t="s">
+        <v>2096</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>2129</v>
+      </c>
+      <c r="AC5" s="3" t="s">
+        <v>2103</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>2132</v>
+      </c>
+      <c r="AE5" s="1"/>
+      <c r="AF5" s="1"/>
+      <c r="AG5" s="1"/>
+      <c r="AH5" s="1" t="s">
+        <v>2097</v>
+      </c>
+      <c r="AP5" s="3"/>
+      <c r="AQ5" s="3"/>
+      <c r="AR5" s="3"/>
+      <c r="AS5" s="3"/>
+      <c r="AT5" s="3"/>
+      <c r="AU5" s="3"/>
+    </row>
+    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AP6" s="3"/>
+      <c r="AQ6" s="3"/>
+      <c r="AR6" s="3"/>
+      <c r="AS6" s="3"/>
+      <c r="AT6" s="3"/>
+      <c r="AU6" s="3"/>
+    </row>
+    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AP7" s="3"/>
+      <c r="AQ7" s="3"/>
+      <c r="AR7" s="3"/>
+      <c r="AS7" s="3"/>
+      <c r="AT7" s="3"/>
+      <c r="AU7" s="3"/>
+    </row>
+    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="O9" s="3"/>
+      <c r="X9"/>
+      <c r="Y9" s="3"/>
+      <c r="Z9"/>
+      <c r="AA9" s="3"/>
+      <c r="AC9"/>
+      <c r="AD9" s="3"/>
+      <c r="AG9"/>
+      <c r="AI9" s="3"/>
+      <c r="AO9"/>
+    </row>
+    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10"/>
+      <c r="R10"/>
+      <c r="W10" s="3"/>
+      <c r="Y10" s="3"/>
+      <c r="AD10" s="3"/>
+      <c r="AE10"/>
+      <c r="AI10" s="3"/>
+      <c r="AL10"/>
+      <c r="AM10"/>
+      <c r="AP10" s="3"/>
+      <c r="AQ10" s="3"/>
+      <c r="AR10" s="3"/>
+      <c r="AS10" s="3"/>
+    </row>
+    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="O11" s="3"/>
+      <c r="Q11"/>
+      <c r="R11"/>
+      <c r="W11" s="3"/>
+      <c r="Y11" s="3"/>
+      <c r="AD11" s="3"/>
+      <c r="AE11"/>
+      <c r="AI11" s="3"/>
+      <c r="AL11"/>
+      <c r="AM11"/>
+      <c r="AP11" s="3"/>
+      <c r="AQ11" s="3"/>
+      <c r="AR11" s="3"/>
+      <c r="AS11" s="3"/>
+    </row>
+    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="R12"/>
+      <c r="W12" s="3"/>
+      <c r="Y12" s="3"/>
+      <c r="AD12" s="3"/>
+      <c r="AE12"/>
+      <c r="AI12" s="3"/>
+      <c r="AL12"/>
+      <c r="AM12"/>
+      <c r="AP12" s="3"/>
+      <c r="AQ12" s="3"/>
+      <c r="AR12" s="3"/>
+      <c r="AS12" s="3"/>
+    </row>
+    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="R13"/>
+      <c r="W13" s="3"/>
+      <c r="Y13" s="3"/>
+      <c r="AD13" s="3"/>
+      <c r="AE13"/>
+      <c r="AI13" s="3"/>
+      <c r="AL13"/>
+      <c r="AM13"/>
+      <c r="AP13" s="3"/>
+      <c r="AQ13" s="3"/>
+      <c r="AR13" s="3"/>
+      <c r="AS13" s="3"/>
+    </row>
+    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="R14"/>
+      <c r="W14" s="3"/>
+      <c r="Y14" s="3"/>
+      <c r="AD14" s="3"/>
+      <c r="AE14"/>
+      <c r="AI14" s="3"/>
+      <c r="AL14"/>
+      <c r="AM14"/>
+      <c r="AP14" s="3"/>
+      <c r="AQ14" s="3"/>
+      <c r="AR14" s="3"/>
+      <c r="AS14" s="3"/>
+    </row>
+    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="R15"/>
+      <c r="W15" s="3"/>
+      <c r="Y15" s="3"/>
+      <c r="AD15" s="3"/>
+      <c r="AE15"/>
+      <c r="AI15" s="3"/>
+      <c r="AL15"/>
+      <c r="AM15"/>
+      <c r="AP15" s="3"/>
+      <c r="AQ15" s="3"/>
+      <c r="AR15" s="3"/>
+      <c r="AS15" s="3"/>
+    </row>
+    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="R16"/>
+      <c r="W16" s="3"/>
+      <c r="Y16" s="3"/>
+      <c r="AD16" s="3"/>
+      <c r="AE16"/>
+      <c r="AI16" s="3"/>
+      <c r="AL16"/>
+      <c r="AM16"/>
+      <c r="AP16" s="3"/>
+      <c r="AQ16" s="3"/>
+      <c r="AR16" s="3"/>
+      <c r="AS16" s="3"/>
+    </row>
+    <row r="17" spans="14:45" x14ac:dyDescent="0.25">
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="R17"/>
+      <c r="W17" s="3"/>
+      <c r="Y17" s="3"/>
+      <c r="AD17" s="3"/>
+      <c r="AE17"/>
+      <c r="AI17" s="3"/>
+      <c r="AL17"/>
+      <c r="AM17"/>
+      <c r="AP17" s="3"/>
+      <c r="AQ17" s="3"/>
+      <c r="AR17" s="3"/>
+      <c r="AS17" s="3"/>
+    </row>
+    <row r="18" spans="14:45" x14ac:dyDescent="0.25">
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="R18"/>
+      <c r="W18" s="3"/>
+      <c r="Y18" s="3"/>
+      <c r="AD18" s="3"/>
+      <c r="AE18"/>
+      <c r="AI18" s="3"/>
+      <c r="AL18"/>
+      <c r="AM18"/>
+      <c r="AP18" s="3"/>
+      <c r="AQ18" s="3"/>
+      <c r="AR18" s="3"/>
+      <c r="AS18" s="3"/>
+    </row>
+    <row r="19" spans="14:45" x14ac:dyDescent="0.25">
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="R19"/>
+      <c r="W19" s="3"/>
+      <c r="Y19" s="3"/>
+      <c r="AD19" s="3"/>
+      <c r="AE19"/>
+      <c r="AI19" s="3"/>
+      <c r="AL19"/>
+      <c r="AM19"/>
+      <c r="AP19" s="3"/>
+      <c r="AQ19" s="3"/>
+      <c r="AR19" s="3"/>
+      <c r="AS19" s="3"/>
+    </row>
+    <row r="20" spans="14:45" x14ac:dyDescent="0.25">
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="R20"/>
+      <c r="W20" s="3"/>
+      <c r="Y20" s="3"/>
+      <c r="AD20" s="3"/>
+      <c r="AE20"/>
+      <c r="AI20" s="3"/>
+      <c r="AL20"/>
+      <c r="AM20"/>
+      <c r="AP20" s="3"/>
+      <c r="AQ20" s="3"/>
+      <c r="AR20" s="3"/>
+      <c r="AS20" s="3"/>
+    </row>
+    <row r="21" spans="14:45" x14ac:dyDescent="0.25">
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="R21"/>
+      <c r="W21" s="3"/>
+      <c r="Y21" s="3"/>
+      <c r="AD21" s="3"/>
+      <c r="AE21"/>
+      <c r="AI21" s="3"/>
+      <c r="AL21"/>
+      <c r="AM21"/>
+      <c r="AP21" s="3"/>
+      <c r="AQ21" s="3"/>
+      <c r="AR21" s="3"/>
+      <c r="AS21" s="3"/>
+    </row>
+    <row r="22" spans="14:45" x14ac:dyDescent="0.25">
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="R22"/>
+      <c r="W22" s="3"/>
+      <c r="Y22" s="3"/>
+      <c r="AD22" s="3"/>
+      <c r="AE22"/>
+      <c r="AI22" s="3"/>
+      <c r="AL22"/>
+      <c r="AM22"/>
+      <c r="AP22" s="3"/>
+      <c r="AQ22" s="3"/>
+      <c r="AR22" s="3"/>
+      <c r="AS22" s="3"/>
+    </row>
+    <row r="23" spans="14:45" x14ac:dyDescent="0.25">
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="R23"/>
+      <c r="W23" s="3"/>
+      <c r="Y23" s="3"/>
+      <c r="AD23" s="3"/>
+      <c r="AE23"/>
+      <c r="AI23" s="3"/>
+      <c r="AL23"/>
+      <c r="AM23"/>
+      <c r="AP23" s="3"/>
+      <c r="AQ23" s="3"/>
+      <c r="AR23" s="3"/>
+      <c r="AS23" s="3"/>
+    </row>
+    <row r="24" spans="14:45" x14ac:dyDescent="0.25">
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="R24"/>
+      <c r="W24" s="3"/>
+      <c r="Y24" s="3"/>
+      <c r="AD24" s="3"/>
+      <c r="AE24"/>
+      <c r="AI24" s="3"/>
+      <c r="AL24"/>
+      <c r="AM24"/>
+      <c r="AP24" s="3"/>
+      <c r="AQ24" s="3"/>
+      <c r="AR24" s="3"/>
+      <c r="AS24" s="3"/>
+    </row>
+    <row r="25" spans="14:45" x14ac:dyDescent="0.25">
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="R25"/>
+      <c r="W25" s="3"/>
+      <c r="Y25" s="3"/>
+      <c r="AD25" s="3"/>
+      <c r="AE25"/>
+      <c r="AI25" s="3"/>
+      <c r="AL25"/>
+      <c r="AM25"/>
+      <c r="AP25" s="3"/>
+      <c r="AQ25" s="3"/>
+      <c r="AR25" s="3"/>
+      <c r="AS25" s="3"/>
+    </row>
+    <row r="26" spans="14:45" x14ac:dyDescent="0.25">
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="R26"/>
+      <c r="W26" s="3"/>
+      <c r="Y26" s="3"/>
+      <c r="AD26" s="3"/>
+      <c r="AE26"/>
+      <c r="AI26" s="3"/>
+      <c r="AL26"/>
+      <c r="AM26"/>
+      <c r="AP26" s="3"/>
+      <c r="AQ26" s="3"/>
+      <c r="AR26" s="3"/>
+      <c r="AS26" s="3"/>
+    </row>
+    <row r="27" spans="14:45" x14ac:dyDescent="0.25">
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="R27"/>
+      <c r="W27" s="3"/>
+      <c r="Y27" s="3"/>
+      <c r="AD27" s="3"/>
+      <c r="AE27"/>
+      <c r="AI27" s="3"/>
+      <c r="AL27"/>
+      <c r="AM27"/>
+      <c r="AP27" s="3"/>
+      <c r="AQ27" s="3"/>
+      <c r="AR27" s="3"/>
+      <c r="AS27" s="3"/>
+    </row>
+    <row r="28" spans="14:45" x14ac:dyDescent="0.25">
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="3"/>
+      <c r="R28"/>
+      <c r="W28" s="3"/>
+      <c r="Y28" s="3"/>
+      <c r="AD28" s="3"/>
+      <c r="AE28"/>
+      <c r="AI28" s="3"/>
+      <c r="AL28"/>
+      <c r="AM28"/>
+      <c r="AP28" s="3"/>
+      <c r="AQ28" s="3"/>
+      <c r="AR28" s="3"/>
+      <c r="AS28" s="3"/>
+    </row>
+    <row r="29" spans="14:45" x14ac:dyDescent="0.25">
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="3"/>
+      <c r="R29"/>
+      <c r="W29" s="3"/>
+      <c r="Y29" s="3"/>
+      <c r="AD29" s="3"/>
+      <c r="AE29"/>
+      <c r="AI29" s="3"/>
+      <c r="AL29"/>
+      <c r="AM29"/>
+      <c r="AP29" s="3"/>
+      <c r="AQ29" s="3"/>
+      <c r="AR29" s="3"/>
+      <c r="AS29" s="3"/>
+    </row>
+    <row r="30" spans="14:45" x14ac:dyDescent="0.25">
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
+      <c r="P30" s="3"/>
+      <c r="R30"/>
+      <c r="W30" s="3"/>
+      <c r="Y30" s="3"/>
+      <c r="AD30" s="3"/>
+      <c r="AE30"/>
+      <c r="AI30" s="3"/>
+      <c r="AL30"/>
+      <c r="AM30"/>
+      <c r="AP30" s="3"/>
+      <c r="AQ30" s="3"/>
+      <c r="AR30" s="3"/>
+      <c r="AS30" s="3"/>
+    </row>
+    <row r="31" spans="14:45" x14ac:dyDescent="0.25">
+      <c r="N31" s="3"/>
+      <c r="O31" s="3"/>
+      <c r="P31" s="3"/>
+      <c r="R31"/>
+      <c r="W31" s="3"/>
+      <c r="Y31" s="3"/>
+      <c r="AD31" s="3"/>
+      <c r="AE31"/>
+      <c r="AI31" s="3"/>
+      <c r="AL31"/>
+      <c r="AM31"/>
+      <c r="AP31" s="3"/>
+      <c r="AQ31" s="3"/>
+      <c r="AR31" s="3"/>
+      <c r="AS31" s="3"/>
+    </row>
+    <row r="32" spans="14:45" x14ac:dyDescent="0.25">
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
+      <c r="P32" s="3"/>
+      <c r="R32"/>
+      <c r="W32" s="3"/>
+      <c r="Y32" s="3"/>
+      <c r="AD32" s="3"/>
+      <c r="AE32"/>
+      <c r="AI32" s="3"/>
+      <c r="AL32"/>
+      <c r="AM32"/>
+      <c r="AP32" s="3"/>
+      <c r="AQ32" s="3"/>
+      <c r="AR32" s="3"/>
+      <c r="AS32" s="3"/>
+    </row>
+    <row r="33" spans="15:45" x14ac:dyDescent="0.25">
+      <c r="O33" s="3"/>
+      <c r="P33" s="3"/>
+      <c r="R33"/>
+      <c r="W33" s="3"/>
+      <c r="Y33" s="3"/>
+      <c r="AD33" s="3"/>
+      <c r="AE33"/>
+      <c r="AI33" s="3"/>
+      <c r="AL33"/>
+      <c r="AM33"/>
+      <c r="AP33" s="3"/>
+      <c r="AQ33" s="3"/>
+      <c r="AR33" s="3"/>
+      <c r="AS33" s="3"/>
+    </row>
+    <row r="34" spans="15:45" x14ac:dyDescent="0.25">
+      <c r="O34" s="3"/>
+      <c r="P34" s="3"/>
+      <c r="W34" s="3"/>
+      <c r="Y34" s="3"/>
+    </row>
+    <row r="35" spans="15:45" x14ac:dyDescent="0.25">
+      <c r="O35" s="3"/>
+      <c r="P35" s="3"/>
+      <c r="W35" s="3"/>
+      <c r="Y35" s="3"/>
+    </row>
+    <row r="36" spans="15:45" x14ac:dyDescent="0.25">
+      <c r="O36" s="3"/>
+      <c r="P36" s="3"/>
+      <c r="W36" s="3"/>
+      <c r="Y36" s="3"/>
+    </row>
+    <row r="37" spans="15:45" x14ac:dyDescent="0.25">
+      <c r="O37" s="3"/>
+      <c r="P37" s="3"/>
+      <c r="W37" s="3"/>
+      <c r="Y37" s="3"/>
+    </row>
+    <row r="38" spans="15:45" x14ac:dyDescent="0.25">
+      <c r="O38" s="3"/>
+      <c r="P38" s="3"/>
+      <c r="W38" s="3"/>
+      <c r="Y38" s="3"/>
+    </row>
+    <row r="39" spans="15:45" x14ac:dyDescent="0.25">
+      <c r="O39" s="3"/>
+      <c r="P39" s="3"/>
+      <c r="W39" s="3"/>
+      <c r="Y39" s="3"/>
+    </row>
+    <row r="40" spans="15:45" x14ac:dyDescent="0.25">
+      <c r="O40" s="3"/>
+      <c r="P40" s="3"/>
+      <c r="W40" s="3"/>
+      <c r="Y40" s="3"/>
+    </row>
+    <row r="41" spans="15:45" x14ac:dyDescent="0.25">
+      <c r="O41" s="3"/>
+      <c r="P41" s="3"/>
+      <c r="W41" s="3"/>
+      <c r="Y41" s="3"/>
+    </row>
+    <row r="42" spans="15:45" x14ac:dyDescent="0.25">
+      <c r="O42" s="3"/>
+      <c r="P42" s="3"/>
+      <c r="W42" s="3"/>
+      <c r="Y42" s="3"/>
+    </row>
+    <row r="43" spans="15:45" x14ac:dyDescent="0.25">
+      <c r="O43" s="3"/>
+      <c r="P43" s="3"/>
+      <c r="W43" s="3"/>
+      <c r="Y43" s="3"/>
+    </row>
+    <row r="44" spans="15:45" x14ac:dyDescent="0.25">
+      <c r="O44" s="3"/>
+      <c r="P44" s="3"/>
+      <c r="W44" s="3"/>
+      <c r="Y44" s="3"/>
+    </row>
+    <row r="45" spans="15:45" x14ac:dyDescent="0.25">
+      <c r="O45" s="3"/>
+      <c r="P45" s="3"/>
+      <c r="W45" s="3"/>
+      <c r="Y45" s="3"/>
+    </row>
+    <row r="46" spans="15:45" x14ac:dyDescent="0.25">
+      <c r="O46" s="3"/>
+      <c r="P46" s="3"/>
+      <c r="W46" s="3"/>
+      <c r="Y46" s="3"/>
+    </row>
+    <row r="47" spans="15:45" x14ac:dyDescent="0.25">
+      <c r="O47" s="3"/>
+      <c r="P47" s="3"/>
+      <c r="W47" s="3"/>
+      <c r="Y47" s="3"/>
+    </row>
+    <row r="48" spans="15:45" x14ac:dyDescent="0.25">
+      <c r="O48" s="3"/>
+      <c r="P48" s="3"/>
+      <c r="W48" s="3"/>
+      <c r="Y48" s="3"/>
+    </row>
+    <row r="49" spans="15:25" x14ac:dyDescent="0.25">
+      <c r="O49" s="3"/>
+      <c r="P49" s="3"/>
+      <c r="W49" s="3"/>
+      <c r="Y49" s="3"/>
+    </row>
+    <row r="50" spans="15:25" x14ac:dyDescent="0.25">
+      <c r="O50" s="3"/>
+      <c r="P50" s="3"/>
+      <c r="W50" s="3"/>
+      <c r="Y50" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16890,178 +17592,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>1105</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1110</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1108</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>848</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1109</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1111</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>679</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>1079</v>
-      </c>
-      <c r="C5" t="s">
-        <v>1119</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>1107</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1121</v>
-      </c>
-      <c r="C6" t="s">
-        <v>1120</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>1080</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1464</v>
-      </c>
-      <c r="C7" t="s">
-        <v>1465</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>1106</v>
-      </c>
-      <c r="B8" t="s">
-        <v>1123</v>
-      </c>
-      <c r="C8" t="s">
-        <v>1122</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>680</v>
-      </c>
-      <c r="B9" t="s">
-        <v>1469</v>
-      </c>
-      <c r="C9" t="s">
-        <v>1468</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>837</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>1571</v>
-      </c>
-      <c r="C10" t="s">
-        <v>1572</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>835</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>1605</v>
-      </c>
-      <c r="C12" t="s">
-        <v>1606</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>756</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>1603</v>
-      </c>
-      <c r="C13" t="s">
-        <v>1604</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>682</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>683</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>684</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>685</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>686</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1"/>
@@ -17082,7 +17613,178 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1105</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1108</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>848</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1109</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>679</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>1079</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1121</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1080</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1464</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1465</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1123</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>680</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1469</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1468</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>837</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>1571</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1572</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>835</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>1605</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1606</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>756</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>1603</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1604</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>686</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE883B56-0E73-42B4-A478-5009BC784D1A}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -17094,7 +17796,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2125</v>
+        <v>2099</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added related feats to Power class
</commit_message>
<xml_diff>
--- a/DND4eCharacterGenerator/Assets/ScrapeData.xlsx
+++ b/DND4eCharacterGenerator/Assets/ScrapeData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="9510" firstSheet="4" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="9510" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Referencer" sheetId="10" r:id="rId1"/>
@@ -190,7 +190,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4087" uniqueCount="2141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4089" uniqueCount="2142">
   <si>
     <t>Source</t>
   </si>
@@ -7178,7 +7178,10 @@
     <t>1d10 + (~CHAMod~)|2d10 + (~CHAMod~)</t>
   </si>
   <si>
-    <t>V</t>
+    <t>Aegis of Assault</t>
+  </si>
+  <si>
+    <t>W</t>
   </si>
 </sst>
 </file>
@@ -7268,7 +7271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -7294,6 +7297,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8624,7 +8630,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8843,10 +8849,10 @@
       </c>
       <c r="B16" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>2140</v>
+        <v>2141</v>
       </c>
       <c r="D16" s="3"/>
     </row>
@@ -11956,7 +11962,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -16578,10 +16586,10 @@
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <sheetPr codeName="Sheet9"/>
-  <dimension ref="A1:AU50"/>
+  <dimension ref="A1:AV50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+      <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16595,19 +16603,19 @@
     <col min="13" max="13" width="14.42578125" style="3" customWidth="1"/>
     <col min="15" max="15" width="16" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="16.85546875" customWidth="1"/>
-    <col min="17" max="20" width="9.140625" style="3"/>
-    <col min="21" max="22" width="10.28515625" style="3" customWidth="1"/>
-    <col min="23" max="23" width="15.5703125" customWidth="1"/>
-    <col min="24" max="24" width="16" style="3" customWidth="1"/>
-    <col min="26" max="26" width="9.140625" style="3"/>
-    <col min="27" max="27" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="15.85546875" style="3" customWidth="1"/>
-    <col min="29" max="29" width="9.28515625" style="3" customWidth="1"/>
-    <col min="31" max="33" width="9.140625" style="3"/>
-    <col min="36" max="41" width="9.140625" style="3"/>
+    <col min="17" max="21" width="9.140625" style="3"/>
+    <col min="22" max="23" width="10.28515625" style="3" customWidth="1"/>
+    <col min="24" max="24" width="15.5703125" customWidth="1"/>
+    <col min="25" max="25" width="16" style="3" customWidth="1"/>
+    <col min="27" max="27" width="9.140625" style="3"/>
+    <col min="28" max="28" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="15.85546875" style="3" customWidth="1"/>
+    <col min="30" max="30" width="9.28515625" style="3" customWidth="1"/>
+    <col min="32" max="34" width="9.140625" style="3"/>
+    <col min="37" max="42" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>690</v>
       </c>
@@ -16669,82 +16677,85 @@
         <v>2127</v>
       </c>
       <c r="U1" s="3" t="s">
+        <v>683</v>
+      </c>
+      <c r="V1" s="3" t="s">
         <v>1479</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>1480</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>2112</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>2114</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>2113</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>2115</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>2117</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>2118</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>2119</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>2120</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>2121</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>2123</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AH1" s="3" t="s">
         <v>2122</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>2124</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>2105</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AK1" s="3" t="s">
         <v>2125</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AL1" s="3" t="s">
         <v>2114</v>
       </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AM1" s="3" t="s">
         <v>2119</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AN1" s="3" t="s">
         <v>2120</v>
       </c>
-      <c r="AN1" s="3" t="s">
+      <c r="AO1" s="3" t="s">
         <v>2105</v>
       </c>
-      <c r="AO1" s="3" t="s">
+      <c r="AP1" s="3" t="s">
         <v>2125</v>
       </c>
-      <c r="AP1" s="3" t="s">
+      <c r="AQ1" s="3" t="s">
         <v>2114</v>
       </c>
-      <c r="AQ1" s="3" t="s">
+      <c r="AR1" s="3" t="s">
         <v>2119</v>
       </c>
-      <c r="AR1" s="3" t="s">
+      <c r="AS1" s="3" t="s">
         <v>2120</v>
       </c>
-      <c r="AS1" s="3"/>
       <c r="AT1" s="3"/>
       <c r="AU1" s="3"/>
-    </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AV1" s="3"/>
+    </row>
+    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2070</v>
       </c>
@@ -16793,41 +16804,41 @@
       <c r="P2" t="s">
         <v>1083</v>
       </c>
-      <c r="U2" s="3" t="str">
-        <f>IF(W2&lt;&gt;"",$W$1,"")&amp;IF(X2&lt;&gt;"","|"&amp;$X$1,"")&amp;IF(Y2&lt;&gt;"","|"&amp;$Y$1,"")&amp;IF(Z2&lt;&gt;"","|"&amp;$Z$1,"")&amp;IF(AA2&lt;&gt;"","|"&amp;$AA$1,"")&amp;IF(AB2&lt;&gt;"","|"&amp;$AB$1,"")&amp;IF(AC2&lt;&gt;"","|"&amp;$AC$1,"")&amp;IF(AD2&lt;&gt;"","|"&amp;$AD$1,"")&amp;IF(AE2&lt;&gt;"","|"&amp;$AE$1,"")&amp;IF(AF2&lt;&gt;"","|"&amp;$AF$1,"")&amp;IF(AG2&lt;&gt;"","|"&amp;$AG$1,"")&amp;IF(AH2&lt;&gt;"","|"&amp;$AH$1,"")&amp;IF(AI2&lt;&gt;"","|"&amp;$AI$1,"")&amp;IF(AJ2&lt;&gt;"","|"&amp;$AJ$1,"")&amp;IF(AK2&lt;&gt;"","|"&amp;$AK$1,"")&amp;IF(AL2&lt;&gt;"","|"&amp;$AL$1,"")&amp;IF(AM2&lt;&gt;"","|"&amp;$AM$1,"")&amp;IF(AN2&lt;&gt;"","|"&amp;$AN$1,"")&amp;IF(AO2&lt;&gt;"","|"&amp;$AO$1,"")&amp;IF(AP2&lt;&gt;"","|"&amp;$AP$1,"")&amp;IF(AQ2&lt;&gt;"","|"&amp;$AQ$1,"")&amp;IF(AR2&lt;&gt;"","|"&amp;$AR$1,"")&amp;IF(AS2&lt;&gt;"","|"&amp;$AS$1,"")&amp;IF(AT2&lt;&gt;"","|"&amp;$AT$1,"")&amp;IF(AU2&lt;&gt;"","|"&amp;$AU$1,"")&amp;IF(AV2&lt;&gt;"","|"&amp;$AV$1,"")&amp;IF(AW2&lt;&gt;"","|"&amp;$AW$1,"")&amp;IF(AX2&lt;&gt;"","|"&amp;$AX$1,"")&amp;IF(AY2&lt;&gt;"","|"&amp;$AY$1,"")&amp;IF(AZ2&lt;&gt;"","|"&amp;$AZ$1,"")&amp;IF(BA2&lt;&gt;"","|"&amp;$BA$1,"")&amp;IF(BB2&lt;&gt;"","|"&amp;$BB$1,"")&amp;IF(BC2&lt;&gt;"","|"&amp;$BC$1,"")&amp;IF(BD2&lt;&gt;"","|"&amp;$BD$1,"")&amp;IF(BE2&lt;&gt;"","|"&amp;$BE$1,"")&amp;IF(BF2&lt;&gt;"","|"&amp;$BF$1,"")&amp;IF(BG2&lt;&gt;"","|"&amp;$BG$1,"")&amp;IF(BH2&lt;&gt;"","|"&amp;$BH$1,"")</f>
+      <c r="V2" s="3" t="str">
+        <f>IF(X2&lt;&gt;"",$X$1,"")&amp;IF(Y2&lt;&gt;"","|"&amp;$Y$1,"")&amp;IF(Z2&lt;&gt;"","|"&amp;$Z$1,"")&amp;IF(AA2&lt;&gt;"","|"&amp;$AA$1,"")&amp;IF(AB2&lt;&gt;"","|"&amp;$AB$1,"")&amp;IF(AC2&lt;&gt;"","|"&amp;$AC$1,"")&amp;IF(AD2&lt;&gt;"","|"&amp;$AD$1,"")&amp;IF(AE2&lt;&gt;"","|"&amp;$AE$1,"")&amp;IF(AF2&lt;&gt;"","|"&amp;$AF$1,"")&amp;IF(AG2&lt;&gt;"","|"&amp;$AG$1,"")&amp;IF(AH2&lt;&gt;"","|"&amp;$AH$1,"")&amp;IF(AI2&lt;&gt;"","|"&amp;$AI$1,"")&amp;IF(AJ2&lt;&gt;"","|"&amp;$AJ$1,"")&amp;IF(AK2&lt;&gt;"","|"&amp;$AK$1,"")&amp;IF(AL2&lt;&gt;"","|"&amp;$AL$1,"")&amp;IF(AM2&lt;&gt;"","|"&amp;$AM$1,"")&amp;IF(AN2&lt;&gt;"","|"&amp;$AN$1,"")&amp;IF(AO2&lt;&gt;"","|"&amp;$AO$1,"")&amp;IF(AP2&lt;&gt;"","|"&amp;$AP$1,"")&amp;IF(AQ2&lt;&gt;"","|"&amp;$AQ$1,"")&amp;IF(AR2&lt;&gt;"","|"&amp;$AR$1,"")&amp;IF(AS2&lt;&gt;"","|"&amp;$AS$1,"")&amp;IF(AT2&lt;&gt;"","|"&amp;$AT$1,"")&amp;IF(AU2&lt;&gt;"","|"&amp;$AU$1,"")&amp;IF(AV2&lt;&gt;"","|"&amp;$AV$1,"")&amp;IF(AW2&lt;&gt;"","|"&amp;$AW$1,"")&amp;IF(AX2&lt;&gt;"","|"&amp;$AX$1,"")&amp;IF(AY2&lt;&gt;"","|"&amp;$AY$1,"")&amp;IF(AZ2&lt;&gt;"","|"&amp;$AZ$1,"")&amp;IF(BA2&lt;&gt;"","|"&amp;$BA$1,"")&amp;IF(BB2&lt;&gt;"","|"&amp;$BB$1,"")&amp;IF(BC2&lt;&gt;"","|"&amp;$BC$1,"")&amp;IF(BD2&lt;&gt;"","|"&amp;$BD$1,"")&amp;IF(BE2&lt;&gt;"","|"&amp;$BE$1,"")&amp;IF(BF2&lt;&gt;"","|"&amp;$BF$1,"")&amp;IF(BG2&lt;&gt;"","|"&amp;$BG$1,"")&amp;IF(BH2&lt;&gt;"","|"&amp;$BH$1,"")&amp;IF(BI2&lt;&gt;"","|"&amp;$BI$1,"")</f>
         <v>Flavor:|Prerequisite:|Keywords:|Attack:|Hit:</v>
       </c>
-      <c r="V2" s="3" t="str">
-        <f>IF(W2&lt;&gt;"",W2,"")&amp;IF(X2&lt;&gt;"","|"&amp;X2,"")&amp;IF(Y2&lt;&gt;"","|"&amp;Y2,"")&amp;IF(Z2&lt;&gt;"","|"&amp;Z2,"")&amp;IF(AA2&lt;&gt;"","|"&amp;AA2,"")&amp;IF(AB2&lt;&gt;"","|"&amp;AB2,"")&amp;IF(AC2&lt;&gt;"","|"&amp;AC2,"")&amp;IF(AD2&lt;&gt;"","|"&amp;AD2,"")&amp;IF(AE2&lt;&gt;"","|"&amp;AE2,"")&amp;IF(AF2&lt;&gt;"","|"&amp;AF2,"")&amp;IF(AG2&lt;&gt;"","|"&amp;AG2,"")&amp;IF(AH2&lt;&gt;"","|"&amp;AH2,"")&amp;IF(AI2&lt;&gt;"","|"&amp;AI2,"")&amp;IF(AJ2&lt;&gt;"","|"&amp;AJ2,"")&amp;IF(AK2&lt;&gt;"","|"&amp;AK2,"")&amp;IF(AL2&lt;&gt;"","|"&amp;AL2,"")&amp;IF(AM2&lt;&gt;"","|"&amp;AM2,"")&amp;IF(AN2&lt;&gt;"","|"&amp;AN2,"")&amp;IF(AO2&lt;&gt;"","|"&amp;AO2,"")&amp;IF(AP2&lt;&gt;"","|"&amp;AP2,"")&amp;IF(AQ2&lt;&gt;"","|"&amp;AQ2,"")&amp;IF(AR2&lt;&gt;"","|"&amp;AR2,"")&amp;IF(AS2&lt;&gt;"","|"&amp;AS2,"")&amp;IF(AT2&lt;&gt;"","|"&amp;AT2,"")&amp;IF(AU2&lt;&gt;"","|"&amp;AU2,"")&amp;IF(AV2&lt;&gt;"","|"&amp;AV2,"")&amp;IF(AW2&lt;&gt;"","|"&amp;AW2,"")&amp;IF(AX2&lt;&gt;"","|"&amp;AX2,"")&amp;IF(AY2&lt;&gt;"","|"&amp;AY2,"")&amp;IF(AZ2&lt;&gt;"","|"&amp;AZ2,"")&amp;IF(BA2&lt;&gt;"","|"&amp;BA2,"")&amp;IF(BB2&lt;&gt;"","|"&amp;BB2,"")&amp;IF(BC2&lt;&gt;"","|"&amp;BC2,"")&amp;IF(BD2&lt;&gt;"","|"&amp;BD2,"")&amp;IF(BE2&lt;&gt;"","|"&amp;BE2,"")&amp;IF(BF2&lt;&gt;"","|"&amp;BF2,"")&amp;IF(BG2&lt;&gt;"","|"&amp;BG2,"")&amp;IF(BH2&lt;&gt;"","|"&amp;BH2,"")</f>
+      <c r="W2" s="3" t="str">
+        <f>IF(X2&lt;&gt;"",X2,"")&amp;IF(Y2&lt;&gt;"","|"&amp;Y2,"")&amp;IF(Z2&lt;&gt;"","|"&amp;Z2,"")&amp;IF(AA2&lt;&gt;"","|"&amp;AA2,"")&amp;IF(AB2&lt;&gt;"","|"&amp;AB2,"")&amp;IF(AC2&lt;&gt;"","|"&amp;AC2,"")&amp;IF(AD2&lt;&gt;"","|"&amp;AD2,"")&amp;IF(AE2&lt;&gt;"","|"&amp;AE2,"")&amp;IF(AF2&lt;&gt;"","|"&amp;AF2,"")&amp;IF(AG2&lt;&gt;"","|"&amp;AG2,"")&amp;IF(AH2&lt;&gt;"","|"&amp;AH2,"")&amp;IF(AI2&lt;&gt;"","|"&amp;AI2,"")&amp;IF(AJ2&lt;&gt;"","|"&amp;AJ2,"")&amp;IF(AK2&lt;&gt;"","|"&amp;AK2,"")&amp;IF(AL2&lt;&gt;"","|"&amp;AL2,"")&amp;IF(AM2&lt;&gt;"","|"&amp;AM2,"")&amp;IF(AN2&lt;&gt;"","|"&amp;AN2,"")&amp;IF(AO2&lt;&gt;"","|"&amp;AO2,"")&amp;IF(AP2&lt;&gt;"","|"&amp;AP2,"")&amp;IF(AQ2&lt;&gt;"","|"&amp;AQ2,"")&amp;IF(AR2&lt;&gt;"","|"&amp;AR2,"")&amp;IF(AS2&lt;&gt;"","|"&amp;AS2,"")&amp;IF(AT2&lt;&gt;"","|"&amp;AT2,"")&amp;IF(AU2&lt;&gt;"","|"&amp;AU2,"")&amp;IF(AV2&lt;&gt;"","|"&amp;AV2,"")&amp;IF(AW2&lt;&gt;"","|"&amp;AW2,"")&amp;IF(AX2&lt;&gt;"","|"&amp;AX2,"")&amp;IF(AY2&lt;&gt;"","|"&amp;AY2,"")&amp;IF(AZ2&lt;&gt;"","|"&amp;AZ2,"")&amp;IF(BA2&lt;&gt;"","|"&amp;BA2,"")&amp;IF(BB2&lt;&gt;"","|"&amp;BB2,"")&amp;IF(BC2&lt;&gt;"","|"&amp;BC2,"")&amp;IF(BD2&lt;&gt;"","|"&amp;BD2,"")&amp;IF(BE2&lt;&gt;"","|"&amp;BE2,"")&amp;IF(BF2&lt;&gt;"","|"&amp;BF2,"")&amp;IF(BG2&lt;&gt;"","|"&amp;BG2,"")&amp;IF(BH2&lt;&gt;"","|"&amp;BH2,"")&amp;IF(BI2&lt;&gt;"","|"&amp;BI2,"")</f>
         <v>You strike at your horrid enemy, using your knowledge of its strengths and weaknesses to twist the knife just a bit more.|You must be trained in Dungeoneering|Martial, Weapon|Dexterity vs AC|1[W] + Dexterity modifier (~DEXMod~). If the target is aberrant and has resistance or vulnerability to your attack, you gain a bonus to damage equal to your Wisdom modifier (~WISMod~).
 Level 21: 2[W] + Dexterity modifier (~DEXMod~).</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>2071</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>2078</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>2129</v>
       </c>
-      <c r="AC2" s="3" t="s">
+      <c r="AD2" s="3" t="s">
         <v>2103</v>
       </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>2130</v>
       </c>
-      <c r="AE2" s="1"/>
       <c r="AF2" s="1"/>
       <c r="AG2" s="1"/>
-      <c r="AP2" s="3"/>
+      <c r="AH2" s="1"/>
       <c r="AQ2" s="3"/>
       <c r="AR2" s="3"/>
       <c r="AS2" s="3"/>
       <c r="AT2" s="3"/>
       <c r="AU2" s="3"/>
-    </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AV2" s="3"/>
+    </row>
+    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2082</v>
       </c>
@@ -16870,35 +16881,35 @@
       <c r="N3" t="s">
         <v>2102</v>
       </c>
-      <c r="U3" s="3" t="str">
-        <f>IF(W3&lt;&gt;"",$W$1,"")&amp;IF(X3&lt;&gt;"","|"&amp;$X$1,"")&amp;IF(Y3&lt;&gt;"","|"&amp;$Y$1,"")&amp;IF(Z3&lt;&gt;"","|"&amp;$Z$1,"")&amp;IF(AA3&lt;&gt;"","|"&amp;$AA$1,"")&amp;IF(AB3&lt;&gt;"","|"&amp;$AB$1,"")&amp;IF(AC3&lt;&gt;"","|"&amp;$AC$1,"")&amp;IF(AD3&lt;&gt;"","|"&amp;$AD$1,"")&amp;IF(AE3&lt;&gt;"","|"&amp;$AE$1,"")&amp;IF(AF3&lt;&gt;"","|"&amp;$AF$1,"")&amp;IF(AG3&lt;&gt;"","|"&amp;$AG$1,"")&amp;IF(AH3&lt;&gt;"","|"&amp;$AH$1,"")&amp;IF(AI3&lt;&gt;"","|"&amp;$AI$1,"")&amp;IF(AJ3&lt;&gt;"","|"&amp;$AJ$1,"")&amp;IF(AK3&lt;&gt;"","|"&amp;$AK$1,"")&amp;IF(AL3&lt;&gt;"","|"&amp;$AL$1,"")&amp;IF(AM3&lt;&gt;"","|"&amp;$AM$1,"")&amp;IF(AN3&lt;&gt;"","|"&amp;$AN$1,"")&amp;IF(AO3&lt;&gt;"","|"&amp;$AO$1,"")&amp;IF(AP3&lt;&gt;"","|"&amp;$AP$1,"")&amp;IF(AQ3&lt;&gt;"","|"&amp;$AQ$1,"")&amp;IF(AR3&lt;&gt;"","|"&amp;$AR$1,"")&amp;IF(AS3&lt;&gt;"","|"&amp;$AS$1,"")&amp;IF(AT3&lt;&gt;"","|"&amp;$AT$1,"")&amp;IF(AU3&lt;&gt;"","|"&amp;$AU$1,"")&amp;IF(AV3&lt;&gt;"","|"&amp;$AV$1,"")&amp;IF(AW3&lt;&gt;"","|"&amp;$AW$1,"")&amp;IF(AX3&lt;&gt;"","|"&amp;$AX$1,"")&amp;IF(AY3&lt;&gt;"","|"&amp;$AY$1,"")&amp;IF(AZ3&lt;&gt;"","|"&amp;$AZ$1,"")&amp;IF(BA3&lt;&gt;"","|"&amp;$BA$1,"")&amp;IF(BB3&lt;&gt;"","|"&amp;$BB$1,"")&amp;IF(BC3&lt;&gt;"","|"&amp;$BC$1,"")&amp;IF(BD3&lt;&gt;"","|"&amp;$BD$1,"")&amp;IF(BE3&lt;&gt;"","|"&amp;$BE$1,"")&amp;IF(BF3&lt;&gt;"","|"&amp;$BF$1,"")&amp;IF(BG3&lt;&gt;"","|"&amp;$BG$1,"")&amp;IF(BH3&lt;&gt;"","|"&amp;$BH$1,"")</f>
+      <c r="V3" s="3" t="str">
+        <f>IF(X3&lt;&gt;"",$X$1,"")&amp;IF(Y3&lt;&gt;"","|"&amp;$Y$1,"")&amp;IF(Z3&lt;&gt;"","|"&amp;$Z$1,"")&amp;IF(AA3&lt;&gt;"","|"&amp;$AA$1,"")&amp;IF(AB3&lt;&gt;"","|"&amp;$AB$1,"")&amp;IF(AC3&lt;&gt;"","|"&amp;$AC$1,"")&amp;IF(AD3&lt;&gt;"","|"&amp;$AD$1,"")&amp;IF(AE3&lt;&gt;"","|"&amp;$AE$1,"")&amp;IF(AF3&lt;&gt;"","|"&amp;$AF$1,"")&amp;IF(AG3&lt;&gt;"","|"&amp;$AG$1,"")&amp;IF(AH3&lt;&gt;"","|"&amp;$AH$1,"")&amp;IF(AI3&lt;&gt;"","|"&amp;$AI$1,"")&amp;IF(AJ3&lt;&gt;"","|"&amp;$AJ$1,"")&amp;IF(AK3&lt;&gt;"","|"&amp;$AK$1,"")&amp;IF(AL3&lt;&gt;"","|"&amp;$AL$1,"")&amp;IF(AM3&lt;&gt;"","|"&amp;$AM$1,"")&amp;IF(AN3&lt;&gt;"","|"&amp;$AN$1,"")&amp;IF(AO3&lt;&gt;"","|"&amp;$AO$1,"")&amp;IF(AP3&lt;&gt;"","|"&amp;$AP$1,"")&amp;IF(AQ3&lt;&gt;"","|"&amp;$AQ$1,"")&amp;IF(AR3&lt;&gt;"","|"&amp;$AR$1,"")&amp;IF(AS3&lt;&gt;"","|"&amp;$AS$1,"")&amp;IF(AT3&lt;&gt;"","|"&amp;$AT$1,"")&amp;IF(AU3&lt;&gt;"","|"&amp;$AU$1,"")&amp;IF(AV3&lt;&gt;"","|"&amp;$AV$1,"")&amp;IF(AW3&lt;&gt;"","|"&amp;$AW$1,"")&amp;IF(AX3&lt;&gt;"","|"&amp;$AX$1,"")&amp;IF(AY3&lt;&gt;"","|"&amp;$AY$1,"")&amp;IF(AZ3&lt;&gt;"","|"&amp;$AZ$1,"")&amp;IF(BA3&lt;&gt;"","|"&amp;$BA$1,"")&amp;IF(BB3&lt;&gt;"","|"&amp;$BB$1,"")&amp;IF(BC3&lt;&gt;"","|"&amp;$BC$1,"")&amp;IF(BD3&lt;&gt;"","|"&amp;$BD$1,"")&amp;IF(BE3&lt;&gt;"","|"&amp;$BE$1,"")&amp;IF(BF3&lt;&gt;"","|"&amp;$BF$1,"")&amp;IF(BG3&lt;&gt;"","|"&amp;$BG$1,"")&amp;IF(BH3&lt;&gt;"","|"&amp;$BH$1,"")&amp;IF(BI3&lt;&gt;"","|"&amp;$BI$1,"")</f>
         <v>|Keywords:|Attack:|Hit:</v>
       </c>
-      <c r="V3" s="3" t="str">
-        <f>IF(W3&lt;&gt;"",W3,"")&amp;IF(X3&lt;&gt;"","|"&amp;X3,"")&amp;IF(Y3&lt;&gt;"","|"&amp;Y3,"")&amp;IF(Z3&lt;&gt;"","|"&amp;Z3,"")&amp;IF(AA3&lt;&gt;"","|"&amp;AA3,"")&amp;IF(AB3&lt;&gt;"","|"&amp;AB3,"")&amp;IF(AC3&lt;&gt;"","|"&amp;AC3,"")&amp;IF(AD3&lt;&gt;"","|"&amp;AD3,"")&amp;IF(AE3&lt;&gt;"","|"&amp;AE3,"")&amp;IF(AF3&lt;&gt;"","|"&amp;AF3,"")&amp;IF(AG3&lt;&gt;"","|"&amp;AG3,"")&amp;IF(AH3&lt;&gt;"","|"&amp;AH3,"")&amp;IF(AI3&lt;&gt;"","|"&amp;AI3,"")&amp;IF(AJ3&lt;&gt;"","|"&amp;AJ3,"")&amp;IF(AK3&lt;&gt;"","|"&amp;AK3,"")&amp;IF(AL3&lt;&gt;"","|"&amp;AL3,"")&amp;IF(AM3&lt;&gt;"","|"&amp;AM3,"")&amp;IF(AN3&lt;&gt;"","|"&amp;AN3,"")&amp;IF(AO3&lt;&gt;"","|"&amp;AO3,"")&amp;IF(AP3&lt;&gt;"","|"&amp;AP3,"")&amp;IF(AQ3&lt;&gt;"","|"&amp;AQ3,"")&amp;IF(AR3&lt;&gt;"","|"&amp;AR3,"")&amp;IF(AS3&lt;&gt;"","|"&amp;AS3,"")&amp;IF(AT3&lt;&gt;"","|"&amp;AT3,"")&amp;IF(AU3&lt;&gt;"","|"&amp;AU3,"")&amp;IF(AV3&lt;&gt;"","|"&amp;AV3,"")&amp;IF(AW3&lt;&gt;"","|"&amp;AW3,"")&amp;IF(AX3&lt;&gt;"","|"&amp;AX3,"")&amp;IF(AY3&lt;&gt;"","|"&amp;AY3,"")&amp;IF(AZ3&lt;&gt;"","|"&amp;AZ3,"")&amp;IF(BA3&lt;&gt;"","|"&amp;BA3,"")&amp;IF(BB3&lt;&gt;"","|"&amp;BB3,"")&amp;IF(BC3&lt;&gt;"","|"&amp;BC3,"")&amp;IF(BD3&lt;&gt;"","|"&amp;BD3,"")&amp;IF(BE3&lt;&gt;"","|"&amp;BE3,"")&amp;IF(BF3&lt;&gt;"","|"&amp;BF3,"")&amp;IF(BG3&lt;&gt;"","|"&amp;BG3,"")&amp;IF(BH3&lt;&gt;"","|"&amp;BH3,"")</f>
+      <c r="W3" s="3" t="str">
+        <f>IF(X3&lt;&gt;"",X3,"")&amp;IF(Y3&lt;&gt;"","|"&amp;Y3,"")&amp;IF(Z3&lt;&gt;"","|"&amp;Z3,"")&amp;IF(AA3&lt;&gt;"","|"&amp;AA3,"")&amp;IF(AB3&lt;&gt;"","|"&amp;AB3,"")&amp;IF(AC3&lt;&gt;"","|"&amp;AC3,"")&amp;IF(AD3&lt;&gt;"","|"&amp;AD3,"")&amp;IF(AE3&lt;&gt;"","|"&amp;AE3,"")&amp;IF(AF3&lt;&gt;"","|"&amp;AF3,"")&amp;IF(AG3&lt;&gt;"","|"&amp;AG3,"")&amp;IF(AH3&lt;&gt;"","|"&amp;AH3,"")&amp;IF(AI3&lt;&gt;"","|"&amp;AI3,"")&amp;IF(AJ3&lt;&gt;"","|"&amp;AJ3,"")&amp;IF(AK3&lt;&gt;"","|"&amp;AK3,"")&amp;IF(AL3&lt;&gt;"","|"&amp;AL3,"")&amp;IF(AM3&lt;&gt;"","|"&amp;AM3,"")&amp;IF(AN3&lt;&gt;"","|"&amp;AN3,"")&amp;IF(AO3&lt;&gt;"","|"&amp;AO3,"")&amp;IF(AP3&lt;&gt;"","|"&amp;AP3,"")&amp;IF(AQ3&lt;&gt;"","|"&amp;AQ3,"")&amp;IF(AR3&lt;&gt;"","|"&amp;AR3,"")&amp;IF(AS3&lt;&gt;"","|"&amp;AS3,"")&amp;IF(AT3&lt;&gt;"","|"&amp;AT3,"")&amp;IF(AU3&lt;&gt;"","|"&amp;AU3,"")&amp;IF(AV3&lt;&gt;"","|"&amp;AV3,"")&amp;IF(AW3&lt;&gt;"","|"&amp;AW3,"")&amp;IF(AX3&lt;&gt;"","|"&amp;AX3,"")&amp;IF(AY3&lt;&gt;"","|"&amp;AY3,"")&amp;IF(AZ3&lt;&gt;"","|"&amp;AZ3,"")&amp;IF(BA3&lt;&gt;"","|"&amp;BA3,"")&amp;IF(BB3&lt;&gt;"","|"&amp;BB3,"")&amp;IF(BC3&lt;&gt;"","|"&amp;BC3,"")&amp;IF(BD3&lt;&gt;"","|"&amp;BD3,"")&amp;IF(BE3&lt;&gt;"","|"&amp;BE3,"")&amp;IF(BF3&lt;&gt;"","|"&amp;BF3,"")&amp;IF(BG3&lt;&gt;"","|"&amp;BG3,"")&amp;IF(BH3&lt;&gt;"","|"&amp;BH3,"")&amp;IF(BI3&lt;&gt;"","|"&amp;BI3,"")</f>
         <v>|Acid, Arcane, Implement|Charisma vs Reflexes|1d10 + Charisma modifier (~CHAMod~) acid damage.
 Level 21: 2d10 + Charisma modifier (~CHAMod~) acid damage.</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AB3" t="s">
         <v>2128</v>
       </c>
-      <c r="AC3" s="3" t="s">
+      <c r="AD3" s="3" t="s">
         <v>2104</v>
       </c>
-      <c r="AD3" s="1" t="s">
+      <c r="AE3" s="1" t="s">
         <v>2131</v>
       </c>
-      <c r="AE3" s="1"/>
       <c r="AF3" s="1"/>
       <c r="AG3" s="1"/>
-      <c r="AP3" s="3"/>
+      <c r="AH3" s="1"/>
       <c r="AQ3" s="3"/>
       <c r="AR3" s="3"/>
       <c r="AS3" s="3"/>
       <c r="AT3" s="3"/>
       <c r="AU3" s="3"/>
-    </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AV3" s="3"/>
+    </row>
+    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2083</v>
       </c>
@@ -16929,33 +16940,33 @@
       <c r="P4" t="s">
         <v>265</v>
       </c>
-      <c r="U4" s="3" t="str">
-        <f>IF(W4&lt;&gt;"",$W$1,"")&amp;IF(X4&lt;&gt;"","|"&amp;$X$1,"")&amp;IF(Y4&lt;&gt;"","|"&amp;$Y$1,"")&amp;IF(Z4&lt;&gt;"","|"&amp;$Z$1,"")&amp;IF(AA4&lt;&gt;"","|"&amp;$AA$1,"")&amp;IF(AB4&lt;&gt;"","|"&amp;$AB$1,"")&amp;IF(AC4&lt;&gt;"","|"&amp;$AC$1,"")&amp;IF(AD4&lt;&gt;"","|"&amp;$AD$1,"")&amp;IF(AE4&lt;&gt;"","|"&amp;$AE$1,"")&amp;IF(AF4&lt;&gt;"","|"&amp;$AF$1,"")&amp;IF(AG4&lt;&gt;"","|"&amp;$AG$1,"")&amp;IF(AH4&lt;&gt;"","|"&amp;$AH$1,"")&amp;IF(AI4&lt;&gt;"","|"&amp;$AI$1,"")&amp;IF(AJ4&lt;&gt;"","|"&amp;$AJ$1,"")&amp;IF(AK4&lt;&gt;"","|"&amp;$AK$1,"")&amp;IF(AL4&lt;&gt;"","|"&amp;$AL$1,"")&amp;IF(AM4&lt;&gt;"","|"&amp;$AM$1,"")&amp;IF(AN4&lt;&gt;"","|"&amp;$AN$1,"")&amp;IF(AO4&lt;&gt;"","|"&amp;$AO$1,"")&amp;IF(AP4&lt;&gt;"","|"&amp;$AP$1,"")&amp;IF(AQ4&lt;&gt;"","|"&amp;$AQ$1,"")&amp;IF(AR4&lt;&gt;"","|"&amp;$AR$1,"")&amp;IF(AS4&lt;&gt;"","|"&amp;$AS$1,"")&amp;IF(AT4&lt;&gt;"","|"&amp;$AT$1,"")&amp;IF(AU4&lt;&gt;"","|"&amp;$AU$1,"")&amp;IF(AV4&lt;&gt;"","|"&amp;$AV$1,"")&amp;IF(AW4&lt;&gt;"","|"&amp;$AW$1,"")&amp;IF(AX4&lt;&gt;"","|"&amp;$AX$1,"")&amp;IF(AY4&lt;&gt;"","|"&amp;$AY$1,"")&amp;IF(AZ4&lt;&gt;"","|"&amp;$AZ$1,"")&amp;IF(BA4&lt;&gt;"","|"&amp;$BA$1,"")&amp;IF(BB4&lt;&gt;"","|"&amp;$BB$1,"")&amp;IF(BC4&lt;&gt;"","|"&amp;$BC$1,"")&amp;IF(BD4&lt;&gt;"","|"&amp;$BD$1,"")&amp;IF(BE4&lt;&gt;"","|"&amp;$BE$1,"")&amp;IF(BF4&lt;&gt;"","|"&amp;$BF$1,"")&amp;IF(BG4&lt;&gt;"","|"&amp;$BG$1,"")&amp;IF(BH4&lt;&gt;"","|"&amp;$BH$1,"")</f>
+      <c r="V4" s="3" t="str">
+        <f>IF(X4&lt;&gt;"",$X$1,"")&amp;IF(Y4&lt;&gt;"","|"&amp;$Y$1,"")&amp;IF(Z4&lt;&gt;"","|"&amp;$Z$1,"")&amp;IF(AA4&lt;&gt;"","|"&amp;$AA$1,"")&amp;IF(AB4&lt;&gt;"","|"&amp;$AB$1,"")&amp;IF(AC4&lt;&gt;"","|"&amp;$AC$1,"")&amp;IF(AD4&lt;&gt;"","|"&amp;$AD$1,"")&amp;IF(AE4&lt;&gt;"","|"&amp;$AE$1,"")&amp;IF(AF4&lt;&gt;"","|"&amp;$AF$1,"")&amp;IF(AG4&lt;&gt;"","|"&amp;$AG$1,"")&amp;IF(AH4&lt;&gt;"","|"&amp;$AH$1,"")&amp;IF(AI4&lt;&gt;"","|"&amp;$AI$1,"")&amp;IF(AJ4&lt;&gt;"","|"&amp;$AJ$1,"")&amp;IF(AK4&lt;&gt;"","|"&amp;$AK$1,"")&amp;IF(AL4&lt;&gt;"","|"&amp;$AL$1,"")&amp;IF(AM4&lt;&gt;"","|"&amp;$AM$1,"")&amp;IF(AN4&lt;&gt;"","|"&amp;$AN$1,"")&amp;IF(AO4&lt;&gt;"","|"&amp;$AO$1,"")&amp;IF(AP4&lt;&gt;"","|"&amp;$AP$1,"")&amp;IF(AQ4&lt;&gt;"","|"&amp;$AQ$1,"")&amp;IF(AR4&lt;&gt;"","|"&amp;$AR$1,"")&amp;IF(AS4&lt;&gt;"","|"&amp;$AS$1,"")&amp;IF(AT4&lt;&gt;"","|"&amp;$AT$1,"")&amp;IF(AU4&lt;&gt;"","|"&amp;$AU$1,"")&amp;IF(AV4&lt;&gt;"","|"&amp;$AV$1,"")&amp;IF(AW4&lt;&gt;"","|"&amp;$AW$1,"")&amp;IF(AX4&lt;&gt;"","|"&amp;$AX$1,"")&amp;IF(AY4&lt;&gt;"","|"&amp;$AY$1,"")&amp;IF(AZ4&lt;&gt;"","|"&amp;$AZ$1,"")&amp;IF(BA4&lt;&gt;"","|"&amp;$BA$1,"")&amp;IF(BB4&lt;&gt;"","|"&amp;$BB$1,"")&amp;IF(BC4&lt;&gt;"","|"&amp;$BC$1,"")&amp;IF(BD4&lt;&gt;"","|"&amp;$BD$1,"")&amp;IF(BE4&lt;&gt;"","|"&amp;$BE$1,"")&amp;IF(BF4&lt;&gt;"","|"&amp;$BF$1,"")&amp;IF(BG4&lt;&gt;"","|"&amp;$BG$1,"")&amp;IF(BH4&lt;&gt;"","|"&amp;$BH$1,"")&amp;IF(BI4&lt;&gt;"","|"&amp;$BI$1,"")</f>
         <v>|Prerequisite:|Keywords:|Effect:</v>
       </c>
-      <c r="V4" s="3" t="str">
-        <f>IF(W4&lt;&gt;"",W4,"")&amp;IF(X4&lt;&gt;"","|"&amp;X4,"")&amp;IF(Y4&lt;&gt;"","|"&amp;Y4,"")&amp;IF(Z4&lt;&gt;"","|"&amp;Z4,"")&amp;IF(AA4&lt;&gt;"","|"&amp;AA4,"")&amp;IF(AB4&lt;&gt;"","|"&amp;AB4,"")&amp;IF(AC4&lt;&gt;"","|"&amp;AC4,"")&amp;IF(AD4&lt;&gt;"","|"&amp;AD4,"")&amp;IF(AE4&lt;&gt;"","|"&amp;AE4,"")&amp;IF(AF4&lt;&gt;"","|"&amp;AF4,"")&amp;IF(AG4&lt;&gt;"","|"&amp;AG4,"")&amp;IF(AH4&lt;&gt;"","|"&amp;AH4,"")&amp;IF(AI4&lt;&gt;"","|"&amp;AI4,"")&amp;IF(AJ4&lt;&gt;"","|"&amp;AJ4,"")&amp;IF(AK4&lt;&gt;"","|"&amp;AK4,"")&amp;IF(AL4&lt;&gt;"","|"&amp;AL4,"")&amp;IF(AM4&lt;&gt;"","|"&amp;AM4,"")&amp;IF(AN4&lt;&gt;"","|"&amp;AN4,"")&amp;IF(AO4&lt;&gt;"","|"&amp;AO4,"")&amp;IF(AP4&lt;&gt;"","|"&amp;AP4,"")&amp;IF(AQ4&lt;&gt;"","|"&amp;AQ4,"")&amp;IF(AR4&lt;&gt;"","|"&amp;AR4,"")&amp;IF(AS4&lt;&gt;"","|"&amp;AS4,"")&amp;IF(AT4&lt;&gt;"","|"&amp;AT4,"")&amp;IF(AU4&lt;&gt;"","|"&amp;AU4,"")&amp;IF(AV4&lt;&gt;"","|"&amp;AV4,"")&amp;IF(AW4&lt;&gt;"","|"&amp;AW4,"")&amp;IF(AX4&lt;&gt;"","|"&amp;AX4,"")&amp;IF(AY4&lt;&gt;"","|"&amp;AY4,"")&amp;IF(AZ4&lt;&gt;"","|"&amp;AZ4,"")&amp;IF(BA4&lt;&gt;"","|"&amp;BA4,"")&amp;IF(BB4&lt;&gt;"","|"&amp;BB4,"")&amp;IF(BC4&lt;&gt;"","|"&amp;BC4,"")&amp;IF(BD4&lt;&gt;"","|"&amp;BD4,"")&amp;IF(BE4&lt;&gt;"","|"&amp;BE4,"")&amp;IF(BF4&lt;&gt;"","|"&amp;BF4,"")&amp;IF(BG4&lt;&gt;"","|"&amp;BG4,"")&amp;IF(BH4&lt;&gt;"","|"&amp;BH4,"")</f>
+      <c r="W4" s="3" t="str">
+        <f>IF(X4&lt;&gt;"",X4,"")&amp;IF(Y4&lt;&gt;"","|"&amp;Y4,"")&amp;IF(Z4&lt;&gt;"","|"&amp;Z4,"")&amp;IF(AA4&lt;&gt;"","|"&amp;AA4,"")&amp;IF(AB4&lt;&gt;"","|"&amp;AB4,"")&amp;IF(AC4&lt;&gt;"","|"&amp;AC4,"")&amp;IF(AD4&lt;&gt;"","|"&amp;AD4,"")&amp;IF(AE4&lt;&gt;"","|"&amp;AE4,"")&amp;IF(AF4&lt;&gt;"","|"&amp;AF4,"")&amp;IF(AG4&lt;&gt;"","|"&amp;AG4,"")&amp;IF(AH4&lt;&gt;"","|"&amp;AH4,"")&amp;IF(AI4&lt;&gt;"","|"&amp;AI4,"")&amp;IF(AJ4&lt;&gt;"","|"&amp;AJ4,"")&amp;IF(AK4&lt;&gt;"","|"&amp;AK4,"")&amp;IF(AL4&lt;&gt;"","|"&amp;AL4,"")&amp;IF(AM4&lt;&gt;"","|"&amp;AM4,"")&amp;IF(AN4&lt;&gt;"","|"&amp;AN4,"")&amp;IF(AO4&lt;&gt;"","|"&amp;AO4,"")&amp;IF(AP4&lt;&gt;"","|"&amp;AP4,"")&amp;IF(AQ4&lt;&gt;"","|"&amp;AQ4,"")&amp;IF(AR4&lt;&gt;"","|"&amp;AR4,"")&amp;IF(AS4&lt;&gt;"","|"&amp;AS4,"")&amp;IF(AT4&lt;&gt;"","|"&amp;AT4,"")&amp;IF(AU4&lt;&gt;"","|"&amp;AU4,"")&amp;IF(AV4&lt;&gt;"","|"&amp;AV4,"")&amp;IF(AW4&lt;&gt;"","|"&amp;AW4,"")&amp;IF(AX4&lt;&gt;"","|"&amp;AX4,"")&amp;IF(AY4&lt;&gt;"","|"&amp;AY4,"")&amp;IF(AZ4&lt;&gt;"","|"&amp;AZ4,"")&amp;IF(BA4&lt;&gt;"","|"&amp;BA4,"")&amp;IF(BB4&lt;&gt;"","|"&amp;BB4,"")&amp;IF(BC4&lt;&gt;"","|"&amp;BC4,"")&amp;IF(BD4&lt;&gt;"","|"&amp;BD4,"")&amp;IF(BE4&lt;&gt;"","|"&amp;BE4,"")&amp;IF(BF4&lt;&gt;"","|"&amp;BF4,"")&amp;IF(BG4&lt;&gt;"","|"&amp;BG4,"")&amp;IF(BH4&lt;&gt;"","|"&amp;BH4,"")&amp;IF(BI4&lt;&gt;"","|"&amp;BI4,"")</f>
         <v>|You must have the selected Acrobat's trick as part of the Rogue's Trick class feature.|Martial|You move up to your speed -2. During this move, you have a climb speed equal to your speed -2. You also gain a +2 power bonus to your next damage roll with a basic attack during this turn.
 Level 11: +4 power bonus.
 Level 21: +6 power bonus.</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="Z4" t="s">
         <v>2084</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AB4" t="s">
         <v>711</v>
       </c>
-      <c r="AH4" s="1" t="s">
+      <c r="AI4" s="1" t="s">
         <v>2087</v>
       </c>
-      <c r="AP4" s="3"/>
       <c r="AQ4" s="3"/>
       <c r="AR4" s="3"/>
       <c r="AS4" s="3"/>
       <c r="AT4" s="3"/>
       <c r="AU4" s="3"/>
-    </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AV4" s="3"/>
+    </row>
+    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2088</v>
       </c>
@@ -17010,581 +17021,584 @@
       <c r="R5" t="s">
         <v>2075</v>
       </c>
-      <c r="U5" s="3" t="str">
-        <f>IF(W5&lt;&gt;"",$W$1,"")&amp;IF(X5&lt;&gt;"","|"&amp;$X$1,"")&amp;IF(Y5&lt;&gt;"","|"&amp;$Y$1,"")&amp;IF(Z5&lt;&gt;"","|"&amp;$Z$1,"")&amp;IF(AA5&lt;&gt;"","|"&amp;$AA$1,"")&amp;IF(AB5&lt;&gt;"","|"&amp;$AB$1,"")&amp;IF(AC5&lt;&gt;"","|"&amp;$AC$1,"")&amp;IF(AD5&lt;&gt;"","|"&amp;$AD$1,"")&amp;IF(AE5&lt;&gt;"","|"&amp;$AE$1,"")&amp;IF(AF5&lt;&gt;"","|"&amp;$AF$1,"")&amp;IF(AG5&lt;&gt;"","|"&amp;$AG$1,"")&amp;IF(AH5&lt;&gt;"","|"&amp;$AH$1,"")&amp;IF(AI5&lt;&gt;"","|"&amp;$AI$1,"")&amp;IF(AJ5&lt;&gt;"","|"&amp;$AJ$1,"")&amp;IF(AK5&lt;&gt;"","|"&amp;$AK$1,"")&amp;IF(AL5&lt;&gt;"","|"&amp;$AL$1,"")&amp;IF(AM5&lt;&gt;"","|"&amp;$AM$1,"")&amp;IF(AN5&lt;&gt;"","|"&amp;$AN$1,"")&amp;IF(AO5&lt;&gt;"","|"&amp;$AO$1,"")&amp;IF(AP5&lt;&gt;"","|"&amp;$AP$1,"")&amp;IF(AQ5&lt;&gt;"","|"&amp;$AQ$1,"")&amp;IF(AR5&lt;&gt;"","|"&amp;$AR$1,"")&amp;IF(AS5&lt;&gt;"","|"&amp;$AS$1,"")&amp;IF(AT5&lt;&gt;"","|"&amp;$AT$1,"")&amp;IF(AU5&lt;&gt;"","|"&amp;$AU$1,"")&amp;IF(AV5&lt;&gt;"","|"&amp;$AV$1,"")&amp;IF(AW5&lt;&gt;"","|"&amp;$AW$1,"")&amp;IF(AX5&lt;&gt;"","|"&amp;$AX$1,"")&amp;IF(AY5&lt;&gt;"","|"&amp;$AY$1,"")&amp;IF(AZ5&lt;&gt;"","|"&amp;$AZ$1,"")&amp;IF(BA5&lt;&gt;"","|"&amp;$BA$1,"")&amp;IF(BB5&lt;&gt;"","|"&amp;$BB$1,"")&amp;IF(BC5&lt;&gt;"","|"&amp;$BC$1,"")&amp;IF(BD5&lt;&gt;"","|"&amp;$BD$1,"")&amp;IF(BE5&lt;&gt;"","|"&amp;$BE$1,"")&amp;IF(BF5&lt;&gt;"","|"&amp;$BF$1,"")&amp;IF(BG5&lt;&gt;"","|"&amp;$BG$1,"")&amp;IF(BH5&lt;&gt;"","|"&amp;$BH$1,"")</f>
+      <c r="V5" s="3" t="str">
+        <f>IF(X5&lt;&gt;"",$X$1,"")&amp;IF(Y5&lt;&gt;"","|"&amp;$Y$1,"")&amp;IF(Z5&lt;&gt;"","|"&amp;$Z$1,"")&amp;IF(AA5&lt;&gt;"","|"&amp;$AA$1,"")&amp;IF(AB5&lt;&gt;"","|"&amp;$AB$1,"")&amp;IF(AC5&lt;&gt;"","|"&amp;$AC$1,"")&amp;IF(AD5&lt;&gt;"","|"&amp;$AD$1,"")&amp;IF(AE5&lt;&gt;"","|"&amp;$AE$1,"")&amp;IF(AF5&lt;&gt;"","|"&amp;$AF$1,"")&amp;IF(AG5&lt;&gt;"","|"&amp;$AG$1,"")&amp;IF(AH5&lt;&gt;"","|"&amp;$AH$1,"")&amp;IF(AI5&lt;&gt;"","|"&amp;$AI$1,"")&amp;IF(AJ5&lt;&gt;"","|"&amp;$AJ$1,"")&amp;IF(AK5&lt;&gt;"","|"&amp;$AK$1,"")&amp;IF(AL5&lt;&gt;"","|"&amp;$AL$1,"")&amp;IF(AM5&lt;&gt;"","|"&amp;$AM$1,"")&amp;IF(AN5&lt;&gt;"","|"&amp;$AN$1,"")&amp;IF(AO5&lt;&gt;"","|"&amp;$AO$1,"")&amp;IF(AP5&lt;&gt;"","|"&amp;$AP$1,"")&amp;IF(AQ5&lt;&gt;"","|"&amp;$AQ$1,"")&amp;IF(AR5&lt;&gt;"","|"&amp;$AR$1,"")&amp;IF(AS5&lt;&gt;"","|"&amp;$AS$1,"")&amp;IF(AT5&lt;&gt;"","|"&amp;$AT$1,"")&amp;IF(AU5&lt;&gt;"","|"&amp;$AU$1,"")&amp;IF(AV5&lt;&gt;"","|"&amp;$AV$1,"")&amp;IF(AW5&lt;&gt;"","|"&amp;$AW$1,"")&amp;IF(AX5&lt;&gt;"","|"&amp;$AX$1,"")&amp;IF(AY5&lt;&gt;"","|"&amp;$AY$1,"")&amp;IF(AZ5&lt;&gt;"","|"&amp;$AZ$1,"")&amp;IF(BA5&lt;&gt;"","|"&amp;$BA$1,"")&amp;IF(BB5&lt;&gt;"","|"&amp;$BB$1,"")&amp;IF(BC5&lt;&gt;"","|"&amp;$BC$1,"")&amp;IF(BD5&lt;&gt;"","|"&amp;$BD$1,"")&amp;IF(BE5&lt;&gt;"","|"&amp;$BE$1,"")&amp;IF(BF5&lt;&gt;"","|"&amp;$BF$1,"")&amp;IF(BG5&lt;&gt;"","|"&amp;$BG$1,"")&amp;IF(BH5&lt;&gt;"","|"&amp;$BH$1,"")&amp;IF(BI5&lt;&gt;"","|"&amp;$BI$1,"")</f>
         <v>Flavor:|Prerequisite:|Requirement:|Keywords:|Attack:|Hit:|Effect:</v>
       </c>
-      <c r="V5" s="3" t="str">
-        <f>IF(W5&lt;&gt;"",W5,"")&amp;IF(X5&lt;&gt;"","|"&amp;X5,"")&amp;IF(Y5&lt;&gt;"","|"&amp;Y5,"")&amp;IF(Z5&lt;&gt;"","|"&amp;Z5,"")&amp;IF(AA5&lt;&gt;"","|"&amp;AA5,"")&amp;IF(AB5&lt;&gt;"","|"&amp;AB5,"")&amp;IF(AC5&lt;&gt;"","|"&amp;AC5,"")&amp;IF(AD5&lt;&gt;"","|"&amp;AD5,"")&amp;IF(AE5&lt;&gt;"","|"&amp;AE5,"")&amp;IF(AF5&lt;&gt;"","|"&amp;AF5,"")&amp;IF(AG5&lt;&gt;"","|"&amp;AG5,"")&amp;IF(AH5&lt;&gt;"","|"&amp;AH5,"")&amp;IF(AI5&lt;&gt;"","|"&amp;AI5,"")&amp;IF(AJ5&lt;&gt;"","|"&amp;AJ5,"")&amp;IF(AK5&lt;&gt;"","|"&amp;AK5,"")&amp;IF(AL5&lt;&gt;"","|"&amp;AL5,"")&amp;IF(AM5&lt;&gt;"","|"&amp;AM5,"")&amp;IF(AN5&lt;&gt;"","|"&amp;AN5,"")&amp;IF(AO5&lt;&gt;"","|"&amp;AO5,"")&amp;IF(AP5&lt;&gt;"","|"&amp;AP5,"")&amp;IF(AQ5&lt;&gt;"","|"&amp;AQ5,"")&amp;IF(AR5&lt;&gt;"","|"&amp;AR5,"")&amp;IF(AS5&lt;&gt;"","|"&amp;AS5,"")&amp;IF(AT5&lt;&gt;"","|"&amp;AT5,"")&amp;IF(AU5&lt;&gt;"","|"&amp;AU5,"")&amp;IF(AV5&lt;&gt;"","|"&amp;AV5,"")&amp;IF(AW5&lt;&gt;"","|"&amp;AW5,"")&amp;IF(AX5&lt;&gt;"","|"&amp;AX5,"")&amp;IF(AY5&lt;&gt;"","|"&amp;AY5,"")&amp;IF(AZ5&lt;&gt;"","|"&amp;AZ5,"")&amp;IF(BA5&lt;&gt;"","|"&amp;BA5,"")&amp;IF(BB5&lt;&gt;"","|"&amp;BB5,"")&amp;IF(BC5&lt;&gt;"","|"&amp;BC5,"")&amp;IF(BD5&lt;&gt;"","|"&amp;BD5,"")&amp;IF(BE5&lt;&gt;"","|"&amp;BE5,"")&amp;IF(BF5&lt;&gt;"","|"&amp;BF5,"")&amp;IF(BG5&lt;&gt;"","|"&amp;BG5,"")&amp;IF(BH5&lt;&gt;"","|"&amp;BH5,"")</f>
+      <c r="W5" s="3" t="str">
+        <f>IF(X5&lt;&gt;"",X5,"")&amp;IF(Y5&lt;&gt;"","|"&amp;Y5,"")&amp;IF(Z5&lt;&gt;"","|"&amp;Z5,"")&amp;IF(AA5&lt;&gt;"","|"&amp;AA5,"")&amp;IF(AB5&lt;&gt;"","|"&amp;AB5,"")&amp;IF(AC5&lt;&gt;"","|"&amp;AC5,"")&amp;IF(AD5&lt;&gt;"","|"&amp;AD5,"")&amp;IF(AE5&lt;&gt;"","|"&amp;AE5,"")&amp;IF(AF5&lt;&gt;"","|"&amp;AF5,"")&amp;IF(AG5&lt;&gt;"","|"&amp;AG5,"")&amp;IF(AH5&lt;&gt;"","|"&amp;AH5,"")&amp;IF(AI5&lt;&gt;"","|"&amp;AI5,"")&amp;IF(AJ5&lt;&gt;"","|"&amp;AJ5,"")&amp;IF(AK5&lt;&gt;"","|"&amp;AK5,"")&amp;IF(AL5&lt;&gt;"","|"&amp;AL5,"")&amp;IF(AM5&lt;&gt;"","|"&amp;AM5,"")&amp;IF(AN5&lt;&gt;"","|"&amp;AN5,"")&amp;IF(AO5&lt;&gt;"","|"&amp;AO5,"")&amp;IF(AP5&lt;&gt;"","|"&amp;AP5,"")&amp;IF(AQ5&lt;&gt;"","|"&amp;AQ5,"")&amp;IF(AR5&lt;&gt;"","|"&amp;AR5,"")&amp;IF(AS5&lt;&gt;"","|"&amp;AS5,"")&amp;IF(AT5&lt;&gt;"","|"&amp;AT5,"")&amp;IF(AU5&lt;&gt;"","|"&amp;AU5,"")&amp;IF(AV5&lt;&gt;"","|"&amp;AV5,"")&amp;IF(AW5&lt;&gt;"","|"&amp;AW5,"")&amp;IF(AX5&lt;&gt;"","|"&amp;AX5,"")&amp;IF(AY5&lt;&gt;"","|"&amp;AY5,"")&amp;IF(AZ5&lt;&gt;"","|"&amp;AZ5,"")&amp;IF(BA5&lt;&gt;"","|"&amp;BA5,"")&amp;IF(BB5&lt;&gt;"","|"&amp;BB5,"")&amp;IF(BC5&lt;&gt;"","|"&amp;BC5,"")&amp;IF(BD5&lt;&gt;"","|"&amp;BD5,"")&amp;IF(BE5&lt;&gt;"","|"&amp;BE5,"")&amp;IF(BF5&lt;&gt;"","|"&amp;BF5,"")&amp;IF(BG5&lt;&gt;"","|"&amp;BG5,"")&amp;IF(BH5&lt;&gt;"","|"&amp;BH5,"")&amp;IF(BI5&lt;&gt;"","|"&amp;BI5,"")</f>
         <v>You strike at your horrid enemy, using your knowledge of its strengths and weaknesses to twist the knife just a bit more.|You must be trained in Acrobatics|You must be wielding a light blade in order to use.|Martial, Weapon|Dexterity vs AC|1[W] + Dexterity modifier (~DEXMod~) damage. If the target is aberrant and has resistance or vulnerability to your attack, you gain a bonus to damage equal to your Wisdom modifier (~WISMod~).
 Level 21: 2[W] + Dexterity modifier (~DEXMod~) damage.|Before or after the attack, you shift 1 square.</v>
       </c>
-      <c r="W5" t="s">
+      <c r="X5" t="s">
         <v>2071</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="Z5" t="s">
         <v>2094</v>
       </c>
-      <c r="Z5" s="3" t="s">
+      <c r="AA5" s="3" t="s">
         <v>2096</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AB5" t="s">
         <v>2129</v>
       </c>
-      <c r="AC5" s="3" t="s">
+      <c r="AD5" s="3" t="s">
         <v>2103</v>
       </c>
-      <c r="AD5" s="1" t="s">
+      <c r="AE5" s="1" t="s">
         <v>2132</v>
       </c>
-      <c r="AE5" s="1"/>
       <c r="AF5" s="1"/>
       <c r="AG5" s="1"/>
-      <c r="AH5" s="1" t="s">
+      <c r="AH5" s="1"/>
+      <c r="AI5" s="1" t="s">
         <v>2097</v>
       </c>
-      <c r="AP5" s="3"/>
       <c r="AQ5" s="3"/>
       <c r="AR5" s="3"/>
       <c r="AS5" s="3"/>
       <c r="AT5" s="3"/>
       <c r="AU5" s="3"/>
-    </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="AP6" s="3"/>
+      <c r="AV5" s="3"/>
+    </row>
+    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2140</v>
+      </c>
       <c r="AQ6" s="3"/>
       <c r="AR6" s="3"/>
       <c r="AS6" s="3"/>
       <c r="AT6" s="3"/>
       <c r="AU6" s="3"/>
-    </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="AP7" s="3"/>
+      <c r="AV6" s="3"/>
+    </row>
+    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
       <c r="AQ7" s="3"/>
       <c r="AR7" s="3"/>
       <c r="AS7" s="3"/>
       <c r="AT7" s="3"/>
       <c r="AU7" s="3"/>
-    </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AV7" s="3"/>
+    </row>
+    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
       <c r="O9" s="3"/>
-      <c r="X9"/>
-      <c r="Y9" s="3"/>
-      <c r="Z9"/>
-      <c r="AA9" s="3"/>
-      <c r="AC9"/>
-      <c r="AD9" s="3"/>
-      <c r="AG9"/>
-      <c r="AI9" s="3"/>
-      <c r="AO9"/>
-    </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="Y9"/>
+      <c r="Z9" s="3"/>
+      <c r="AA9"/>
+      <c r="AB9" s="3"/>
+      <c r="AD9"/>
+      <c r="AE9" s="3"/>
+      <c r="AH9"/>
+      <c r="AJ9" s="3"/>
+      <c r="AP9"/>
+    </row>
+    <row r="10" spans="1:48" x14ac:dyDescent="0.25">
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
       <c r="Q10"/>
       <c r="R10"/>
-      <c r="W10" s="3"/>
-      <c r="Y10" s="3"/>
-      <c r="AD10" s="3"/>
-      <c r="AE10"/>
-      <c r="AI10" s="3"/>
-      <c r="AL10"/>
+      <c r="X10" s="3"/>
+      <c r="Z10" s="3"/>
+      <c r="AE10" s="3"/>
+      <c r="AF10"/>
+      <c r="AJ10" s="3"/>
       <c r="AM10"/>
-      <c r="AP10" s="3"/>
+      <c r="AN10"/>
       <c r="AQ10" s="3"/>
       <c r="AR10" s="3"/>
       <c r="AS10" s="3"/>
-    </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AT10" s="3"/>
+    </row>
+    <row r="11" spans="1:48" x14ac:dyDescent="0.25">
       <c r="O11" s="3"/>
       <c r="Q11"/>
       <c r="R11"/>
-      <c r="W11" s="3"/>
-      <c r="Y11" s="3"/>
-      <c r="AD11" s="3"/>
-      <c r="AE11"/>
-      <c r="AI11" s="3"/>
-      <c r="AL11"/>
+      <c r="X11" s="3"/>
+      <c r="Z11" s="3"/>
+      <c r="AE11" s="3"/>
+      <c r="AF11"/>
+      <c r="AJ11" s="3"/>
       <c r="AM11"/>
-      <c r="AP11" s="3"/>
+      <c r="AN11"/>
       <c r="AQ11" s="3"/>
       <c r="AR11" s="3"/>
       <c r="AS11" s="3"/>
-    </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AT11" s="3"/>
+    </row>
+    <row r="12" spans="1:48" x14ac:dyDescent="0.25">
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
       <c r="R12"/>
-      <c r="W12" s="3"/>
-      <c r="Y12" s="3"/>
-      <c r="AD12" s="3"/>
-      <c r="AE12"/>
-      <c r="AI12" s="3"/>
-      <c r="AL12"/>
+      <c r="X12" s="3"/>
+      <c r="Z12" s="3"/>
+      <c r="AE12" s="3"/>
+      <c r="AF12"/>
+      <c r="AJ12" s="3"/>
       <c r="AM12"/>
-      <c r="AP12" s="3"/>
+      <c r="AN12"/>
       <c r="AQ12" s="3"/>
       <c r="AR12" s="3"/>
       <c r="AS12" s="3"/>
-    </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AT12" s="3"/>
+    </row>
+    <row r="13" spans="1:48" x14ac:dyDescent="0.25">
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
       <c r="R13"/>
-      <c r="W13" s="3"/>
-      <c r="Y13" s="3"/>
-      <c r="AD13" s="3"/>
-      <c r="AE13"/>
-      <c r="AI13" s="3"/>
-      <c r="AL13"/>
+      <c r="X13" s="3"/>
+      <c r="Z13" s="3"/>
+      <c r="AE13" s="3"/>
+      <c r="AF13"/>
+      <c r="AJ13" s="3"/>
       <c r="AM13"/>
-      <c r="AP13" s="3"/>
+      <c r="AN13"/>
       <c r="AQ13" s="3"/>
       <c r="AR13" s="3"/>
       <c r="AS13" s="3"/>
-    </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AT13" s="3"/>
+    </row>
+    <row r="14" spans="1:48" x14ac:dyDescent="0.25">
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
       <c r="R14"/>
-      <c r="W14" s="3"/>
-      <c r="Y14" s="3"/>
-      <c r="AD14" s="3"/>
-      <c r="AE14"/>
-      <c r="AI14" s="3"/>
-      <c r="AL14"/>
+      <c r="X14" s="3"/>
+      <c r="Z14" s="3"/>
+      <c r="AE14" s="3"/>
+      <c r="AF14"/>
+      <c r="AJ14" s="3"/>
       <c r="AM14"/>
-      <c r="AP14" s="3"/>
+      <c r="AN14"/>
       <c r="AQ14" s="3"/>
       <c r="AR14" s="3"/>
       <c r="AS14" s="3"/>
-    </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AT14" s="3"/>
+    </row>
+    <row r="15" spans="1:48" x14ac:dyDescent="0.25">
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
       <c r="R15"/>
-      <c r="W15" s="3"/>
-      <c r="Y15" s="3"/>
-      <c r="AD15" s="3"/>
-      <c r="AE15"/>
-      <c r="AI15" s="3"/>
-      <c r="AL15"/>
+      <c r="X15" s="3"/>
+      <c r="Z15" s="3"/>
+      <c r="AE15" s="3"/>
+      <c r="AF15"/>
+      <c r="AJ15" s="3"/>
       <c r="AM15"/>
-      <c r="AP15" s="3"/>
+      <c r="AN15"/>
       <c r="AQ15" s="3"/>
       <c r="AR15" s="3"/>
       <c r="AS15" s="3"/>
-    </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AT15" s="3"/>
+    </row>
+    <row r="16" spans="1:48" x14ac:dyDescent="0.25">
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
       <c r="R16"/>
-      <c r="W16" s="3"/>
-      <c r="Y16" s="3"/>
-      <c r="AD16" s="3"/>
-      <c r="AE16"/>
-      <c r="AI16" s="3"/>
-      <c r="AL16"/>
+      <c r="X16" s="3"/>
+      <c r="Z16" s="3"/>
+      <c r="AE16" s="3"/>
+      <c r="AF16"/>
+      <c r="AJ16" s="3"/>
       <c r="AM16"/>
-      <c r="AP16" s="3"/>
+      <c r="AN16"/>
       <c r="AQ16" s="3"/>
       <c r="AR16" s="3"/>
       <c r="AS16" s="3"/>
-    </row>
-    <row r="17" spans="14:45" x14ac:dyDescent="0.25">
+      <c r="AT16" s="3"/>
+    </row>
+    <row r="17" spans="14:46" x14ac:dyDescent="0.25">
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
       <c r="P17" s="3"/>
       <c r="R17"/>
-      <c r="W17" s="3"/>
-      <c r="Y17" s="3"/>
-      <c r="AD17" s="3"/>
-      <c r="AE17"/>
-      <c r="AI17" s="3"/>
-      <c r="AL17"/>
+      <c r="X17" s="3"/>
+      <c r="Z17" s="3"/>
+      <c r="AE17" s="3"/>
+      <c r="AF17"/>
+      <c r="AJ17" s="3"/>
       <c r="AM17"/>
-      <c r="AP17" s="3"/>
+      <c r="AN17"/>
       <c r="AQ17" s="3"/>
       <c r="AR17" s="3"/>
       <c r="AS17" s="3"/>
-    </row>
-    <row r="18" spans="14:45" x14ac:dyDescent="0.25">
+      <c r="AT17" s="3"/>
+    </row>
+    <row r="18" spans="14:46" x14ac:dyDescent="0.25">
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
       <c r="P18" s="3"/>
       <c r="R18"/>
-      <c r="W18" s="3"/>
-      <c r="Y18" s="3"/>
-      <c r="AD18" s="3"/>
-      <c r="AE18"/>
-      <c r="AI18" s="3"/>
-      <c r="AL18"/>
+      <c r="X18" s="3"/>
+      <c r="Z18" s="3"/>
+      <c r="AE18" s="3"/>
+      <c r="AF18"/>
+      <c r="AJ18" s="3"/>
       <c r="AM18"/>
-      <c r="AP18" s="3"/>
+      <c r="AN18"/>
       <c r="AQ18" s="3"/>
       <c r="AR18" s="3"/>
       <c r="AS18" s="3"/>
-    </row>
-    <row r="19" spans="14:45" x14ac:dyDescent="0.25">
+      <c r="AT18" s="3"/>
+    </row>
+    <row r="19" spans="14:46" x14ac:dyDescent="0.25">
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
       <c r="P19" s="3"/>
       <c r="R19"/>
-      <c r="W19" s="3"/>
-      <c r="Y19" s="3"/>
-      <c r="AD19" s="3"/>
-      <c r="AE19"/>
-      <c r="AI19" s="3"/>
-      <c r="AL19"/>
+      <c r="X19" s="3"/>
+      <c r="Z19" s="3"/>
+      <c r="AE19" s="3"/>
+      <c r="AF19"/>
+      <c r="AJ19" s="3"/>
       <c r="AM19"/>
-      <c r="AP19" s="3"/>
+      <c r="AN19"/>
       <c r="AQ19" s="3"/>
       <c r="AR19" s="3"/>
       <c r="AS19" s="3"/>
-    </row>
-    <row r="20" spans="14:45" x14ac:dyDescent="0.25">
+      <c r="AT19" s="3"/>
+    </row>
+    <row r="20" spans="14:46" x14ac:dyDescent="0.25">
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
       <c r="P20" s="3"/>
       <c r="R20"/>
-      <c r="W20" s="3"/>
-      <c r="Y20" s="3"/>
-      <c r="AD20" s="3"/>
-      <c r="AE20"/>
-      <c r="AI20" s="3"/>
-      <c r="AL20"/>
+      <c r="X20" s="3"/>
+      <c r="Z20" s="3"/>
+      <c r="AE20" s="3"/>
+      <c r="AF20"/>
+      <c r="AJ20" s="3"/>
       <c r="AM20"/>
-      <c r="AP20" s="3"/>
+      <c r="AN20"/>
       <c r="AQ20" s="3"/>
       <c r="AR20" s="3"/>
       <c r="AS20" s="3"/>
-    </row>
-    <row r="21" spans="14:45" x14ac:dyDescent="0.25">
+      <c r="AT20" s="3"/>
+    </row>
+    <row r="21" spans="14:46" x14ac:dyDescent="0.25">
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
       <c r="P21" s="3"/>
       <c r="R21"/>
-      <c r="W21" s="3"/>
-      <c r="Y21" s="3"/>
-      <c r="AD21" s="3"/>
-      <c r="AE21"/>
-      <c r="AI21" s="3"/>
-      <c r="AL21"/>
+      <c r="X21" s="3"/>
+      <c r="Z21" s="3"/>
+      <c r="AE21" s="3"/>
+      <c r="AF21"/>
+      <c r="AJ21" s="3"/>
       <c r="AM21"/>
-      <c r="AP21" s="3"/>
+      <c r="AN21"/>
       <c r="AQ21" s="3"/>
       <c r="AR21" s="3"/>
       <c r="AS21" s="3"/>
-    </row>
-    <row r="22" spans="14:45" x14ac:dyDescent="0.25">
+      <c r="AT21" s="3"/>
+    </row>
+    <row r="22" spans="14:46" x14ac:dyDescent="0.25">
       <c r="N22" s="3"/>
       <c r="O22" s="3"/>
       <c r="P22" s="3"/>
       <c r="R22"/>
-      <c r="W22" s="3"/>
-      <c r="Y22" s="3"/>
-      <c r="AD22" s="3"/>
-      <c r="AE22"/>
-      <c r="AI22" s="3"/>
-      <c r="AL22"/>
+      <c r="X22" s="3"/>
+      <c r="Z22" s="3"/>
+      <c r="AE22" s="3"/>
+      <c r="AF22"/>
+      <c r="AJ22" s="3"/>
       <c r="AM22"/>
-      <c r="AP22" s="3"/>
+      <c r="AN22"/>
       <c r="AQ22" s="3"/>
       <c r="AR22" s="3"/>
       <c r="AS22" s="3"/>
-    </row>
-    <row r="23" spans="14:45" x14ac:dyDescent="0.25">
+      <c r="AT22" s="3"/>
+    </row>
+    <row r="23" spans="14:46" x14ac:dyDescent="0.25">
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
       <c r="P23" s="3"/>
       <c r="R23"/>
-      <c r="W23" s="3"/>
-      <c r="Y23" s="3"/>
-      <c r="AD23" s="3"/>
-      <c r="AE23"/>
-      <c r="AI23" s="3"/>
-      <c r="AL23"/>
+      <c r="X23" s="3"/>
+      <c r="Z23" s="3"/>
+      <c r="AE23" s="3"/>
+      <c r="AF23"/>
+      <c r="AJ23" s="3"/>
       <c r="AM23"/>
-      <c r="AP23" s="3"/>
+      <c r="AN23"/>
       <c r="AQ23" s="3"/>
       <c r="AR23" s="3"/>
       <c r="AS23" s="3"/>
-    </row>
-    <row r="24" spans="14:45" x14ac:dyDescent="0.25">
+      <c r="AT23" s="3"/>
+    </row>
+    <row r="24" spans="14:46" x14ac:dyDescent="0.25">
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
       <c r="P24" s="3"/>
       <c r="R24"/>
-      <c r="W24" s="3"/>
-      <c r="Y24" s="3"/>
-      <c r="AD24" s="3"/>
-      <c r="AE24"/>
-      <c r="AI24" s="3"/>
-      <c r="AL24"/>
+      <c r="X24" s="3"/>
+      <c r="Z24" s="3"/>
+      <c r="AE24" s="3"/>
+      <c r="AF24"/>
+      <c r="AJ24" s="3"/>
       <c r="AM24"/>
-      <c r="AP24" s="3"/>
+      <c r="AN24"/>
       <c r="AQ24" s="3"/>
       <c r="AR24" s="3"/>
       <c r="AS24" s="3"/>
-    </row>
-    <row r="25" spans="14:45" x14ac:dyDescent="0.25">
+      <c r="AT24" s="3"/>
+    </row>
+    <row r="25" spans="14:46" x14ac:dyDescent="0.25">
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
       <c r="P25" s="3"/>
       <c r="R25"/>
-      <c r="W25" s="3"/>
-      <c r="Y25" s="3"/>
-      <c r="AD25" s="3"/>
-      <c r="AE25"/>
-      <c r="AI25" s="3"/>
-      <c r="AL25"/>
+      <c r="X25" s="3"/>
+      <c r="Z25" s="3"/>
+      <c r="AE25" s="3"/>
+      <c r="AF25"/>
+      <c r="AJ25" s="3"/>
       <c r="AM25"/>
-      <c r="AP25" s="3"/>
+      <c r="AN25"/>
       <c r="AQ25" s="3"/>
       <c r="AR25" s="3"/>
       <c r="AS25" s="3"/>
-    </row>
-    <row r="26" spans="14:45" x14ac:dyDescent="0.25">
+      <c r="AT25" s="3"/>
+    </row>
+    <row r="26" spans="14:46" x14ac:dyDescent="0.25">
       <c r="N26" s="3"/>
       <c r="O26" s="3"/>
       <c r="P26" s="3"/>
       <c r="R26"/>
-      <c r="W26" s="3"/>
-      <c r="Y26" s="3"/>
-      <c r="AD26" s="3"/>
-      <c r="AE26"/>
-      <c r="AI26" s="3"/>
-      <c r="AL26"/>
+      <c r="X26" s="3"/>
+      <c r="Z26" s="3"/>
+      <c r="AE26" s="3"/>
+      <c r="AF26"/>
+      <c r="AJ26" s="3"/>
       <c r="AM26"/>
-      <c r="AP26" s="3"/>
+      <c r="AN26"/>
       <c r="AQ26" s="3"/>
       <c r="AR26" s="3"/>
       <c r="AS26" s="3"/>
-    </row>
-    <row r="27" spans="14:45" x14ac:dyDescent="0.25">
+      <c r="AT26" s="3"/>
+    </row>
+    <row r="27" spans="14:46" x14ac:dyDescent="0.25">
       <c r="N27" s="3"/>
       <c r="O27" s="3"/>
       <c r="P27" s="3"/>
       <c r="R27"/>
-      <c r="W27" s="3"/>
-      <c r="Y27" s="3"/>
-      <c r="AD27" s="3"/>
-      <c r="AE27"/>
-      <c r="AI27" s="3"/>
-      <c r="AL27"/>
+      <c r="X27" s="3"/>
+      <c r="Z27" s="3"/>
+      <c r="AE27" s="3"/>
+      <c r="AF27"/>
+      <c r="AJ27" s="3"/>
       <c r="AM27"/>
-      <c r="AP27" s="3"/>
+      <c r="AN27"/>
       <c r="AQ27" s="3"/>
       <c r="AR27" s="3"/>
       <c r="AS27" s="3"/>
-    </row>
-    <row r="28" spans="14:45" x14ac:dyDescent="0.25">
+      <c r="AT27" s="3"/>
+    </row>
+    <row r="28" spans="14:46" x14ac:dyDescent="0.25">
       <c r="N28" s="3"/>
       <c r="O28" s="3"/>
       <c r="P28" s="3"/>
       <c r="R28"/>
-      <c r="W28" s="3"/>
-      <c r="Y28" s="3"/>
-      <c r="AD28" s="3"/>
-      <c r="AE28"/>
-      <c r="AI28" s="3"/>
-      <c r="AL28"/>
+      <c r="X28" s="3"/>
+      <c r="Z28" s="3"/>
+      <c r="AE28" s="3"/>
+      <c r="AF28"/>
+      <c r="AJ28" s="3"/>
       <c r="AM28"/>
-      <c r="AP28" s="3"/>
+      <c r="AN28"/>
       <c r="AQ28" s="3"/>
       <c r="AR28" s="3"/>
       <c r="AS28" s="3"/>
-    </row>
-    <row r="29" spans="14:45" x14ac:dyDescent="0.25">
+      <c r="AT28" s="3"/>
+    </row>
+    <row r="29" spans="14:46" x14ac:dyDescent="0.25">
       <c r="N29" s="3"/>
       <c r="O29" s="3"/>
       <c r="P29" s="3"/>
       <c r="R29"/>
-      <c r="W29" s="3"/>
-      <c r="Y29" s="3"/>
-      <c r="AD29" s="3"/>
-      <c r="AE29"/>
-      <c r="AI29" s="3"/>
-      <c r="AL29"/>
+      <c r="X29" s="3"/>
+      <c r="Z29" s="3"/>
+      <c r="AE29" s="3"/>
+      <c r="AF29"/>
+      <c r="AJ29" s="3"/>
       <c r="AM29"/>
-      <c r="AP29" s="3"/>
+      <c r="AN29"/>
       <c r="AQ29" s="3"/>
       <c r="AR29" s="3"/>
       <c r="AS29" s="3"/>
-    </row>
-    <row r="30" spans="14:45" x14ac:dyDescent="0.25">
+      <c r="AT29" s="3"/>
+    </row>
+    <row r="30" spans="14:46" x14ac:dyDescent="0.25">
       <c r="N30" s="3"/>
       <c r="O30" s="3"/>
       <c r="P30" s="3"/>
       <c r="R30"/>
-      <c r="W30" s="3"/>
-      <c r="Y30" s="3"/>
-      <c r="AD30" s="3"/>
-      <c r="AE30"/>
-      <c r="AI30" s="3"/>
-      <c r="AL30"/>
+      <c r="X30" s="3"/>
+      <c r="Z30" s="3"/>
+      <c r="AE30" s="3"/>
+      <c r="AF30"/>
+      <c r="AJ30" s="3"/>
       <c r="AM30"/>
-      <c r="AP30" s="3"/>
+      <c r="AN30"/>
       <c r="AQ30" s="3"/>
       <c r="AR30" s="3"/>
       <c r="AS30" s="3"/>
-    </row>
-    <row r="31" spans="14:45" x14ac:dyDescent="0.25">
+      <c r="AT30" s="3"/>
+    </row>
+    <row r="31" spans="14:46" x14ac:dyDescent="0.25">
       <c r="N31" s="3"/>
       <c r="O31" s="3"/>
       <c r="P31" s="3"/>
       <c r="R31"/>
-      <c r="W31" s="3"/>
-      <c r="Y31" s="3"/>
-      <c r="AD31" s="3"/>
-      <c r="AE31"/>
-      <c r="AI31" s="3"/>
-      <c r="AL31"/>
+      <c r="X31" s="3"/>
+      <c r="Z31" s="3"/>
+      <c r="AE31" s="3"/>
+      <c r="AF31"/>
+      <c r="AJ31" s="3"/>
       <c r="AM31"/>
-      <c r="AP31" s="3"/>
+      <c r="AN31"/>
       <c r="AQ31" s="3"/>
       <c r="AR31" s="3"/>
       <c r="AS31" s="3"/>
-    </row>
-    <row r="32" spans="14:45" x14ac:dyDescent="0.25">
+      <c r="AT31" s="3"/>
+    </row>
+    <row r="32" spans="14:46" x14ac:dyDescent="0.25">
       <c r="N32" s="3"/>
       <c r="O32" s="3"/>
       <c r="P32" s="3"/>
       <c r="R32"/>
-      <c r="W32" s="3"/>
-      <c r="Y32" s="3"/>
-      <c r="AD32" s="3"/>
-      <c r="AE32"/>
-      <c r="AI32" s="3"/>
-      <c r="AL32"/>
+      <c r="X32" s="3"/>
+      <c r="Z32" s="3"/>
+      <c r="AE32" s="3"/>
+      <c r="AF32"/>
+      <c r="AJ32" s="3"/>
       <c r="AM32"/>
-      <c r="AP32" s="3"/>
+      <c r="AN32"/>
       <c r="AQ32" s="3"/>
       <c r="AR32" s="3"/>
       <c r="AS32" s="3"/>
-    </row>
-    <row r="33" spans="15:45" x14ac:dyDescent="0.25">
+      <c r="AT32" s="3"/>
+    </row>
+    <row r="33" spans="15:46" x14ac:dyDescent="0.25">
       <c r="O33" s="3"/>
       <c r="P33" s="3"/>
       <c r="R33"/>
-      <c r="W33" s="3"/>
-      <c r="Y33" s="3"/>
-      <c r="AD33" s="3"/>
-      <c r="AE33"/>
-      <c r="AI33" s="3"/>
-      <c r="AL33"/>
+      <c r="X33" s="3"/>
+      <c r="Z33" s="3"/>
+      <c r="AE33" s="3"/>
+      <c r="AF33"/>
+      <c r="AJ33" s="3"/>
       <c r="AM33"/>
-      <c r="AP33" s="3"/>
+      <c r="AN33"/>
       <c r="AQ33" s="3"/>
       <c r="AR33" s="3"/>
       <c r="AS33" s="3"/>
-    </row>
-    <row r="34" spans="15:45" x14ac:dyDescent="0.25">
+      <c r="AT33" s="3"/>
+    </row>
+    <row r="34" spans="15:46" x14ac:dyDescent="0.25">
       <c r="O34" s="3"/>
       <c r="P34" s="3"/>
-      <c r="W34" s="3"/>
-      <c r="Y34" s="3"/>
-    </row>
-    <row r="35" spans="15:45" x14ac:dyDescent="0.25">
+      <c r="X34" s="3"/>
+      <c r="Z34" s="3"/>
+    </row>
+    <row r="35" spans="15:46" x14ac:dyDescent="0.25">
       <c r="O35" s="3"/>
       <c r="P35" s="3"/>
-      <c r="W35" s="3"/>
-      <c r="Y35" s="3"/>
-    </row>
-    <row r="36" spans="15:45" x14ac:dyDescent="0.25">
+      <c r="X35" s="3"/>
+      <c r="Z35" s="3"/>
+    </row>
+    <row r="36" spans="15:46" x14ac:dyDescent="0.25">
       <c r="O36" s="3"/>
       <c r="P36" s="3"/>
-      <c r="W36" s="3"/>
-      <c r="Y36" s="3"/>
-    </row>
-    <row r="37" spans="15:45" x14ac:dyDescent="0.25">
+      <c r="X36" s="3"/>
+      <c r="Z36" s="3"/>
+    </row>
+    <row r="37" spans="15:46" x14ac:dyDescent="0.25">
       <c r="O37" s="3"/>
       <c r="P37" s="3"/>
-      <c r="W37" s="3"/>
-      <c r="Y37" s="3"/>
-    </row>
-    <row r="38" spans="15:45" x14ac:dyDescent="0.25">
+      <c r="X37" s="3"/>
+      <c r="Z37" s="3"/>
+    </row>
+    <row r="38" spans="15:46" x14ac:dyDescent="0.25">
       <c r="O38" s="3"/>
       <c r="P38" s="3"/>
-      <c r="W38" s="3"/>
-      <c r="Y38" s="3"/>
-    </row>
-    <row r="39" spans="15:45" x14ac:dyDescent="0.25">
+      <c r="X38" s="3"/>
+      <c r="Z38" s="3"/>
+    </row>
+    <row r="39" spans="15:46" x14ac:dyDescent="0.25">
       <c r="O39" s="3"/>
       <c r="P39" s="3"/>
-      <c r="W39" s="3"/>
-      <c r="Y39" s="3"/>
-    </row>
-    <row r="40" spans="15:45" x14ac:dyDescent="0.25">
+      <c r="X39" s="3"/>
+      <c r="Z39" s="3"/>
+    </row>
+    <row r="40" spans="15:46" x14ac:dyDescent="0.25">
       <c r="O40" s="3"/>
       <c r="P40" s="3"/>
-      <c r="W40" s="3"/>
-      <c r="Y40" s="3"/>
-    </row>
-    <row r="41" spans="15:45" x14ac:dyDescent="0.25">
+      <c r="X40" s="3"/>
+      <c r="Z40" s="3"/>
+    </row>
+    <row r="41" spans="15:46" x14ac:dyDescent="0.25">
       <c r="O41" s="3"/>
       <c r="P41" s="3"/>
-      <c r="W41" s="3"/>
-      <c r="Y41" s="3"/>
-    </row>
-    <row r="42" spans="15:45" x14ac:dyDescent="0.25">
+      <c r="X41" s="3"/>
+      <c r="Z41" s="3"/>
+    </row>
+    <row r="42" spans="15:46" x14ac:dyDescent="0.25">
       <c r="O42" s="3"/>
       <c r="P42" s="3"/>
-      <c r="W42" s="3"/>
-      <c r="Y42" s="3"/>
-    </row>
-    <row r="43" spans="15:45" x14ac:dyDescent="0.25">
+      <c r="X42" s="3"/>
+      <c r="Z42" s="3"/>
+    </row>
+    <row r="43" spans="15:46" x14ac:dyDescent="0.25">
       <c r="O43" s="3"/>
       <c r="P43" s="3"/>
-      <c r="W43" s="3"/>
-      <c r="Y43" s="3"/>
-    </row>
-    <row r="44" spans="15:45" x14ac:dyDescent="0.25">
+      <c r="X43" s="3"/>
+      <c r="Z43" s="3"/>
+    </row>
+    <row r="44" spans="15:46" x14ac:dyDescent="0.25">
       <c r="O44" s="3"/>
       <c r="P44" s="3"/>
-      <c r="W44" s="3"/>
-      <c r="Y44" s="3"/>
-    </row>
-    <row r="45" spans="15:45" x14ac:dyDescent="0.25">
+      <c r="X44" s="3"/>
+      <c r="Z44" s="3"/>
+    </row>
+    <row r="45" spans="15:46" x14ac:dyDescent="0.25">
       <c r="O45" s="3"/>
       <c r="P45" s="3"/>
-      <c r="W45" s="3"/>
-      <c r="Y45" s="3"/>
-    </row>
-    <row r="46" spans="15:45" x14ac:dyDescent="0.25">
+      <c r="X45" s="3"/>
+      <c r="Z45" s="3"/>
+    </row>
+    <row r="46" spans="15:46" x14ac:dyDescent="0.25">
       <c r="O46" s="3"/>
       <c r="P46" s="3"/>
-      <c r="W46" s="3"/>
-      <c r="Y46" s="3"/>
-    </row>
-    <row r="47" spans="15:45" x14ac:dyDescent="0.25">
+      <c r="X46" s="3"/>
+      <c r="Z46" s="3"/>
+    </row>
+    <row r="47" spans="15:46" x14ac:dyDescent="0.25">
       <c r="O47" s="3"/>
       <c r="P47" s="3"/>
-      <c r="W47" s="3"/>
-      <c r="Y47" s="3"/>
-    </row>
-    <row r="48" spans="15:45" x14ac:dyDescent="0.25">
+      <c r="X47" s="3"/>
+      <c r="Z47" s="3"/>
+    </row>
+    <row r="48" spans="15:46" x14ac:dyDescent="0.25">
       <c r="O48" s="3"/>
       <c r="P48" s="3"/>
-      <c r="W48" s="3"/>
-      <c r="Y48" s="3"/>
-    </row>
-    <row r="49" spans="15:25" x14ac:dyDescent="0.25">
+      <c r="X48" s="3"/>
+      <c r="Z48" s="3"/>
+    </row>
+    <row r="49" spans="15:26" x14ac:dyDescent="0.25">
       <c r="O49" s="3"/>
       <c r="P49" s="3"/>
-      <c r="W49" s="3"/>
-      <c r="Y49" s="3"/>
-    </row>
-    <row r="50" spans="15:25" x14ac:dyDescent="0.25">
+      <c r="X49" s="3"/>
+      <c r="Z49" s="3"/>
+    </row>
+    <row r="50" spans="15:26" x14ac:dyDescent="0.25">
       <c r="O50" s="3"/>
       <c r="P50" s="3"/>
-      <c r="W50" s="3"/>
-      <c r="Y50" s="3"/>
+      <c r="X50" s="3"/>
+      <c r="Z50" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17615,10 +17629,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17626,7 +17640,7 @@
     <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1105</v>
       </c>
@@ -17637,12 +17651,12 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>678</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1108</v>
       </c>
@@ -17650,7 +17664,7 @@
         <v>1112</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>848</v>
       </c>
@@ -17661,7 +17675,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>679</v>
       </c>
@@ -17672,7 +17686,7 @@
         <v>1119</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1107</v>
       </c>
@@ -17683,7 +17697,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1080</v>
       </c>
@@ -17693,8 +17707,9 @@
       <c r="C7" t="s">
         <v>1465</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="L7" s="19"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1106</v>
       </c>
@@ -17705,7 +17720,7 @@
         <v>1122</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>680</v>
       </c>
@@ -17716,7 +17731,7 @@
         <v>1468</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>837</v>
       </c>
@@ -17727,12 +17742,12 @@
         <v>1572</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>835</v>
       </c>
@@ -17743,7 +17758,7 @@
         <v>1606</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>756</v>
       </c>
@@ -17754,30 +17769,33 @@
         <v>1604</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>682</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>683</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>684</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>685</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>686</v>
       </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K23" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18089,7 +18107,7 @@
   <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18758,10 +18776,10 @@
   <dimension ref="A1:BH49"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AK31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomRight" activeCell="AZ60" sqref="AY60:AZ60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Finished current data to DB, now gathering all powers.
</commit_message>
<xml_diff>
--- a/DND4eCharacterGenerator/Assets/ScrapeData.xlsx
+++ b/DND4eCharacterGenerator/Assets/ScrapeData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="9510" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="9510" firstSheet="1" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Referencer" sheetId="10" r:id="rId1"/>
@@ -190,7 +190,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4089" uniqueCount="2142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4130" uniqueCount="2157">
   <si>
     <t>Source</t>
   </si>
@@ -5328,9 +5328,6 @@
     <t>Pact Boon|Pact Lore|Shadow Claws|Shadow Twist|Shadow Walk</t>
   </si>
   <si>
-    <t>Players Hand Book 1|Players Hand Book 2|Players Hand Book 3|Eberron Player's  Guide|Neverwinter Campaign Setting|Forgotten Realms Player's Guide|Dragon Magazine|Heroes of the Fallen Lands|Heroes of the Forgotten Kingdoms|Heroes of the Feywild|Heroes of Shadow|Heroes of the Elemental Chaos|Martial Power|Martial Power 2</t>
-  </si>
-  <si>
     <t>NWCS</t>
   </si>
   <si>
@@ -5663,12 +5660,6 @@
   </si>
   <si>
     <t>MM1</t>
-  </si>
-  <si>
-    <t>Players Hand Book 1|Players Hand Book 2|Players Hand Book 3|Eberron Player's  Guide|Neverwinter Campaign Setting|Forgotten Realms Player's Guide|Dark Sun Campaign Setting|Dragon Magazine|Heroes of the Fallen Lands|Heroes of the Forgotten Kingdoms|Heroes of the Feywild|Heroes of Shadow|Heroes of the Elemental Chaos|Martial Power|Martial Power 2|Manual of the Planes|Monster Manual|Monster Manual 2</t>
-  </si>
-  <si>
-    <t>PHB|PHB2|PHB3|EPG|NWCS|FRPG|DSCS|DRMZ|HoFL|HoFK|HoF|HoS|HoEC|MP|MP2|MoP|MM1|MM2</t>
   </si>
   <si>
     <t>Doppleganger</t>
@@ -7145,10 +7136,6 @@
     <t>Martial, Weapon</t>
   </si>
   <si>
-    <t>1[W] + Dexterity modifier (~DEXMod~). If the target is aberrant and has resistance or vulnerability to your attack, you gain a bonus to damage equal to your Wisdom modifier (~WISMod~).
-Level 21: 2[W] + Dexterity modifier (~DEXMod~).</t>
-  </si>
-  <si>
     <t>1d10 + Charisma modifier (~CHAMod~) acid damage.
 Level 21: 2d10 + Charisma modifier (~CHAMod~) acid damage.</t>
   </si>
@@ -7169,19 +7156,83 @@
     <t>Hit Levels</t>
   </si>
   <si>
-    <t>1[W] + (~DEXMod~)|2[W] + (~DEXMod~)</t>
-  </si>
-  <si>
     <t>1|21</t>
   </si>
   <si>
-    <t>1d10 + (~CHAMod~)|2d10 + (~CHAMod~)</t>
-  </si>
-  <si>
     <t>Aegis of Assault</t>
   </si>
   <si>
     <t>W</t>
+  </si>
+  <si>
+    <t>Minor Action</t>
+  </si>
+  <si>
+    <t>Close Burst</t>
+  </si>
+  <si>
+    <t>One creature within the power's area of effect</t>
+  </si>
+  <si>
+    <t>Double Aegis|Escalating Assault|Elemental Assault|Rapid Aegis|Shadowed Aegis|Total Aegis|Vigorous Assualt</t>
+  </si>
+  <si>
+    <t>You mark the target. The target remains marked until you use this power against another target. If you mark other creatures using other powers, the target is still marked. A creature can be subject to only one mark at a time. A new mark supersedes a mark that was already in place.
+If your marked target makes an attack that doesn't include you as a target, it takes a −2 penalty to attack rolls. If that attack hits and the marked target is within 10 squares of you, you can use an immediate reaction to teleport to a square adjacent to the target and make a melee basic attack against it. If no unoccupied space exists adjacent to the target, you can't use this immediate reaction.</t>
+  </si>
+  <si>
+    <t>Aegis of Ensnarement</t>
+  </si>
+  <si>
+    <t>AP</t>
+  </si>
+  <si>
+    <t>Players Hand Book 1|Players Hand Book 2|Players Hand Book 3|Eberron Player's  Guide|Neverwinter Campaign Setting|Forgotten Realms Player's Guide|Dark Sun Campaign Setting|Dragon Magazine|Heroes of the Fallen Lands|Heroes of the Forgotten Kingdoms|Heroes of the Feywild|Heroes of Shadow|Heroes of the Elemental Chaos|Martial Power|Martial Power 2|Manual of the Planes|Monster Manual|Monster Manual 2|Arcane Power</t>
+  </si>
+  <si>
+    <t>PHB|PHB2|PHB3|EPG|NWCS|FRPG|DSCS|DRMZ|HoFL|HoFK|HoF|HoS|HoEC|MP|MP2|MoP|MM1|MM2|AP</t>
+  </si>
+  <si>
+    <t>You mark the target. The target remains marked until you use this power against another target. If you mark another creature using other powers, the target is still marked.
+Until the mark ends, if the target makes any attack that does not include you as a target, it takes a −2 penalty to the attack roll.
+If a target marked by this power is within 10 squares of you when it hits with an attack that does not include you as a target, you can use an immediate reaction after the target's entire attack is resolved to teleport the target to any space adjacent to you. In addition, the target grants combat advantage to all creatures until the end of your next turn. If no unoccupied space exists adjacent to you, you can't use this immediate reaction, and the target doesn't grant combat advantage as a result of this effect.</t>
+  </si>
+  <si>
+    <t>Aegis of Shielding</t>
+  </si>
+  <si>
+    <t>You mark the target. The target remains marked until you use this power against another target. If you mark other creatures using other powers, the target is still marked. A creature can be subject to only one mark at a time. A new mark supersedes a mark that was already in place.
+     If your marked target makes an attack that doesn't include you as a target, it takes a −2 penalty to attack rolls. If that attack hits and the marked target is within 10 squares of you, you can use an immediate interrupt to reduce the damage dealt by that attack to any one creature by an amount equal to 5 + your Constitution modifier (~CONMod~).
+At 11th level, reduce the damage dealt by 10 + your Constitution modifier (~CONMod~). At 21st level, reduce the damage dealt by 15 + your Constitution modifier (~CONMod~).</t>
+  </si>
+  <si>
+    <t>Aggravating Force</t>
+  </si>
+  <si>
+    <t>INT</t>
+  </si>
+  <si>
+    <t>AV</t>
+  </si>
+  <si>
+    <t>1d10 + (~CHAMod~) acid damage|2d10 + (~CHAMod~) acid damage</t>
+  </si>
+  <si>
+    <t>1[~W~] + (~DEXMod~) damage|2[~W~] + (~DEXMod~) damage</t>
+  </si>
+  <si>
+    <t>1[~W~] + Dexterity modifier (~DEXMod~) damage. If the target is aberrant and has resistance or vulnerability to your attack, you gain a bonus to damage equal to your Wisdom modifier (~WISMod~).
+Level 21: 2[~W~] + Dexterity modifier (~DEXMod~) damage.</t>
+  </si>
+  <si>
+    <t>1[~W~] + (~INTMod~) force damage.</t>
+  </si>
+  <si>
+    <t>Intelligence vs. AC</t>
+  </si>
+  <si>
+    <t>1[~W~] + Intelligence modifier (~INTMod~) force damage. Before the end of the user's next turn, the next time an ally attacks the target, that attack's attack roll gains a +2 power bonus.
+Level 21: 2[~W~] + Intelligence modifier (~INTMod~) force damage.</t>
   </si>
 </sst>
 </file>
@@ -8630,7 +8681,10 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8646,7 +8700,7 @@
         <v>677</v>
       </c>
       <c r="C1" t="s">
-        <v>2100</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -8849,10 +8903,10 @@
       </c>
       <c r="B16" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>2141</v>
+        <v>2135</v>
       </c>
       <c r="D16" s="3"/>
     </row>
@@ -8872,7 +8926,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>2098</v>
+        <v>2095</v>
       </c>
       <c r="B18">
         <f ca="1">COUNTA(INDIRECT(A18&amp;"!A:A"))-1</f>
@@ -8898,7 +8952,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9019,7 +9073,7 @@
         <v>148</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1786</v>
+        <v>1785</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>378</v>
@@ -9073,10 +9127,10 @@
         <v>1331</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>1837</v>
+        <v>1834</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>1983</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
@@ -9084,7 +9138,7 @@
         <v>133</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1787</v>
+        <v>1786</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>378</v>
@@ -9132,10 +9186,10 @@
         <v>1317</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>1837</v>
+        <v>1834</v>
       </c>
       <c r="Y3" s="1" t="s">
-        <v>1984</v>
+        <v>1981</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
@@ -9164,7 +9218,7 @@
         <v>485</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>1801</v>
+        <v>1798</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>1266</v>
@@ -9185,10 +9239,10 @@
         <v>1322</v>
       </c>
       <c r="X4" s="1" t="s">
-        <v>1838</v>
+        <v>1835</v>
       </c>
       <c r="Y4" s="1" t="s">
-        <v>1985</v>
+        <v>1982</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
@@ -9211,16 +9265,16 @@
         <v>399</v>
       </c>
       <c r="J5" s="14" t="s">
+        <v>1799</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>1800</v>
+      </c>
+      <c r="L5" s="14" t="s">
+        <v>1801</v>
+      </c>
+      <c r="N5" s="15" t="s">
         <v>1802</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>1803</v>
-      </c>
-      <c r="L5" s="14" t="s">
-        <v>1804</v>
-      </c>
-      <c r="N5" s="15" t="s">
-        <v>1805</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>1267</v>
@@ -9235,7 +9289,7 @@
         <v>1</v>
       </c>
       <c r="S5" s="8" t="s">
-        <v>1795</v>
+        <v>1792</v>
       </c>
       <c r="U5" s="1" t="s">
         <v>1312</v>
@@ -9244,13 +9298,13 @@
         <v>834</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>1806</v>
+        <v>1803</v>
       </c>
       <c r="X5" s="1" t="s">
-        <v>1839</v>
+        <v>1836</v>
       </c>
       <c r="Y5" s="1" t="s">
-        <v>1986</v>
+        <v>1983</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
@@ -9270,13 +9324,13 @@
         <v>403</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>1808</v>
+        <v>1805</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>1809</v>
+        <v>1806</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>1810</v>
+        <v>1807</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>1268</v>
@@ -9291,7 +9345,7 @@
         <v>0</v>
       </c>
       <c r="S6" s="8" t="s">
-        <v>1811</v>
+        <v>1808</v>
       </c>
       <c r="T6" s="1" t="s">
         <v>1310</v>
@@ -9300,28 +9354,28 @@
         <v>801</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>1812</v>
+        <v>1809</v>
       </c>
       <c r="W6" s="1" t="s">
-        <v>1813</v>
+        <v>1810</v>
       </c>
       <c r="X6" s="1" t="s">
-        <v>1840</v>
+        <v>1837</v>
       </c>
       <c r="Y6" s="1" t="s">
-        <v>1987</v>
+        <v>1984</v>
       </c>
       <c r="Z6" s="1" t="s">
-        <v>1807</v>
+        <v>1804</v>
       </c>
       <c r="AH6" s="1"/>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>1790</v>
+        <v>1787</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>1787</v>
+        <v>1786</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>378</v>
@@ -9333,40 +9387,40 @@
         <v>403</v>
       </c>
       <c r="I7" s="1" t="s">
+        <v>1788</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>1789</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>1790</v>
+      </c>
+      <c r="O7" s="1" t="s">
         <v>1791</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="P7" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>0</v>
+      </c>
+      <c r="R7" s="1">
+        <v>1</v>
+      </c>
+      <c r="S7" s="8" t="s">
         <v>1792</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="U7" s="1" t="s">
         <v>1793</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>1794</v>
-      </c>
-      <c r="P7" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="1">
-        <v>0</v>
-      </c>
-      <c r="R7" s="1">
-        <v>1</v>
-      </c>
-      <c r="S7" s="8" t="s">
-        <v>1795</v>
-      </c>
-      <c r="U7" s="1" t="s">
-        <v>1796</v>
       </c>
       <c r="V7" s="1" t="s">
         <v>834</v>
       </c>
       <c r="X7" s="1" t="s">
-        <v>1841</v>
+        <v>1838</v>
       </c>
       <c r="Y7" s="1" t="s">
-        <v>1988</v>
+        <v>1985</v>
       </c>
       <c r="AH7" s="1"/>
     </row>
@@ -9375,7 +9429,7 @@
         <v>131</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>1784</v>
+        <v>1783</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>378</v>
@@ -9423,16 +9477,16 @@
         <v>1290</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>1814</v>
+        <v>1811</v>
       </c>
       <c r="V8" s="1" t="s">
         <v>1318</v>
       </c>
       <c r="X8" s="1" t="s">
-        <v>1842</v>
+        <v>1839</v>
       </c>
       <c r="Y8" s="1" t="s">
-        <v>1989</v>
+        <v>1986</v>
       </c>
       <c r="Z8" s="1" t="s">
         <v>1491</v>
@@ -9459,7 +9513,7 @@
         <v>126</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>1787</v>
+        <v>1786</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>378</v>
@@ -9471,13 +9525,13 @@
         <v>7</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>1798</v>
+        <v>1795</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>1799</v>
+        <v>1796</v>
       </c>
       <c r="N9" s="8" t="s">
-        <v>1797</v>
+        <v>1794</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>1270</v>
@@ -9495,19 +9549,19 @@
         <v>1289</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>1815</v>
+        <v>1812</v>
       </c>
       <c r="V9" s="1" t="s">
         <v>834</v>
       </c>
       <c r="W9" s="1" t="s">
-        <v>1816</v>
+        <v>1813</v>
       </c>
       <c r="X9" s="1" t="s">
-        <v>1843</v>
+        <v>1840</v>
       </c>
       <c r="Y9" s="1" t="s">
-        <v>1990</v>
+        <v>1987</v>
       </c>
       <c r="AH9" s="1"/>
     </row>
@@ -9528,13 +9582,13 @@
         <v>7</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>1817</v>
+        <v>1814</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>480</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>1800</v>
+        <v>1797</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>167</v>
@@ -9561,10 +9615,10 @@
         <v>1319</v>
       </c>
       <c r="X10" s="1" t="s">
-        <v>1844</v>
+        <v>1841</v>
       </c>
       <c r="Y10" s="1" t="s">
-        <v>1991</v>
+        <v>1988</v>
       </c>
       <c r="AH10" s="1"/>
     </row>
@@ -9573,7 +9627,7 @@
         <v>135</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>1784</v>
+        <v>1783</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>378</v>
@@ -9606,7 +9660,7 @@
         <v>1255</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>1818</v>
+        <v>1815</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>1272</v>
@@ -9630,13 +9684,13 @@
         <v>1320</v>
       </c>
       <c r="W11" s="1" t="s">
-        <v>1819</v>
+        <v>1816</v>
       </c>
       <c r="X11" s="1" t="s">
-        <v>1845</v>
+        <v>1842</v>
       </c>
       <c r="Y11" s="1" t="s">
-        <v>1992</v>
+        <v>1989</v>
       </c>
       <c r="Z11" s="1" t="s">
         <v>1496</v>
@@ -9664,7 +9718,7 @@
         <v>134</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>1784</v>
+        <v>1783</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>378</v>
@@ -9697,7 +9751,7 @@
         <v>1256</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>1820</v>
+        <v>1817</v>
       </c>
       <c r="O12" s="1" t="s">
         <v>1273</v>
@@ -9721,13 +9775,13 @@
         <v>1321</v>
       </c>
       <c r="W12" s="1" t="s">
-        <v>1821</v>
+        <v>1818</v>
       </c>
       <c r="X12" s="1" t="s">
-        <v>1846</v>
+        <v>1843</v>
       </c>
       <c r="Y12" s="1" t="s">
-        <v>1993</v>
+        <v>1990</v>
       </c>
       <c r="Z12" s="1" t="s">
         <v>1499</v>
@@ -9754,7 +9808,7 @@
         <v>139</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>1784</v>
+        <v>1783</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>378</v>
@@ -9787,7 +9841,7 @@
         <v>1257</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>1822</v>
+        <v>1819</v>
       </c>
       <c r="O13" s="1" t="s">
         <v>1274</v>
@@ -9811,13 +9865,13 @@
         <v>1321</v>
       </c>
       <c r="W13" s="1" t="s">
-        <v>1823</v>
+        <v>1820</v>
       </c>
       <c r="X13" s="1" t="s">
-        <v>1847</v>
+        <v>1844</v>
       </c>
       <c r="Y13" s="1" t="s">
-        <v>1994</v>
+        <v>1991</v>
       </c>
       <c r="Z13" s="1" t="s">
         <v>1502</v>
@@ -9844,7 +9898,7 @@
         <v>120</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>1783</v>
+        <v>1782</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>378</v>
@@ -9889,13 +9943,13 @@
         <v>1322</v>
       </c>
       <c r="X14" s="1" t="s">
-        <v>1848</v>
+        <v>1845</v>
       </c>
       <c r="Y14" s="1" t="s">
-        <v>1995</v>
+        <v>1992</v>
       </c>
       <c r="Z14" s="1" t="s">
-        <v>1824</v>
+        <v>1821</v>
       </c>
       <c r="AH14" s="1"/>
       <c r="AK14" s="17"/>
@@ -9905,7 +9959,7 @@
         <v>118</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>1787</v>
+        <v>1786</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>378</v>
@@ -9917,7 +9971,7 @@
         <v>403</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>1828</v>
+        <v>1825</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>459</v>
@@ -9932,7 +9986,7 @@
         <v>456</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>1825</v>
+        <v>1822</v>
       </c>
       <c r="O15" s="1" t="s">
         <v>1586</v>
@@ -9956,13 +10010,13 @@
         <v>1323</v>
       </c>
       <c r="X15" s="1" t="s">
-        <v>1849</v>
+        <v>1846</v>
       </c>
       <c r="Y15" s="1" t="s">
-        <v>1996</v>
+        <v>1993</v>
       </c>
       <c r="Z15" s="1" t="s">
-        <v>1827</v>
+        <v>1824</v>
       </c>
       <c r="AH15" s="1"/>
     </row>
@@ -9983,16 +10037,16 @@
         <v>403</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>1832</v>
+        <v>1829</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>1833</v>
+        <v>1830</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>1829</v>
+        <v>1826</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>1831</v>
+        <v>1828</v>
       </c>
       <c r="P16" s="1">
         <v>0</v>
@@ -10004,7 +10058,7 @@
         <v>0</v>
       </c>
       <c r="S16" s="8" t="s">
-        <v>1830</v>
+        <v>1827</v>
       </c>
       <c r="U16" s="1" t="s">
         <v>803</v>
@@ -10013,13 +10067,13 @@
         <v>1323</v>
       </c>
       <c r="X16" s="1" t="s">
-        <v>1850</v>
+        <v>1847</v>
       </c>
       <c r="Y16" s="1" t="s">
-        <v>1997</v>
+        <v>1994</v>
       </c>
       <c r="Z16" s="1" t="s">
-        <v>1826</v>
+        <v>1823</v>
       </c>
       <c r="AH16" s="1"/>
     </row>
@@ -10028,7 +10082,7 @@
         <v>145</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>1787</v>
+        <v>1786</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>378</v>
@@ -10052,7 +10106,7 @@
         <v>452</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>1835</v>
+        <v>1832</v>
       </c>
       <c r="O17" s="1" t="s">
         <v>1266</v>
@@ -10079,13 +10133,13 @@
         <v>1332</v>
       </c>
       <c r="X17" s="1" t="s">
-        <v>1851</v>
+        <v>1848</v>
       </c>
       <c r="Y17" s="1" t="s">
-        <v>1998</v>
+        <v>1995</v>
       </c>
       <c r="Z17" s="1" t="s">
-        <v>1834</v>
+        <v>1831</v>
       </c>
       <c r="AH17" s="1"/>
     </row>
@@ -10118,7 +10172,7 @@
         <v>448</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>1836</v>
+        <v>1833</v>
       </c>
       <c r="O18" s="1" t="s">
         <v>1273</v>
@@ -10142,10 +10196,10 @@
         <v>1321</v>
       </c>
       <c r="X18" s="1" t="s">
-        <v>1852</v>
+        <v>1849</v>
       </c>
       <c r="Y18" s="1" t="s">
-        <v>1999</v>
+        <v>1996</v>
       </c>
       <c r="AH18" s="1"/>
     </row>
@@ -10154,7 +10208,7 @@
         <v>426</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>1787</v>
+        <v>1786</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>383</v>
@@ -10196,10 +10250,10 @@
         <v>1317</v>
       </c>
       <c r="X19" s="1" t="s">
-        <v>1856</v>
+        <v>1853</v>
       </c>
       <c r="Y19" s="1" t="s">
-        <v>2000</v>
+        <v>1997</v>
       </c>
       <c r="AH19" s="1"/>
     </row>
@@ -10220,28 +10274,28 @@
         <v>403</v>
       </c>
       <c r="H20" s="1" t="s">
+        <v>1854</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>1856</v>
+      </c>
+      <c r="K20" s="1" t="s">
         <v>1857</v>
       </c>
-      <c r="I20" s="1" t="s">
+      <c r="N20" s="1" t="s">
+        <v>1858</v>
+      </c>
+      <c r="P20" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>0</v>
+      </c>
+      <c r="R20" s="8">
+        <v>1</v>
+      </c>
+      <c r="S20" s="8" t="s">
         <v>1859</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>1860</v>
-      </c>
-      <c r="N20" s="1" t="s">
-        <v>1861</v>
-      </c>
-      <c r="P20" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="1">
-        <v>0</v>
-      </c>
-      <c r="R20" s="8">
-        <v>1</v>
-      </c>
-      <c r="S20" s="8" t="s">
-        <v>1862</v>
       </c>
       <c r="U20" s="1" t="s">
         <v>806</v>
@@ -10250,16 +10304,16 @@
         <v>1325</v>
       </c>
       <c r="X20" s="1" t="s">
-        <v>1863</v>
+        <v>1860</v>
       </c>
       <c r="Y20" s="1" t="s">
-        <v>2001</v>
+        <v>1998</v>
       </c>
       <c r="Z20" s="1" t="s">
-        <v>1858</v>
+        <v>1855</v>
       </c>
       <c r="AA20" s="1" t="s">
-        <v>1857</v>
+        <v>1854</v>
       </c>
       <c r="AH20" s="1"/>
       <c r="AK20" s="17"/>
@@ -10269,7 +10323,7 @@
         <v>1616</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>1784</v>
+        <v>1783</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>378</v>
@@ -10299,7 +10353,7 @@
         <v>441</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>1864</v>
+        <v>1861</v>
       </c>
       <c r="O21" s="1" t="s">
         <v>1276</v>
@@ -10323,10 +10377,10 @@
         <v>1333</v>
       </c>
       <c r="X21" s="1" t="s">
-        <v>1865</v>
+        <v>1862</v>
       </c>
       <c r="Y21" s="1" t="s">
-        <v>2002</v>
+        <v>1999</v>
       </c>
       <c r="Z21" s="1" t="s">
         <v>1505</v>
@@ -10353,7 +10407,7 @@
         <v>1617</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>1784</v>
+        <v>1783</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>378</v>
@@ -10365,28 +10419,28 @@
         <v>377</v>
       </c>
       <c r="I22" s="1" t="s">
+        <v>1863</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>1864</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>1865</v>
+      </c>
+      <c r="O22" s="1" t="s">
         <v>1866</v>
       </c>
-      <c r="K22" s="1" t="s">
+      <c r="P22" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="1">
+        <v>0</v>
+      </c>
+      <c r="R22" s="1">
+        <v>0</v>
+      </c>
+      <c r="S22" s="8" t="s">
         <v>1867</v>
-      </c>
-      <c r="N22" s="1" t="s">
-        <v>1868</v>
-      </c>
-      <c r="O22" s="1" t="s">
-        <v>1869</v>
-      </c>
-      <c r="P22" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="1">
-        <v>0</v>
-      </c>
-      <c r="R22" s="1">
-        <v>0</v>
-      </c>
-      <c r="S22" s="8" t="s">
-        <v>1870</v>
       </c>
       <c r="U22" s="1" t="s">
         <v>807</v>
@@ -10398,10 +10452,10 @@
         <v>1334</v>
       </c>
       <c r="X22" s="1" t="s">
-        <v>1871</v>
+        <v>1868</v>
       </c>
       <c r="Y22" s="1" t="s">
-        <v>2003</v>
+        <v>2000</v>
       </c>
       <c r="AH22" s="1"/>
     </row>
@@ -10440,7 +10494,7 @@
         <v>436</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>1872</v>
+        <v>1869</v>
       </c>
       <c r="O23" s="1" t="s">
         <v>1277</v>
@@ -10461,10 +10515,10 @@
         <v>1327</v>
       </c>
       <c r="X23" s="1" t="s">
-        <v>1854</v>
+        <v>1851</v>
       </c>
       <c r="Y23" s="1" t="s">
-        <v>2004</v>
+        <v>2001</v>
       </c>
       <c r="Z23" s="1" t="s">
         <v>1508</v>
@@ -10491,7 +10545,7 @@
         <v>146</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>1777</v>
+        <v>1776</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>378</v>
@@ -10515,7 +10569,7 @@
         <v>396</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>1873</v>
+        <v>1870</v>
       </c>
       <c r="O24" s="1" t="s">
         <v>1268</v>
@@ -10539,10 +10593,10 @@
         <v>1321</v>
       </c>
       <c r="X24" s="1" t="s">
-        <v>1874</v>
+        <v>1871</v>
       </c>
       <c r="Y24" s="1" t="s">
-        <v>2005</v>
+        <v>2002</v>
       </c>
       <c r="AH24" s="1"/>
     </row>
@@ -10575,7 +10629,7 @@
         <v>431</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>1875</v>
+        <v>1872</v>
       </c>
       <c r="O25" s="1" t="s">
         <v>1270</v>
@@ -10596,10 +10650,10 @@
         <v>1327</v>
       </c>
       <c r="X25" s="1" t="s">
-        <v>1876</v>
+        <v>1873</v>
       </c>
       <c r="Y25" s="1" t="s">
-        <v>2006</v>
+        <v>2003</v>
       </c>
       <c r="AH25" s="1"/>
       <c r="AJ25" s="16"/>
@@ -10609,7 +10663,7 @@
         <v>155</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>1787</v>
+        <v>1786</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>378</v>
@@ -10627,7 +10681,7 @@
         <v>429</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>1877</v>
+        <v>1874</v>
       </c>
       <c r="O26" s="1" t="s">
         <v>1278</v>
@@ -10651,10 +10705,10 @@
         <v>1317</v>
       </c>
       <c r="X26" s="1" t="s">
-        <v>1878</v>
+        <v>1875</v>
       </c>
       <c r="Y26" s="1" t="s">
-        <v>2007</v>
+        <v>2004</v>
       </c>
       <c r="AH26" s="1"/>
     </row>
@@ -10663,7 +10717,7 @@
         <v>150</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>1784</v>
+        <v>1783</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>378</v>
@@ -10693,7 +10747,7 @@
         <v>422</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>1879</v>
+        <v>1876</v>
       </c>
       <c r="O27" s="1" t="s">
         <v>379</v>
@@ -10717,10 +10771,10 @@
         <v>1335</v>
       </c>
       <c r="X27" s="1" t="s">
-        <v>1880</v>
+        <v>1877</v>
       </c>
       <c r="Y27" s="1" t="s">
-        <v>2008</v>
+        <v>2005</v>
       </c>
       <c r="Z27" s="1" t="s">
         <v>1511</v>
@@ -10759,13 +10813,13 @@
         <v>403</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>1881</v>
+        <v>1878</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>1882</v>
+        <v>1879</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>1923</v>
+        <v>1920</v>
       </c>
       <c r="P28" s="1">
         <v>0</v>
@@ -10777,7 +10831,7 @@
         <v>0</v>
       </c>
       <c r="S28" s="8" t="s">
-        <v>1883</v>
+        <v>1880</v>
       </c>
       <c r="U28" s="1" t="s">
         <v>808</v>
@@ -10786,10 +10840,10 @@
         <v>834</v>
       </c>
       <c r="X28" s="1" t="s">
-        <v>1924</v>
+        <v>1921</v>
       </c>
       <c r="Y28" s="1" t="s">
-        <v>2009</v>
+        <v>2006</v>
       </c>
       <c r="AH28" s="1"/>
     </row>
@@ -10822,7 +10876,7 @@
         <v>418</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>1887</v>
+        <v>1884</v>
       </c>
       <c r="O29" s="1" t="s">
         <v>1279</v>
@@ -10846,10 +10900,10 @@
         <v>1327</v>
       </c>
       <c r="X29" s="1" t="s">
-        <v>1884</v>
+        <v>1881</v>
       </c>
       <c r="Y29" s="1" t="s">
-        <v>2010</v>
+        <v>2007</v>
       </c>
       <c r="AH29" s="1"/>
     </row>
@@ -10858,7 +10912,7 @@
         <v>151</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>1787</v>
+        <v>1786</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>383</v>
@@ -10870,17 +10924,17 @@
         <v>403</v>
       </c>
       <c r="I30" s="1" t="s">
+        <v>1882</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>1883</v>
+      </c>
+      <c r="N30" s="1" t="s">
         <v>1885</v>
       </c>
-      <c r="K30" s="1" t="s">
+      <c r="O30" s="1" t="s">
         <v>1886</v>
       </c>
-      <c r="N30" s="1" t="s">
-        <v>1888</v>
-      </c>
-      <c r="O30" s="1" t="s">
-        <v>1889</v>
-      </c>
       <c r="P30" s="1">
         <v>0</v>
       </c>
@@ -10891,16 +10945,16 @@
         <v>0</v>
       </c>
       <c r="S30" s="8" t="s">
-        <v>1890</v>
+        <v>1887</v>
       </c>
       <c r="V30" s="1" t="s">
         <v>1318</v>
       </c>
       <c r="X30" s="1" t="s">
-        <v>1891</v>
+        <v>1888</v>
       </c>
       <c r="Y30" s="1" t="s">
-        <v>2011</v>
+        <v>2008</v>
       </c>
       <c r="AH30" s="1"/>
     </row>
@@ -10936,7 +10990,7 @@
         <v>414</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>1892</v>
+        <v>1889</v>
       </c>
       <c r="O31" s="1" t="s">
         <v>1280</v>
@@ -10963,10 +11017,10 @@
         <v>1336</v>
       </c>
       <c r="X31" s="1" t="s">
-        <v>1893</v>
+        <v>1890</v>
       </c>
       <c r="Y31" s="1" t="s">
-        <v>2012</v>
+        <v>2009</v>
       </c>
       <c r="AH31" s="1"/>
     </row>
@@ -10990,13 +11044,13 @@
         <v>694</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>1894</v>
+        <v>1891</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>1895</v>
+        <v>1892</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>1896</v>
+        <v>1893</v>
       </c>
       <c r="O32" s="1" t="s">
         <v>1280</v>
@@ -11011,7 +11065,7 @@
         <v>0</v>
       </c>
       <c r="S32" s="8" t="s">
-        <v>1897</v>
+        <v>1894</v>
       </c>
       <c r="U32" s="1" t="s">
         <v>810</v>
@@ -11020,10 +11074,10 @@
         <v>1320</v>
       </c>
       <c r="X32" s="1" t="s">
-        <v>1898</v>
+        <v>1895</v>
       </c>
       <c r="Y32" s="1" t="s">
-        <v>2013</v>
+        <v>2010</v>
       </c>
       <c r="AH32" s="1"/>
     </row>
@@ -11032,7 +11086,7 @@
         <v>142</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>1787</v>
+        <v>1786</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>378</v>
@@ -11044,16 +11098,16 @@
         <v>377</v>
       </c>
       <c r="I33" s="1" t="s">
+        <v>1896</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>1897</v>
+      </c>
+      <c r="N33" s="1" t="s">
         <v>1899</v>
       </c>
-      <c r="K33" s="1" t="s">
-        <v>1900</v>
-      </c>
-      <c r="N33" s="1" t="s">
-        <v>1902</v>
-      </c>
       <c r="O33" s="1" t="s">
-        <v>1901</v>
+        <v>1898</v>
       </c>
       <c r="P33" s="1">
         <v>0</v>
@@ -11074,10 +11128,10 @@
         <v>1328</v>
       </c>
       <c r="X33" s="1" t="s">
-        <v>1903</v>
+        <v>1900</v>
       </c>
       <c r="Y33" s="1" t="s">
-        <v>2014</v>
+        <v>2011</v>
       </c>
       <c r="AH33" s="1"/>
     </row>
@@ -11086,7 +11140,7 @@
         <v>144</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>1777</v>
+        <v>1776</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>413</v>
@@ -11113,7 +11167,7 @@
         <v>408</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>1904</v>
+        <v>1901</v>
       </c>
       <c r="O34" s="1" t="s">
         <v>1279</v>
@@ -11131,16 +11185,16 @@
         <v>1303</v>
       </c>
       <c r="U34" s="1" t="s">
-        <v>1905</v>
+        <v>1902</v>
       </c>
       <c r="V34" s="1" t="s">
         <v>1321</v>
       </c>
       <c r="X34" s="1" t="s">
-        <v>1906</v>
+        <v>1903</v>
       </c>
       <c r="Y34" s="1" t="s">
-        <v>2015</v>
+        <v>2012</v>
       </c>
       <c r="AH34" s="1"/>
     </row>
@@ -11149,7 +11203,7 @@
         <v>130</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>1775</v>
+        <v>1774</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>378</v>
@@ -11164,10 +11218,10 @@
         <v>407</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>1913</v>
+        <v>1910</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>1907</v>
+        <v>1904</v>
       </c>
       <c r="O35" s="1" t="s">
         <v>1279</v>
@@ -11182,7 +11236,7 @@
         <v>0</v>
       </c>
       <c r="S35" s="8" t="s">
-        <v>1870</v>
+        <v>1867</v>
       </c>
       <c r="U35" s="1" t="s">
         <v>812</v>
@@ -11191,13 +11245,13 @@
         <v>834</v>
       </c>
       <c r="X35" s="1" t="s">
-        <v>1908</v>
+        <v>1905</v>
       </c>
       <c r="Y35" s="1" t="s">
-        <v>2016</v>
+        <v>2013</v>
       </c>
       <c r="Z35" s="1" t="s">
-        <v>1909</v>
+        <v>1906</v>
       </c>
       <c r="AH35" s="1"/>
       <c r="AK35" s="17"/>
@@ -11207,7 +11261,7 @@
         <v>116</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>1777</v>
+        <v>1776</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>378</v>
@@ -11219,13 +11273,13 @@
         <v>377</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>1911</v>
+        <v>1908</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>1912</v>
+        <v>1909</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>1910</v>
+        <v>1907</v>
       </c>
       <c r="O36" s="1" t="s">
         <v>1281</v>
@@ -11249,10 +11303,10 @@
         <v>1321</v>
       </c>
       <c r="X36" s="1" t="s">
-        <v>1853</v>
+        <v>1850</v>
       </c>
       <c r="Y36" s="1" t="s">
-        <v>2017</v>
+        <v>2014</v>
       </c>
       <c r="AH36" s="1"/>
     </row>
@@ -11261,7 +11315,7 @@
         <v>115</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>1787</v>
+        <v>1786</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>378</v>
@@ -11285,7 +11339,7 @@
         <v>405</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>1914</v>
+        <v>1911</v>
       </c>
       <c r="O37" s="1" t="s">
         <v>1274</v>
@@ -11309,13 +11363,13 @@
         <v>834</v>
       </c>
       <c r="W37" s="1" t="s">
-        <v>1915</v>
+        <v>1912</v>
       </c>
       <c r="X37" s="1" t="s">
-        <v>1916</v>
+        <v>1913</v>
       </c>
       <c r="Y37" s="1" t="s">
-        <v>2018</v>
+        <v>2015</v>
       </c>
       <c r="AH37" s="1"/>
     </row>
@@ -11324,7 +11378,7 @@
         <v>124</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>1775</v>
+        <v>1774</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>378</v>
@@ -11336,16 +11390,16 @@
         <v>7</v>
       </c>
       <c r="H38" s="1" t="s">
+        <v>1914</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>1915</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>1916</v>
+      </c>
+      <c r="N38" s="1" t="s">
         <v>1917</v>
-      </c>
-      <c r="I38" s="1" t="s">
-        <v>1918</v>
-      </c>
-      <c r="K38" s="1" t="s">
-        <v>1919</v>
-      </c>
-      <c r="N38" s="1" t="s">
-        <v>1920</v>
       </c>
       <c r="O38" s="1" t="s">
         <v>1279</v>
@@ -11363,16 +11417,16 @@
         <v>1296</v>
       </c>
       <c r="U38" s="1" t="s">
-        <v>1921</v>
+        <v>1918</v>
       </c>
       <c r="V38" s="1" t="s">
         <v>1327</v>
       </c>
       <c r="X38" s="1" t="s">
-        <v>1922</v>
+        <v>1919</v>
       </c>
       <c r="Y38" s="1" t="s">
-        <v>2019</v>
+        <v>2016</v>
       </c>
       <c r="AH38" s="1"/>
     </row>
@@ -11393,7 +11447,7 @@
         <v>403</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>1926</v>
+        <v>1923</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>402</v>
@@ -11402,7 +11456,7 @@
         <v>401</v>
       </c>
       <c r="N39" s="1" t="s">
-        <v>1925</v>
+        <v>1922</v>
       </c>
       <c r="O39" s="1" t="s">
         <v>1282</v>
@@ -11429,10 +11483,10 @@
         <v>1329</v>
       </c>
       <c r="X39" s="1" t="s">
-        <v>1927</v>
+        <v>1924</v>
       </c>
       <c r="Y39" s="1" t="s">
-        <v>2020</v>
+        <v>2017</v>
       </c>
       <c r="AH39" s="1"/>
     </row>
@@ -11453,7 +11507,7 @@
         <v>377</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>1928</v>
+        <v>1925</v>
       </c>
       <c r="I40" s="1" t="s">
         <v>399</v>
@@ -11489,10 +11543,10 @@
         <v>1327</v>
       </c>
       <c r="X40" s="1" t="s">
-        <v>1853</v>
+        <v>1850</v>
       </c>
       <c r="Y40" s="1" t="s">
-        <v>2021</v>
+        <v>2018</v>
       </c>
       <c r="AH40" s="1"/>
     </row>
@@ -11501,7 +11555,7 @@
         <v>125</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>1777</v>
+        <v>1776</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>383</v>
@@ -11522,7 +11576,7 @@
         <v>391</v>
       </c>
       <c r="N41" s="1" t="s">
-        <v>1929</v>
+        <v>1926</v>
       </c>
       <c r="O41" s="1" t="s">
         <v>1284</v>
@@ -11543,13 +11597,13 @@
         <v>389</v>
       </c>
       <c r="V41" s="1" t="s">
-        <v>1930</v>
+        <v>1927</v>
       </c>
       <c r="X41" s="1" t="s">
-        <v>1931</v>
+        <v>1928</v>
       </c>
       <c r="Y41" s="1" t="s">
-        <v>2022</v>
+        <v>2019</v>
       </c>
       <c r="AH41" s="1"/>
     </row>
@@ -11570,17 +11624,17 @@
         <v>377</v>
       </c>
       <c r="I42" s="1" t="s">
+        <v>1929</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>1930</v>
+      </c>
+      <c r="N42" s="1" t="s">
+        <v>1931</v>
+      </c>
+      <c r="O42" s="1" t="s">
         <v>1932</v>
       </c>
-      <c r="K42" s="1" t="s">
-        <v>1933</v>
-      </c>
-      <c r="N42" s="1" t="s">
-        <v>1934</v>
-      </c>
-      <c r="O42" s="1" t="s">
-        <v>1935</v>
-      </c>
       <c r="P42" s="1">
         <v>0</v>
       </c>
@@ -11591,7 +11645,7 @@
         <v>0</v>
       </c>
       <c r="S42" s="8" t="s">
-        <v>1862</v>
+        <v>1859</v>
       </c>
       <c r="U42" s="1" t="s">
         <v>814</v>
@@ -11600,10 +11654,10 @@
         <v>1330</v>
       </c>
       <c r="X42" s="1" t="s">
-        <v>1936</v>
+        <v>1933</v>
       </c>
       <c r="Y42" s="1" t="s">
-        <v>2023</v>
+        <v>2020</v>
       </c>
       <c r="AH42" s="1"/>
     </row>
@@ -11642,7 +11696,7 @@
         <v>385</v>
       </c>
       <c r="N43" s="1" t="s">
-        <v>1937</v>
+        <v>1934</v>
       </c>
       <c r="O43" s="1" t="s">
         <v>1285</v>
@@ -11663,13 +11717,13 @@
         <v>208</v>
       </c>
       <c r="V43" s="1" t="s">
-        <v>1938</v>
+        <v>1935</v>
       </c>
       <c r="X43" s="1" t="s">
-        <v>1855</v>
+        <v>1852</v>
       </c>
       <c r="Y43" s="1" t="s">
-        <v>2024</v>
+        <v>2021</v>
       </c>
       <c r="Z43" s="1" t="s">
         <v>1514</v>
@@ -11711,7 +11765,7 @@
         <v>381</v>
       </c>
       <c r="N44" s="1" t="s">
-        <v>1939</v>
+        <v>1936</v>
       </c>
       <c r="O44" s="1" t="s">
         <v>1286</v>
@@ -11732,16 +11786,16 @@
         <v>817</v>
       </c>
       <c r="U44" s="1" t="s">
-        <v>1940</v>
+        <v>1937</v>
       </c>
       <c r="V44" s="1" t="s">
         <v>1327</v>
       </c>
       <c r="X44" s="1" t="s">
-        <v>1941</v>
+        <v>1938</v>
       </c>
       <c r="Y44" s="1" t="s">
-        <v>2025</v>
+        <v>2022</v>
       </c>
       <c r="AH44" s="1"/>
     </row>
@@ -11750,7 +11804,7 @@
         <v>153</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>1775</v>
+        <v>1774</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>378</v>
@@ -11762,49 +11816,49 @@
         <v>377</v>
       </c>
       <c r="H45" s="1" t="s">
+        <v>1939</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>1941</v>
+      </c>
+      <c r="K45" s="1" t="s">
         <v>1942</v>
       </c>
-      <c r="I45" s="1" t="s">
+      <c r="N45" s="17" t="s">
+        <v>1943</v>
+      </c>
+      <c r="O45" s="1" t="s">
         <v>1944</v>
       </c>
-      <c r="K45" s="1" t="s">
+      <c r="P45" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q45" s="1">
+        <v>0</v>
+      </c>
+      <c r="R45" s="1">
+        <v>0</v>
+      </c>
+      <c r="S45" s="8" t="s">
         <v>1945</v>
       </c>
-      <c r="N45" s="17" t="s">
+      <c r="T45" s="1" t="s">
+        <v>1948</v>
+      </c>
+      <c r="U45" s="1" t="s">
         <v>1946</v>
-      </c>
-      <c r="O45" s="1" t="s">
-        <v>1947</v>
-      </c>
-      <c r="P45" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q45" s="1">
-        <v>0</v>
-      </c>
-      <c r="R45" s="1">
-        <v>0</v>
-      </c>
-      <c r="S45" s="8" t="s">
-        <v>1948</v>
-      </c>
-      <c r="T45" s="1" t="s">
-        <v>1951</v>
-      </c>
-      <c r="U45" s="1" t="s">
-        <v>1949</v>
       </c>
       <c r="V45" s="1" t="s">
         <v>1327</v>
       </c>
       <c r="X45" s="1" t="s">
-        <v>1950</v>
+        <v>1947</v>
       </c>
       <c r="Y45" s="1" t="s">
-        <v>2026</v>
+        <v>2023</v>
       </c>
       <c r="Z45" s="1" t="s">
-        <v>1943</v>
+        <v>1940</v>
       </c>
       <c r="AH45" s="1"/>
       <c r="AK45" s="17"/>
@@ -11814,7 +11868,7 @@
         <v>152</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>1784</v>
+        <v>1783</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>378</v>
@@ -11826,13 +11880,13 @@
         <v>403</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>1952</v>
+        <v>1949</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>1953</v>
+        <v>1950</v>
       </c>
       <c r="N46" s="1" t="s">
-        <v>1954</v>
+        <v>1951</v>
       </c>
       <c r="P46" s="1">
         <v>0</v>
@@ -11844,7 +11898,7 @@
         <v>1</v>
       </c>
       <c r="S46" s="8" t="s">
-        <v>1870</v>
+        <v>1867</v>
       </c>
       <c r="U46" s="1" t="s">
         <v>815</v>
@@ -11853,10 +11907,10 @@
         <v>834</v>
       </c>
       <c r="X46" s="1" t="s">
-        <v>1955</v>
+        <v>1952</v>
       </c>
       <c r="Y46" s="1" t="s">
-        <v>2027</v>
+        <v>2024</v>
       </c>
       <c r="AH46" s="1"/>
     </row>
@@ -11880,7 +11934,7 @@
         <v>696</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>1961</v>
+        <v>1958</v>
       </c>
       <c r="I47" s="1" t="s">
         <v>376</v>
@@ -11889,7 +11943,7 @@
         <v>375</v>
       </c>
       <c r="N47" s="1" t="s">
-        <v>1956</v>
+        <v>1953</v>
       </c>
       <c r="O47" s="1" t="s">
         <v>1287</v>
@@ -11913,22 +11967,22 @@
         <v>1321</v>
       </c>
       <c r="X47" s="1" t="s">
-        <v>1853</v>
+        <v>1850</v>
       </c>
       <c r="Y47" s="1" t="s">
-        <v>2028</v>
+        <v>2025</v>
       </c>
       <c r="Z47" s="1" t="s">
+        <v>1954</v>
+      </c>
+      <c r="AA47" s="1" t="s">
+        <v>1955</v>
+      </c>
+      <c r="AC47" s="1" t="s">
+        <v>1956</v>
+      </c>
+      <c r="AD47" s="1" t="s">
         <v>1957</v>
-      </c>
-      <c r="AA47" s="1" t="s">
-        <v>1958</v>
-      </c>
-      <c r="AC47" s="1" t="s">
-        <v>1959</v>
-      </c>
-      <c r="AD47" s="1" t="s">
-        <v>1960</v>
       </c>
       <c r="AH47" s="1"/>
     </row>
@@ -11962,8 +12016,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12232,7 +12289,12 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:D113"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -13320,7 +13382,12 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -13536,7 +13603,10 @@
   <dimension ref="A1:E230"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15372,7 +15442,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15392,7 +15465,12 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:F106"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -16588,13 +16666,18 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:AV50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="C1" sqref="C1"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.5703125" style="3" customWidth="1"/>
     <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
@@ -16623,58 +16706,58 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>2103</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2104</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2069</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2088</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2070</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2076</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2077</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>2131</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>2132</v>
+      </c>
+      <c r="L1" t="s">
+        <v>2107</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>2106</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>2107</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>2072</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2091</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="N1" t="s">
+        <v>2108</v>
+      </c>
+      <c r="O1" t="s">
         <v>2073</v>
       </c>
-      <c r="H1" t="s">
-        <v>2079</v>
-      </c>
-      <c r="I1" t="s">
-        <v>2080</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>2135</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>2136</v>
-      </c>
-      <c r="L1" t="s">
-        <v>2110</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>2109</v>
-      </c>
-      <c r="N1" t="s">
-        <v>2111</v>
-      </c>
-      <c r="O1" t="s">
-        <v>2076</v>
-      </c>
       <c r="P1" t="s">
-        <v>2077</v>
+        <v>2074</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>2116</v>
+        <v>2113</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>2095</v>
+        <v>2092</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>2126</v>
+        <v>2123</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>2127</v>
+        <v>2124</v>
       </c>
       <c r="U1" s="3" t="s">
         <v>683</v>
@@ -16686,70 +16769,70 @@
         <v>1480</v>
       </c>
       <c r="X1" t="s">
+        <v>2109</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>2111</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>2110</v>
+      </c>
+      <c r="AA1" s="3" t="s">
         <v>2112</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="AB1" t="s">
         <v>2114</v>
       </c>
-      <c r="Z1" t="s">
-        <v>2113</v>
-      </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>2115</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" s="3" t="s">
+        <v>2116</v>
+      </c>
+      <c r="AE1" t="s">
         <v>2117</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>2118</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
+        <v>2120</v>
+      </c>
+      <c r="AH1" s="3" t="s">
         <v>2119</v>
       </c>
-      <c r="AE1" t="s">
-        <v>2120</v>
-      </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AI1" t="s">
         <v>2121</v>
       </c>
-      <c r="AG1" s="3" t="s">
-        <v>2123</v>
-      </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AJ1" t="s">
+        <v>2102</v>
+      </c>
+      <c r="AK1" s="3" t="s">
         <v>2122</v>
       </c>
-      <c r="AI1" t="s">
-        <v>2124</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>2105</v>
-      </c>
-      <c r="AK1" s="3" t="s">
-        <v>2125</v>
-      </c>
       <c r="AL1" s="3" t="s">
-        <v>2114</v>
+        <v>2111</v>
       </c>
       <c r="AM1" s="3" t="s">
-        <v>2119</v>
+        <v>2116</v>
       </c>
       <c r="AN1" s="3" t="s">
-        <v>2120</v>
+        <v>2117</v>
       </c>
       <c r="AO1" s="3" t="s">
-        <v>2105</v>
+        <v>2102</v>
       </c>
       <c r="AP1" s="3" t="s">
-        <v>2125</v>
+        <v>2122</v>
       </c>
       <c r="AQ1" s="3" t="s">
-        <v>2114</v>
+        <v>2111</v>
       </c>
       <c r="AR1" s="3" t="s">
-        <v>2119</v>
+        <v>2116</v>
       </c>
       <c r="AS1" s="3" t="s">
-        <v>2120</v>
+        <v>2117</v>
       </c>
       <c r="AT1" s="3"/>
       <c r="AU1" s="3"/>
@@ -16757,7 +16840,7 @@
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2070</v>
+        <v>2067</v>
       </c>
       <c r="B2" t="s">
         <v>700</v>
@@ -16775,28 +16858,28 @@
         <v>1084</v>
       </c>
       <c r="G2" t="s">
-        <v>2074</v>
+        <v>2071</v>
       </c>
       <c r="H2" t="s">
+        <v>2129</v>
+      </c>
+      <c r="I2" t="s">
+        <v>2078</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>2152</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>2133</v>
       </c>
-      <c r="I2" t="s">
-        <v>2081</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>2137</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>2138</v>
-      </c>
       <c r="L2" t="s">
-        <v>2101</v>
+        <v>2098</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>2108</v>
+        <v>2105</v>
       </c>
       <c r="N2" t="s">
-        <v>2102</v>
+        <v>2099</v>
       </c>
       <c r="O2" t="s">
         <v>390</v>
@@ -16810,23 +16893,23 @@
       </c>
       <c r="W2" s="3" t="str">
         <f>IF(X2&lt;&gt;"",X2,"")&amp;IF(Y2&lt;&gt;"","|"&amp;Y2,"")&amp;IF(Z2&lt;&gt;"","|"&amp;Z2,"")&amp;IF(AA2&lt;&gt;"","|"&amp;AA2,"")&amp;IF(AB2&lt;&gt;"","|"&amp;AB2,"")&amp;IF(AC2&lt;&gt;"","|"&amp;AC2,"")&amp;IF(AD2&lt;&gt;"","|"&amp;AD2,"")&amp;IF(AE2&lt;&gt;"","|"&amp;AE2,"")&amp;IF(AF2&lt;&gt;"","|"&amp;AF2,"")&amp;IF(AG2&lt;&gt;"","|"&amp;AG2,"")&amp;IF(AH2&lt;&gt;"","|"&amp;AH2,"")&amp;IF(AI2&lt;&gt;"","|"&amp;AI2,"")&amp;IF(AJ2&lt;&gt;"","|"&amp;AJ2,"")&amp;IF(AK2&lt;&gt;"","|"&amp;AK2,"")&amp;IF(AL2&lt;&gt;"","|"&amp;AL2,"")&amp;IF(AM2&lt;&gt;"","|"&amp;AM2,"")&amp;IF(AN2&lt;&gt;"","|"&amp;AN2,"")&amp;IF(AO2&lt;&gt;"","|"&amp;AO2,"")&amp;IF(AP2&lt;&gt;"","|"&amp;AP2,"")&amp;IF(AQ2&lt;&gt;"","|"&amp;AQ2,"")&amp;IF(AR2&lt;&gt;"","|"&amp;AR2,"")&amp;IF(AS2&lt;&gt;"","|"&amp;AS2,"")&amp;IF(AT2&lt;&gt;"","|"&amp;AT2,"")&amp;IF(AU2&lt;&gt;"","|"&amp;AU2,"")&amp;IF(AV2&lt;&gt;"","|"&amp;AV2,"")&amp;IF(AW2&lt;&gt;"","|"&amp;AW2,"")&amp;IF(AX2&lt;&gt;"","|"&amp;AX2,"")&amp;IF(AY2&lt;&gt;"","|"&amp;AY2,"")&amp;IF(AZ2&lt;&gt;"","|"&amp;AZ2,"")&amp;IF(BA2&lt;&gt;"","|"&amp;BA2,"")&amp;IF(BB2&lt;&gt;"","|"&amp;BB2,"")&amp;IF(BC2&lt;&gt;"","|"&amp;BC2,"")&amp;IF(BD2&lt;&gt;"","|"&amp;BD2,"")&amp;IF(BE2&lt;&gt;"","|"&amp;BE2,"")&amp;IF(BF2&lt;&gt;"","|"&amp;BF2,"")&amp;IF(BG2&lt;&gt;"","|"&amp;BG2,"")&amp;IF(BH2&lt;&gt;"","|"&amp;BH2,"")&amp;IF(BI2&lt;&gt;"","|"&amp;BI2,"")</f>
-        <v>You strike at your horrid enemy, using your knowledge of its strengths and weaknesses to twist the knife just a bit more.|You must be trained in Dungeoneering|Martial, Weapon|Dexterity vs AC|1[W] + Dexterity modifier (~DEXMod~). If the target is aberrant and has resistance or vulnerability to your attack, you gain a bonus to damage equal to your Wisdom modifier (~WISMod~).
-Level 21: 2[W] + Dexterity modifier (~DEXMod~).</v>
+        <v>You strike at your horrid enemy, using your knowledge of its strengths and weaknesses to twist the knife just a bit more.|You must be trained in Dungeoneering|Martial, Weapon|Dexterity vs AC|1[~W~] + Dexterity modifier (~DEXMod~) damage. If the target is aberrant and has resistance or vulnerability to your attack, you gain a bonus to damage equal to your Wisdom modifier (~WISMod~).
+Level 21: 2[~W~] + Dexterity modifier (~DEXMod~) damage.</v>
       </c>
       <c r="X2" t="s">
-        <v>2071</v>
+        <v>2068</v>
       </c>
       <c r="Z2" t="s">
-        <v>2078</v>
+        <v>2075</v>
       </c>
       <c r="AB2" t="s">
-        <v>2129</v>
+        <v>2126</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>2103</v>
+        <v>2100</v>
       </c>
       <c r="AE2" s="1" t="s">
-        <v>2130</v>
+        <v>2153</v>
       </c>
       <c r="AF2" s="1"/>
       <c r="AG2" s="1"/>
@@ -16840,7 +16923,7 @@
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2082</v>
+        <v>2079</v>
       </c>
       <c r="B3" t="s">
         <v>746</v>
@@ -16858,19 +16941,19 @@
         <v>1084</v>
       </c>
       <c r="G3" t="s">
-        <v>2074</v>
+        <v>2071</v>
       </c>
       <c r="H3" t="s">
-        <v>2134</v>
+        <v>2130</v>
       </c>
       <c r="I3" t="s">
         <v>752</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>2139</v>
+        <v>2151</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>2138</v>
+        <v>2133</v>
       </c>
       <c r="L3" t="s">
         <v>758</v>
@@ -16879,7 +16962,7 @@
         <v>20</v>
       </c>
       <c r="N3" t="s">
-        <v>2102</v>
+        <v>2099</v>
       </c>
       <c r="V3" s="3" t="str">
         <f>IF(X3&lt;&gt;"",$X$1,"")&amp;IF(Y3&lt;&gt;"","|"&amp;$Y$1,"")&amp;IF(Z3&lt;&gt;"","|"&amp;$Z$1,"")&amp;IF(AA3&lt;&gt;"","|"&amp;$AA$1,"")&amp;IF(AB3&lt;&gt;"","|"&amp;$AB$1,"")&amp;IF(AC3&lt;&gt;"","|"&amp;$AC$1,"")&amp;IF(AD3&lt;&gt;"","|"&amp;$AD$1,"")&amp;IF(AE3&lt;&gt;"","|"&amp;$AE$1,"")&amp;IF(AF3&lt;&gt;"","|"&amp;$AF$1,"")&amp;IF(AG3&lt;&gt;"","|"&amp;$AG$1,"")&amp;IF(AH3&lt;&gt;"","|"&amp;$AH$1,"")&amp;IF(AI3&lt;&gt;"","|"&amp;$AI$1,"")&amp;IF(AJ3&lt;&gt;"","|"&amp;$AJ$1,"")&amp;IF(AK3&lt;&gt;"","|"&amp;$AK$1,"")&amp;IF(AL3&lt;&gt;"","|"&amp;$AL$1,"")&amp;IF(AM3&lt;&gt;"","|"&amp;$AM$1,"")&amp;IF(AN3&lt;&gt;"","|"&amp;$AN$1,"")&amp;IF(AO3&lt;&gt;"","|"&amp;$AO$1,"")&amp;IF(AP3&lt;&gt;"","|"&amp;$AP$1,"")&amp;IF(AQ3&lt;&gt;"","|"&amp;$AQ$1,"")&amp;IF(AR3&lt;&gt;"","|"&amp;$AR$1,"")&amp;IF(AS3&lt;&gt;"","|"&amp;$AS$1,"")&amp;IF(AT3&lt;&gt;"","|"&amp;$AT$1,"")&amp;IF(AU3&lt;&gt;"","|"&amp;$AU$1,"")&amp;IF(AV3&lt;&gt;"","|"&amp;$AV$1,"")&amp;IF(AW3&lt;&gt;"","|"&amp;$AW$1,"")&amp;IF(AX3&lt;&gt;"","|"&amp;$AX$1,"")&amp;IF(AY3&lt;&gt;"","|"&amp;$AY$1,"")&amp;IF(AZ3&lt;&gt;"","|"&amp;$AZ$1,"")&amp;IF(BA3&lt;&gt;"","|"&amp;$BA$1,"")&amp;IF(BB3&lt;&gt;"","|"&amp;$BB$1,"")&amp;IF(BC3&lt;&gt;"","|"&amp;$BC$1,"")&amp;IF(BD3&lt;&gt;"","|"&amp;$BD$1,"")&amp;IF(BE3&lt;&gt;"","|"&amp;$BE$1,"")&amp;IF(BF3&lt;&gt;"","|"&amp;$BF$1,"")&amp;IF(BG3&lt;&gt;"","|"&amp;$BG$1,"")&amp;IF(BH3&lt;&gt;"","|"&amp;$BH$1,"")&amp;IF(BI3&lt;&gt;"","|"&amp;$BI$1,"")</f>
@@ -16891,13 +16974,13 @@
 Level 21: 2d10 + Charisma modifier (~CHAMod~) acid damage.</v>
       </c>
       <c r="AB3" t="s">
-        <v>2128</v>
+        <v>2125</v>
       </c>
       <c r="AD3" s="3" t="s">
-        <v>2104</v>
+        <v>2101</v>
       </c>
       <c r="AE3" s="1" t="s">
-        <v>2131</v>
+        <v>2127</v>
       </c>
       <c r="AF3" s="1"/>
       <c r="AG3" s="1"/>
@@ -16911,10 +16994,10 @@
     </row>
     <row r="4" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2083</v>
+        <v>2080</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1774</v>
+        <v>1773</v>
       </c>
       <c r="C4" t="s">
         <v>731</v>
@@ -16923,19 +17006,19 @@
         <v>265</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>2090</v>
+        <v>2087</v>
       </c>
       <c r="F4" t="s">
         <v>1084</v>
       </c>
       <c r="G4" t="s">
-        <v>2085</v>
+        <v>2082</v>
       </c>
       <c r="L4" t="s">
-        <v>2086</v>
+        <v>2083</v>
       </c>
       <c r="O4" t="s">
-        <v>2083</v>
+        <v>2080</v>
       </c>
       <c r="P4" t="s">
         <v>265</v>
@@ -16951,13 +17034,13 @@
 Level 21: +6 power bonus.</v>
       </c>
       <c r="Z4" t="s">
-        <v>2084</v>
+        <v>2081</v>
       </c>
       <c r="AB4" t="s">
         <v>711</v>
       </c>
       <c r="AI4" s="1" t="s">
-        <v>2087</v>
+        <v>2084</v>
       </c>
       <c r="AQ4" s="3"/>
       <c r="AR4" s="3"/>
@@ -16968,10 +17051,10 @@
     </row>
     <row r="5" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2088</v>
+        <v>2085</v>
       </c>
       <c r="B5" t="s">
-        <v>2089</v>
+        <v>2086</v>
       </c>
       <c r="C5" t="s">
         <v>731</v>
@@ -16986,19 +17069,19 @@
         <v>1084</v>
       </c>
       <c r="G5" t="s">
-        <v>2074</v>
+        <v>2071</v>
       </c>
       <c r="H5" t="s">
+        <v>2129</v>
+      </c>
+      <c r="I5" t="s">
+        <v>2078</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>2152</v>
+      </c>
+      <c r="K5" s="3" t="s">
         <v>2133</v>
-      </c>
-      <c r="I5" t="s">
-        <v>2081</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>2137</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>2138</v>
       </c>
       <c r="L5" t="s">
         <v>757</v>
@@ -17007,19 +17090,19 @@
         <v>780</v>
       </c>
       <c r="N5" t="s">
-        <v>2102</v>
+        <v>2099</v>
       </c>
       <c r="O5" t="s">
-        <v>2093</v>
+        <v>2090</v>
       </c>
       <c r="P5" t="s">
         <v>1083</v>
       </c>
       <c r="Q5" t="s">
-        <v>2092</v>
+        <v>2089</v>
       </c>
       <c r="R5" t="s">
-        <v>2075</v>
+        <v>2072</v>
       </c>
       <c r="V5" s="3" t="str">
         <f>IF(X5&lt;&gt;"",$X$1,"")&amp;IF(Y5&lt;&gt;"","|"&amp;$Y$1,"")&amp;IF(Z5&lt;&gt;"","|"&amp;$Z$1,"")&amp;IF(AA5&lt;&gt;"","|"&amp;$AA$1,"")&amp;IF(AB5&lt;&gt;"","|"&amp;$AB$1,"")&amp;IF(AC5&lt;&gt;"","|"&amp;$AC$1,"")&amp;IF(AD5&lt;&gt;"","|"&amp;$AD$1,"")&amp;IF(AE5&lt;&gt;"","|"&amp;$AE$1,"")&amp;IF(AF5&lt;&gt;"","|"&amp;$AF$1,"")&amp;IF(AG5&lt;&gt;"","|"&amp;$AG$1,"")&amp;IF(AH5&lt;&gt;"","|"&amp;$AH$1,"")&amp;IF(AI5&lt;&gt;"","|"&amp;$AI$1,"")&amp;IF(AJ5&lt;&gt;"","|"&amp;$AJ$1,"")&amp;IF(AK5&lt;&gt;"","|"&amp;$AK$1,"")&amp;IF(AL5&lt;&gt;"","|"&amp;$AL$1,"")&amp;IF(AM5&lt;&gt;"","|"&amp;$AM$1,"")&amp;IF(AN5&lt;&gt;"","|"&amp;$AN$1,"")&amp;IF(AO5&lt;&gt;"","|"&amp;$AO$1,"")&amp;IF(AP5&lt;&gt;"","|"&amp;$AP$1,"")&amp;IF(AQ5&lt;&gt;"","|"&amp;$AQ$1,"")&amp;IF(AR5&lt;&gt;"","|"&amp;$AR$1,"")&amp;IF(AS5&lt;&gt;"","|"&amp;$AS$1,"")&amp;IF(AT5&lt;&gt;"","|"&amp;$AT$1,"")&amp;IF(AU5&lt;&gt;"","|"&amp;$AU$1,"")&amp;IF(AV5&lt;&gt;"","|"&amp;$AV$1,"")&amp;IF(AW5&lt;&gt;"","|"&amp;$AW$1,"")&amp;IF(AX5&lt;&gt;"","|"&amp;$AX$1,"")&amp;IF(AY5&lt;&gt;"","|"&amp;$AY$1,"")&amp;IF(AZ5&lt;&gt;"","|"&amp;$AZ$1,"")&amp;IF(BA5&lt;&gt;"","|"&amp;$BA$1,"")&amp;IF(BB5&lt;&gt;"","|"&amp;$BB$1,"")&amp;IF(BC5&lt;&gt;"","|"&amp;$BC$1,"")&amp;IF(BD5&lt;&gt;"","|"&amp;$BD$1,"")&amp;IF(BE5&lt;&gt;"","|"&amp;$BE$1,"")&amp;IF(BF5&lt;&gt;"","|"&amp;$BF$1,"")&amp;IF(BG5&lt;&gt;"","|"&amp;$BG$1,"")&amp;IF(BH5&lt;&gt;"","|"&amp;$BH$1,"")&amp;IF(BI5&lt;&gt;"","|"&amp;$BI$1,"")</f>
@@ -17031,28 +17114,28 @@
 Level 21: 2[W] + Dexterity modifier (~DEXMod~) damage.|Before or after the attack, you shift 1 square.</v>
       </c>
       <c r="X5" t="s">
-        <v>2071</v>
+        <v>2068</v>
       </c>
       <c r="Z5" t="s">
-        <v>2094</v>
+        <v>2091</v>
       </c>
       <c r="AA5" s="3" t="s">
-        <v>2096</v>
+        <v>2093</v>
       </c>
       <c r="AB5" t="s">
-        <v>2129</v>
+        <v>2126</v>
       </c>
       <c r="AD5" s="3" t="s">
-        <v>2103</v>
+        <v>2100</v>
       </c>
       <c r="AE5" s="1" t="s">
-        <v>2132</v>
+        <v>2128</v>
       </c>
       <c r="AF5" s="1"/>
       <c r="AG5" s="1"/>
       <c r="AH5" s="1"/>
       <c r="AI5" s="1" t="s">
-        <v>2097</v>
+        <v>2094</v>
       </c>
       <c r="AQ5" s="3"/>
       <c r="AR5" s="3"/>
@@ -17063,6 +17146,45 @@
     </row>
     <row r="6" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>2134</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1782</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>739</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1084</v>
+      </c>
+      <c r="G6" t="s">
+        <v>2136</v>
+      </c>
+      <c r="L6" t="s">
+        <v>2137</v>
+      </c>
+      <c r="M6" s="3">
+        <v>2</v>
+      </c>
+      <c r="N6" t="s">
+        <v>2138</v>
+      </c>
+      <c r="U6" s="3" t="s">
+        <v>2139</v>
+      </c>
+      <c r="V6" s="3" t="str">
+        <f>IF(X6&lt;&gt;"",$X$1,"")&amp;IF(Y6&lt;&gt;"","|"&amp;$Y$1,"")&amp;IF(Z6&lt;&gt;"","|"&amp;$Z$1,"")&amp;IF(AA6&lt;&gt;"","|"&amp;$AA$1,"")&amp;IF(AB6&lt;&gt;"","|"&amp;$AB$1,"")&amp;IF(AC6&lt;&gt;"","|"&amp;$AC$1,"")&amp;IF(AD6&lt;&gt;"","|"&amp;$AD$1,"")&amp;IF(AE6&lt;&gt;"","|"&amp;$AE$1,"")&amp;IF(AF6&lt;&gt;"","|"&amp;$AF$1,"")&amp;IF(AG6&lt;&gt;"","|"&amp;$AG$1,"")&amp;IF(AH6&lt;&gt;"","|"&amp;$AH$1,"")&amp;IF(AI6&lt;&gt;"","|"&amp;$AI$1,"")&amp;IF(AJ6&lt;&gt;"","|"&amp;$AJ$1,"")&amp;IF(AK6&lt;&gt;"","|"&amp;$AK$1,"")&amp;IF(AL6&lt;&gt;"","|"&amp;$AL$1,"")&amp;IF(AM6&lt;&gt;"","|"&amp;$AM$1,"")&amp;IF(AN6&lt;&gt;"","|"&amp;$AN$1,"")&amp;IF(AO6&lt;&gt;"","|"&amp;$AO$1,"")&amp;IF(AP6&lt;&gt;"","|"&amp;$AP$1,"")&amp;IF(AQ6&lt;&gt;"","|"&amp;$AQ$1,"")&amp;IF(AR6&lt;&gt;"","|"&amp;$AR$1,"")&amp;IF(AS6&lt;&gt;"","|"&amp;$AS$1,"")&amp;IF(AT6&lt;&gt;"","|"&amp;$AT$1,"")&amp;IF(AU6&lt;&gt;"","|"&amp;$AU$1,"")&amp;IF(AV6&lt;&gt;"","|"&amp;$AV$1,"")&amp;IF(AW6&lt;&gt;"","|"&amp;$AW$1,"")&amp;IF(AX6&lt;&gt;"","|"&amp;$AX$1,"")&amp;IF(AY6&lt;&gt;"","|"&amp;$AY$1,"")&amp;IF(AZ6&lt;&gt;"","|"&amp;$AZ$1,"")&amp;IF(BA6&lt;&gt;"","|"&amp;$BA$1,"")&amp;IF(BB6&lt;&gt;"","|"&amp;$BB$1,"")&amp;IF(BC6&lt;&gt;"","|"&amp;$BC$1,"")&amp;IF(BD6&lt;&gt;"","|"&amp;$BD$1,"")&amp;IF(BE6&lt;&gt;"","|"&amp;$BE$1,"")&amp;IF(BF6&lt;&gt;"","|"&amp;$BF$1,"")&amp;IF(BG6&lt;&gt;"","|"&amp;$BG$1,"")&amp;IF(BH6&lt;&gt;"","|"&amp;$BH$1,"")&amp;IF(BI6&lt;&gt;"","|"&amp;$BI$1,"")</f>
+        <v>|Effect:</v>
+      </c>
+      <c r="W6" s="3" t="str">
+        <f>IF(X6&lt;&gt;"",X6,"")&amp;IF(Y6&lt;&gt;"","|"&amp;Y6,"")&amp;IF(Z6&lt;&gt;"","|"&amp;Z6,"")&amp;IF(AA6&lt;&gt;"","|"&amp;AA6,"")&amp;IF(AB6&lt;&gt;"","|"&amp;AB6,"")&amp;IF(AC6&lt;&gt;"","|"&amp;AC6,"")&amp;IF(AD6&lt;&gt;"","|"&amp;AD6,"")&amp;IF(AE6&lt;&gt;"","|"&amp;AE6,"")&amp;IF(AF6&lt;&gt;"","|"&amp;AF6,"")&amp;IF(AG6&lt;&gt;"","|"&amp;AG6,"")&amp;IF(AH6&lt;&gt;"","|"&amp;AH6,"")&amp;IF(AI6&lt;&gt;"","|"&amp;AI6,"")&amp;IF(AJ6&lt;&gt;"","|"&amp;AJ6,"")&amp;IF(AK6&lt;&gt;"","|"&amp;AK6,"")&amp;IF(AL6&lt;&gt;"","|"&amp;AL6,"")&amp;IF(AM6&lt;&gt;"","|"&amp;AM6,"")&amp;IF(AN6&lt;&gt;"","|"&amp;AN6,"")&amp;IF(AO6&lt;&gt;"","|"&amp;AO6,"")&amp;IF(AP6&lt;&gt;"","|"&amp;AP6,"")&amp;IF(AQ6&lt;&gt;"","|"&amp;AQ6,"")&amp;IF(AR6&lt;&gt;"","|"&amp;AR6,"")&amp;IF(AS6&lt;&gt;"","|"&amp;AS6,"")&amp;IF(AT6&lt;&gt;"","|"&amp;AT6,"")&amp;IF(AU6&lt;&gt;"","|"&amp;AU6,"")&amp;IF(AV6&lt;&gt;"","|"&amp;AV6,"")&amp;IF(AW6&lt;&gt;"","|"&amp;AW6,"")&amp;IF(AX6&lt;&gt;"","|"&amp;AX6,"")&amp;IF(AY6&lt;&gt;"","|"&amp;AY6,"")&amp;IF(AZ6&lt;&gt;"","|"&amp;AZ6,"")&amp;IF(BA6&lt;&gt;"","|"&amp;BA6,"")&amp;IF(BB6&lt;&gt;"","|"&amp;BB6,"")&amp;IF(BC6&lt;&gt;"","|"&amp;BC6,"")&amp;IF(BD6&lt;&gt;"","|"&amp;BD6,"")&amp;IF(BE6&lt;&gt;"","|"&amp;BE6,"")&amp;IF(BF6&lt;&gt;"","|"&amp;BF6,"")&amp;IF(BG6&lt;&gt;"","|"&amp;BG6,"")&amp;IF(BH6&lt;&gt;"","|"&amp;BH6,"")&amp;IF(BI6&lt;&gt;"","|"&amp;BI6,"")</f>
+        <v>|You mark the target. The target remains marked until you use this power against another target. If you mark other creatures using other powers, the target is still marked. A creature can be subject to only one mark at a time. A new mark supersedes a mark that was already in place.
+If your marked target makes an attack that doesn't include you as a target, it takes a −2 penalty to attack rolls. If that attack hits and the marked target is within 10 squares of you, you can use an immediate reaction to teleport to a square adjacent to the target and make a melee basic attack against it. If no unoccupied space exists adjacent to the target, you can't use this immediate reaction.</v>
+      </c>
+      <c r="AI6" s="1" t="s">
         <v>2140</v>
       </c>
       <c r="AQ6" s="3"/>
@@ -17073,6 +17195,46 @@
       <c r="AV6" s="3"/>
     </row>
     <row r="7" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>2141</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2142</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>739</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1084</v>
+      </c>
+      <c r="G7" t="s">
+        <v>2136</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>2137</v>
+      </c>
+      <c r="M7" s="3">
+        <v>2</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>2138</v>
+      </c>
+      <c r="V7" s="3" t="str">
+        <f>IF(X7&lt;&gt;"",$X$1,"")&amp;IF(Y7&lt;&gt;"","|"&amp;$Y$1,"")&amp;IF(Z7&lt;&gt;"","|"&amp;$Z$1,"")&amp;IF(AA7&lt;&gt;"","|"&amp;$AA$1,"")&amp;IF(AB7&lt;&gt;"","|"&amp;$AB$1,"")&amp;IF(AC7&lt;&gt;"","|"&amp;$AC$1,"")&amp;IF(AD7&lt;&gt;"","|"&amp;$AD$1,"")&amp;IF(AE7&lt;&gt;"","|"&amp;$AE$1,"")&amp;IF(AF7&lt;&gt;"","|"&amp;$AF$1,"")&amp;IF(AG7&lt;&gt;"","|"&amp;$AG$1,"")&amp;IF(AH7&lt;&gt;"","|"&amp;$AH$1,"")&amp;IF(AI7&lt;&gt;"","|"&amp;$AI$1,"")&amp;IF(AJ7&lt;&gt;"","|"&amp;$AJ$1,"")&amp;IF(AK7&lt;&gt;"","|"&amp;$AK$1,"")&amp;IF(AL7&lt;&gt;"","|"&amp;$AL$1,"")&amp;IF(AM7&lt;&gt;"","|"&amp;$AM$1,"")&amp;IF(AN7&lt;&gt;"","|"&amp;$AN$1,"")&amp;IF(AO7&lt;&gt;"","|"&amp;$AO$1,"")&amp;IF(AP7&lt;&gt;"","|"&amp;$AP$1,"")&amp;IF(AQ7&lt;&gt;"","|"&amp;$AQ$1,"")&amp;IF(AR7&lt;&gt;"","|"&amp;$AR$1,"")&amp;IF(AS7&lt;&gt;"","|"&amp;$AS$1,"")&amp;IF(AT7&lt;&gt;"","|"&amp;$AT$1,"")&amp;IF(AU7&lt;&gt;"","|"&amp;$AU$1,"")&amp;IF(AV7&lt;&gt;"","|"&amp;$AV$1,"")&amp;IF(AW7&lt;&gt;"","|"&amp;$AW$1,"")&amp;IF(AX7&lt;&gt;"","|"&amp;$AX$1,"")&amp;IF(AY7&lt;&gt;"","|"&amp;$AY$1,"")&amp;IF(AZ7&lt;&gt;"","|"&amp;$AZ$1,"")&amp;IF(BA7&lt;&gt;"","|"&amp;$BA$1,"")&amp;IF(BB7&lt;&gt;"","|"&amp;$BB$1,"")&amp;IF(BC7&lt;&gt;"","|"&amp;$BC$1,"")&amp;IF(BD7&lt;&gt;"","|"&amp;$BD$1,"")&amp;IF(BE7&lt;&gt;"","|"&amp;$BE$1,"")&amp;IF(BF7&lt;&gt;"","|"&amp;$BF$1,"")&amp;IF(BG7&lt;&gt;"","|"&amp;$BG$1,"")&amp;IF(BH7&lt;&gt;"","|"&amp;$BH$1,"")&amp;IF(BI7&lt;&gt;"","|"&amp;$BI$1,"")</f>
+        <v>|Effect:</v>
+      </c>
+      <c r="W7" s="3" t="str">
+        <f>IF(X7&lt;&gt;"",X7,"")&amp;IF(Y7&lt;&gt;"","|"&amp;Y7,"")&amp;IF(Z7&lt;&gt;"","|"&amp;Z7,"")&amp;IF(AA7&lt;&gt;"","|"&amp;AA7,"")&amp;IF(AB7&lt;&gt;"","|"&amp;AB7,"")&amp;IF(AC7&lt;&gt;"","|"&amp;AC7,"")&amp;IF(AD7&lt;&gt;"","|"&amp;AD7,"")&amp;IF(AE7&lt;&gt;"","|"&amp;AE7,"")&amp;IF(AF7&lt;&gt;"","|"&amp;AF7,"")&amp;IF(AG7&lt;&gt;"","|"&amp;AG7,"")&amp;IF(AH7&lt;&gt;"","|"&amp;AH7,"")&amp;IF(AI7&lt;&gt;"","|"&amp;AI7,"")&amp;IF(AJ7&lt;&gt;"","|"&amp;AJ7,"")&amp;IF(AK7&lt;&gt;"","|"&amp;AK7,"")&amp;IF(AL7&lt;&gt;"","|"&amp;AL7,"")&amp;IF(AM7&lt;&gt;"","|"&amp;AM7,"")&amp;IF(AN7&lt;&gt;"","|"&amp;AN7,"")&amp;IF(AO7&lt;&gt;"","|"&amp;AO7,"")&amp;IF(AP7&lt;&gt;"","|"&amp;AP7,"")&amp;IF(AQ7&lt;&gt;"","|"&amp;AQ7,"")&amp;IF(AR7&lt;&gt;"","|"&amp;AR7,"")&amp;IF(AS7&lt;&gt;"","|"&amp;AS7,"")&amp;IF(AT7&lt;&gt;"","|"&amp;AT7,"")&amp;IF(AU7&lt;&gt;"","|"&amp;AU7,"")&amp;IF(AV7&lt;&gt;"","|"&amp;AV7,"")&amp;IF(AW7&lt;&gt;"","|"&amp;AW7,"")&amp;IF(AX7&lt;&gt;"","|"&amp;AX7,"")&amp;IF(AY7&lt;&gt;"","|"&amp;AY7,"")&amp;IF(AZ7&lt;&gt;"","|"&amp;AZ7,"")&amp;IF(BA7&lt;&gt;"","|"&amp;BA7,"")&amp;IF(BB7&lt;&gt;"","|"&amp;BB7,"")&amp;IF(BC7&lt;&gt;"","|"&amp;BC7,"")&amp;IF(BD7&lt;&gt;"","|"&amp;BD7,"")&amp;IF(BE7&lt;&gt;"","|"&amp;BE7,"")&amp;IF(BF7&lt;&gt;"","|"&amp;BF7,"")&amp;IF(BG7&lt;&gt;"","|"&amp;BG7,"")&amp;IF(BH7&lt;&gt;"","|"&amp;BH7,"")&amp;IF(BI7&lt;&gt;"","|"&amp;BI7,"")</f>
+        <v>|You mark the target. The target remains marked until you use this power against another target. If you mark another creature using other powers, the target is still marked.
+Until the mark ends, if the target makes any attack that does not include you as a target, it takes a −2 penalty to the attack roll.
+If a target marked by this power is within 10 squares of you when it hits with an attack that does not include you as a target, you can use an immediate reaction after the target's entire attack is resolved to teleport the target to any space adjacent to you. In addition, the target grants combat advantage to all creatures until the end of your next turn. If no unoccupied space exists adjacent to you, you can't use this immediate reaction, and the target doesn't grant combat advantage as a result of this effect.</v>
+      </c>
+      <c r="AI7" s="1" t="s">
+        <v>2145</v>
+      </c>
       <c r="AQ7" s="3"/>
       <c r="AR7" s="3"/>
       <c r="AS7" s="3"/>
@@ -17080,14 +17242,102 @@
       <c r="AU7" s="3"/>
       <c r="AV7" s="3"/>
     </row>
+    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>2146</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1782</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>739</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1084</v>
+      </c>
+      <c r="G8" t="s">
+        <v>2136</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>2137</v>
+      </c>
+      <c r="M8" s="3">
+        <v>2</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>2138</v>
+      </c>
+      <c r="V8" s="3" t="str">
+        <f>IF(X8&lt;&gt;"",$X$1,"")&amp;IF(Y8&lt;&gt;"","|"&amp;$Y$1,"")&amp;IF(Z8&lt;&gt;"","|"&amp;$Z$1,"")&amp;IF(AA8&lt;&gt;"","|"&amp;$AA$1,"")&amp;IF(AB8&lt;&gt;"","|"&amp;$AB$1,"")&amp;IF(AC8&lt;&gt;"","|"&amp;$AC$1,"")&amp;IF(AD8&lt;&gt;"","|"&amp;$AD$1,"")&amp;IF(AE8&lt;&gt;"","|"&amp;$AE$1,"")&amp;IF(AF8&lt;&gt;"","|"&amp;$AF$1,"")&amp;IF(AG8&lt;&gt;"","|"&amp;$AG$1,"")&amp;IF(AH8&lt;&gt;"","|"&amp;$AH$1,"")&amp;IF(AI8&lt;&gt;"","|"&amp;$AI$1,"")&amp;IF(AJ8&lt;&gt;"","|"&amp;$AJ$1,"")&amp;IF(AK8&lt;&gt;"","|"&amp;$AK$1,"")&amp;IF(AL8&lt;&gt;"","|"&amp;$AL$1,"")&amp;IF(AM8&lt;&gt;"","|"&amp;$AM$1,"")&amp;IF(AN8&lt;&gt;"","|"&amp;$AN$1,"")&amp;IF(AO8&lt;&gt;"","|"&amp;$AO$1,"")&amp;IF(AP8&lt;&gt;"","|"&amp;$AP$1,"")&amp;IF(AQ8&lt;&gt;"","|"&amp;$AQ$1,"")&amp;IF(AR8&lt;&gt;"","|"&amp;$AR$1,"")&amp;IF(AS8&lt;&gt;"","|"&amp;$AS$1,"")&amp;IF(AT8&lt;&gt;"","|"&amp;$AT$1,"")&amp;IF(AU8&lt;&gt;"","|"&amp;$AU$1,"")&amp;IF(AV8&lt;&gt;"","|"&amp;$AV$1,"")&amp;IF(AW8&lt;&gt;"","|"&amp;$AW$1,"")&amp;IF(AX8&lt;&gt;"","|"&amp;$AX$1,"")&amp;IF(AY8&lt;&gt;"","|"&amp;$AY$1,"")&amp;IF(AZ8&lt;&gt;"","|"&amp;$AZ$1,"")&amp;IF(BA8&lt;&gt;"","|"&amp;$BA$1,"")&amp;IF(BB8&lt;&gt;"","|"&amp;$BB$1,"")&amp;IF(BC8&lt;&gt;"","|"&amp;$BC$1,"")&amp;IF(BD8&lt;&gt;"","|"&amp;$BD$1,"")&amp;IF(BE8&lt;&gt;"","|"&amp;$BE$1,"")&amp;IF(BF8&lt;&gt;"","|"&amp;$BF$1,"")&amp;IF(BG8&lt;&gt;"","|"&amp;$BG$1,"")&amp;IF(BH8&lt;&gt;"","|"&amp;$BH$1,"")&amp;IF(BI8&lt;&gt;"","|"&amp;$BI$1,"")</f>
+        <v>|Effect:</v>
+      </c>
+      <c r="W8" s="3" t="str">
+        <f>IF(X8&lt;&gt;"",X8,"")&amp;IF(Y8&lt;&gt;"","|"&amp;Y8,"")&amp;IF(Z8&lt;&gt;"","|"&amp;Z8,"")&amp;IF(AA8&lt;&gt;"","|"&amp;AA8,"")&amp;IF(AB8&lt;&gt;"","|"&amp;AB8,"")&amp;IF(AC8&lt;&gt;"","|"&amp;AC8,"")&amp;IF(AD8&lt;&gt;"","|"&amp;AD8,"")&amp;IF(AE8&lt;&gt;"","|"&amp;AE8,"")&amp;IF(AF8&lt;&gt;"","|"&amp;AF8,"")&amp;IF(AG8&lt;&gt;"","|"&amp;AG8,"")&amp;IF(AH8&lt;&gt;"","|"&amp;AH8,"")&amp;IF(AI8&lt;&gt;"","|"&amp;AI8,"")&amp;IF(AJ8&lt;&gt;"","|"&amp;AJ8,"")&amp;IF(AK8&lt;&gt;"","|"&amp;AK8,"")&amp;IF(AL8&lt;&gt;"","|"&amp;AL8,"")&amp;IF(AM8&lt;&gt;"","|"&amp;AM8,"")&amp;IF(AN8&lt;&gt;"","|"&amp;AN8,"")&amp;IF(AO8&lt;&gt;"","|"&amp;AO8,"")&amp;IF(AP8&lt;&gt;"","|"&amp;AP8,"")&amp;IF(AQ8&lt;&gt;"","|"&amp;AQ8,"")&amp;IF(AR8&lt;&gt;"","|"&amp;AR8,"")&amp;IF(AS8&lt;&gt;"","|"&amp;AS8,"")&amp;IF(AT8&lt;&gt;"","|"&amp;AT8,"")&amp;IF(AU8&lt;&gt;"","|"&amp;AU8,"")&amp;IF(AV8&lt;&gt;"","|"&amp;AV8,"")&amp;IF(AW8&lt;&gt;"","|"&amp;AW8,"")&amp;IF(AX8&lt;&gt;"","|"&amp;AX8,"")&amp;IF(AY8&lt;&gt;"","|"&amp;AY8,"")&amp;IF(AZ8&lt;&gt;"","|"&amp;AZ8,"")&amp;IF(BA8&lt;&gt;"","|"&amp;BA8,"")&amp;IF(BB8&lt;&gt;"","|"&amp;BB8,"")&amp;IF(BC8&lt;&gt;"","|"&amp;BC8,"")&amp;IF(BD8&lt;&gt;"","|"&amp;BD8,"")&amp;IF(BE8&lt;&gt;"","|"&amp;BE8,"")&amp;IF(BF8&lt;&gt;"","|"&amp;BF8,"")&amp;IF(BG8&lt;&gt;"","|"&amp;BG8,"")&amp;IF(BH8&lt;&gt;"","|"&amp;BH8,"")&amp;IF(BI8&lt;&gt;"","|"&amp;BI8,"")</f>
+        <v>|You mark the target. The target remains marked until you use this power against another target. If you mark other creatures using other powers, the target is still marked. A creature can be subject to only one mark at a time. A new mark supersedes a mark that was already in place.
+     If your marked target makes an attack that doesn't include you as a target, it takes a −2 penalty to attack rolls. If that attack hits and the marked target is within 10 squares of you, you can use an immediate interrupt to reduce the damage dealt by that attack to any one creature by an amount equal to 5 + your Constitution modifier (~CONMod~).
+At 11th level, reduce the damage dealt by 10 + your Constitution modifier (~CONMod~). At 21st level, reduce the damage dealt by 15 + your Constitution modifier (~CONMod~).</v>
+      </c>
+      <c r="AI8" s="1" t="s">
+        <v>2147</v>
+      </c>
+    </row>
     <row r="9" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>2148</v>
+      </c>
+      <c r="B9" t="s">
+        <v>697</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>713</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>754</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1084</v>
+      </c>
+      <c r="G9" t="s">
+        <v>2071</v>
+      </c>
+      <c r="H9" t="s">
+        <v>2149</v>
+      </c>
+      <c r="I9" t="s">
+        <v>2150</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>2154</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>2133</v>
+      </c>
+      <c r="L9" t="s">
+        <v>2098</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>2105</v>
+      </c>
+      <c r="N9" t="s">
+        <v>2099</v>
+      </c>
       <c r="O9" s="3"/>
       <c r="Y9"/>
       <c r="Z9" s="3"/>
       <c r="AA9"/>
       <c r="AB9" s="3"/>
-      <c r="AD9"/>
-      <c r="AE9" s="3"/>
+      <c r="AD9" t="s">
+        <v>2155</v>
+      </c>
+      <c r="AE9" s="1" t="s">
+        <v>2156</v>
+      </c>
       <c r="AH9"/>
       <c r="AJ9" s="3"/>
       <c r="AP9"/>
@@ -17612,7 +17862,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="X26" sqref="X26"/>
+      <selection activeCell="Z21" sqref="Z21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17631,8 +17881,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17814,7 +18067,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2099</v>
+        <v>2096</v>
       </c>
     </row>
   </sheetData>
@@ -17825,10 +18078,13 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17855,10 +18111,10 @@
         <v>678</v>
       </c>
       <c r="B2" t="s">
-        <v>1788</v>
+        <v>2143</v>
       </c>
       <c r="D2" t="s">
-        <v>1789</v>
+        <v>2144</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -17905,11 +18161,6 @@
       </c>
       <c r="B7" t="s">
         <v>1614</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
-        <v>1685</v>
       </c>
     </row>
   </sheetData>
@@ -17942,10 +18193,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2062</v>
+        <v>2059</v>
       </c>
       <c r="E1" t="s">
-        <v>2063</v>
+        <v>2060</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -17953,16 +18204,16 @@
         <v>961</v>
       </c>
       <c r="B2" t="s">
-        <v>2061</v>
+        <v>2058</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>2068</v>
+        <v>2065</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>2069</v>
+        <v>2066</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>2066</v>
+        <v>2063</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -17973,7 +18224,7 @@
         <v>1023</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>2065</v>
+        <v>2062</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -17984,7 +18235,7 @@
         <v>1024</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>2064</v>
+        <v>2061</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -17995,7 +18246,7 @@
         <v>1025</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>2067</v>
+        <v>2064</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -18025,7 +18276,10 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18107,7 +18361,10 @@
   <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18198,7 +18455,7 @@
         <v>1144</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>1771</v>
+        <v>1770</v>
       </c>
       <c r="D4" t="s">
         <v>705</v>
@@ -18244,7 +18501,7 @@
         <v>1145</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>1772</v>
+        <v>1771</v>
       </c>
       <c r="D6" t="s">
         <v>705</v>
@@ -18267,7 +18524,7 @@
         <v>1146</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>1772</v>
+        <v>1771</v>
       </c>
       <c r="D7" t="s">
         <v>703</v>
@@ -18310,10 +18567,10 @@
         <v>719</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>1765</v>
+        <v>1764</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>1778</v>
+        <v>1777</v>
       </c>
       <c r="D9" t="s">
         <v>703</v>
@@ -18333,7 +18590,7 @@
         <v>1147</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>1779</v>
+        <v>1778</v>
       </c>
       <c r="D10" t="s">
         <v>703</v>
@@ -18353,10 +18610,10 @@
         <v>721</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>1770</v>
+        <v>1769</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>1778</v>
+        <v>1777</v>
       </c>
       <c r="D11" t="s">
         <v>708</v>
@@ -18425,7 +18682,7 @@
         <v>1148</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>1780</v>
+        <v>1779</v>
       </c>
       <c r="D14" t="s">
         <v>708</v>
@@ -18468,7 +18725,7 @@
         <v>1149</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>1781</v>
+        <v>1780</v>
       </c>
       <c r="D16" t="s">
         <v>705</v>
@@ -18488,10 +18745,10 @@
         <v>731</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>1768</v>
+        <v>1767</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>1778</v>
+        <v>1777</v>
       </c>
       <c r="D17" t="s">
         <v>705</v>
@@ -18580,7 +18837,7 @@
         <v>1150</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>1782</v>
+        <v>1781</v>
       </c>
       <c r="D21" t="s">
         <v>705</v>
@@ -18603,7 +18860,7 @@
         <v>739</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>1783</v>
+        <v>1782</v>
       </c>
       <c r="D22" t="s">
         <v>708</v>
@@ -18623,7 +18880,7 @@
         <v>828</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>1775</v>
+        <v>1774</v>
       </c>
       <c r="D23" t="s">
         <v>705</v>
@@ -18666,7 +18923,7 @@
         <v>1151</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>1780</v>
+        <v>1779</v>
       </c>
       <c r="D25" t="s">
         <v>705</v>
@@ -18689,7 +18946,7 @@
         <v>743</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>1784</v>
+        <v>1783</v>
       </c>
       <c r="D26" t="s">
         <v>703</v>
@@ -18709,7 +18966,7 @@
         <v>1152</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>1785</v>
+        <v>1784</v>
       </c>
       <c r="D27" t="s">
         <v>710</v>
@@ -18718,7 +18975,7 @@
         <v>1070</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>1700</v>
+        <v>1699</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -18776,15 +19033,15 @@
   <dimension ref="A1:BH49"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AK31" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AK10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AZ60" sqref="AY60:AZ60"/>
+      <selection pane="bottomRight" activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="8" width="9.140625" style="1"/>
@@ -19119,25 +19376,25 @@
         <v>404</v>
       </c>
       <c r="AV2" s="4" t="s">
-        <v>1962</v>
+        <v>1959</v>
       </c>
       <c r="AW2" s="1" t="s">
         <v>855</v>
       </c>
       <c r="AY2" s="1" t="s">
-        <v>2040</v>
+        <v>2037</v>
       </c>
       <c r="AZ2" s="12" t="s">
-        <v>2034</v>
+        <v>2031</v>
       </c>
       <c r="BA2" s="1" t="s">
-        <v>1963</v>
+        <v>1960</v>
       </c>
       <c r="BB2" s="1" t="s">
         <v>1184</v>
       </c>
       <c r="BC2" s="1" t="s">
-        <v>1964</v>
+        <v>1961</v>
       </c>
       <c r="BE2" s="4"/>
       <c r="BG2" s="7" t="s">
@@ -19284,16 +19541,16 @@
         <v>784</v>
       </c>
       <c r="AV3" s="4" t="s">
-        <v>1965</v>
+        <v>1962</v>
       </c>
       <c r="AW3" s="1" t="s">
         <v>1639</v>
       </c>
       <c r="AY3" s="1" t="s">
-        <v>1967</v>
+        <v>1964</v>
       </c>
       <c r="AZ3" s="12" t="s">
-        <v>1966</v>
+        <v>1963</v>
       </c>
       <c r="BE3" s="4"/>
       <c r="BG3" s="7" t="s">
@@ -19437,34 +19694,34 @@
         <v>785</v>
       </c>
       <c r="AV4" s="4" t="s">
-        <v>1968</v>
+        <v>1965</v>
       </c>
       <c r="AW4" s="4" t="s">
         <v>1665</v>
       </c>
       <c r="AY4" s="1" t="s">
-        <v>2039</v>
+        <v>2036</v>
       </c>
       <c r="AZ4" s="12" t="s">
-        <v>1982</v>
+        <v>1979</v>
       </c>
       <c r="BA4" s="1" t="s">
-        <v>1969</v>
+        <v>1966</v>
       </c>
       <c r="BB4" s="1" t="s">
         <v>1186</v>
       </c>
       <c r="BC4" s="1" t="s">
+        <v>1967</v>
+      </c>
+      <c r="BD4" s="1" t="s">
+        <v>1968</v>
+      </c>
+      <c r="BE4" s="4" t="s">
+        <v>1969</v>
+      </c>
+      <c r="BF4" s="4" t="s">
         <v>1970</v>
-      </c>
-      <c r="BD4" s="1" t="s">
-        <v>1971</v>
-      </c>
-      <c r="BE4" s="4" t="s">
-        <v>1972</v>
-      </c>
-      <c r="BF4" s="4" t="s">
-        <v>1973</v>
       </c>
       <c r="BG4" s="7" t="s">
         <v>847</v>
@@ -19475,7 +19732,7 @@
         <v>819</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>1775</v>
+        <v>1774</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>1670</v>
@@ -19607,34 +19864,34 @@
         <v>776</v>
       </c>
       <c r="AV5" s="4" t="s">
-        <v>1974</v>
+        <v>1971</v>
       </c>
       <c r="AW5" s="4" t="s">
         <v>870</v>
       </c>
       <c r="AY5" s="4" t="s">
-        <v>2038</v>
+        <v>2035</v>
       </c>
       <c r="AZ5" s="13" t="s">
-        <v>2036</v>
+        <v>2033</v>
       </c>
       <c r="BA5" s="4" t="s">
-        <v>1975</v>
+        <v>1972</v>
       </c>
       <c r="BB5" s="4" t="s">
         <v>1672</v>
       </c>
       <c r="BC5" s="4" t="s">
-        <v>1976</v>
+        <v>1973</v>
       </c>
       <c r="BD5" s="4" t="s">
-        <v>1977</v>
+        <v>1974</v>
       </c>
       <c r="BE5" s="4" t="s">
-        <v>1978</v>
+        <v>1975</v>
       </c>
       <c r="BF5" s="4" t="s">
-        <v>2035</v>
+        <v>2032</v>
       </c>
       <c r="BG5" s="7" t="s">
         <v>847</v>
@@ -19777,25 +20034,25 @@
         <v>786</v>
       </c>
       <c r="AV6" s="4" t="s">
-        <v>1979</v>
+        <v>1976</v>
       </c>
       <c r="AW6" s="1" t="s">
         <v>862</v>
       </c>
       <c r="AY6" s="1" t="s">
-        <v>1980</v>
+        <v>1977</v>
       </c>
       <c r="AZ6" s="12" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="BA6" s="4" t="s">
-        <v>1981</v>
+        <v>1978</v>
       </c>
       <c r="BB6" s="4" t="s">
         <v>1187</v>
       </c>
       <c r="BC6" s="4" t="s">
-        <v>2044</v>
+        <v>2041</v>
       </c>
       <c r="BE6" s="4"/>
       <c r="BG6" s="7" t="s">
@@ -19939,25 +20196,25 @@
         <v>404</v>
       </c>
       <c r="AV7" s="4" t="s">
-        <v>2029</v>
+        <v>2026</v>
       </c>
       <c r="AW7" s="1" t="s">
         <v>863</v>
       </c>
       <c r="AY7" s="1" t="s">
-        <v>2059</v>
+        <v>2056</v>
       </c>
       <c r="AZ7" s="12" t="s">
-        <v>2041</v>
+        <v>2038</v>
       </c>
       <c r="BA7" s="1" t="s">
-        <v>2031</v>
+        <v>2028</v>
       </c>
       <c r="BB7" s="4" t="s">
         <v>1188</v>
       </c>
       <c r="BC7" s="4" t="s">
-        <v>2032</v>
+        <v>2029</v>
       </c>
       <c r="BE7" s="4"/>
       <c r="BG7" s="7" t="s">
@@ -19972,7 +20229,7 @@
         <v>746</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1736</v>
+        <v>1735</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>705</v>
@@ -20101,22 +20358,22 @@
         <v>404</v>
       </c>
       <c r="AV8" s="4" t="s">
-        <v>2030</v>
+        <v>2027</v>
       </c>
       <c r="AY8" s="1" t="s">
-        <v>2042</v>
+        <v>2039</v>
       </c>
       <c r="AZ8" s="12" t="s">
-        <v>2043</v>
+        <v>2040</v>
       </c>
       <c r="BA8" s="1" t="s">
+        <v>1736</v>
+      </c>
+      <c r="BB8" s="1" t="s">
         <v>1737</v>
       </c>
-      <c r="BB8" s="1" t="s">
+      <c r="BC8" s="1" t="s">
         <v>1738</v>
-      </c>
-      <c r="BC8" s="1" t="s">
-        <v>1739</v>
       </c>
       <c r="BE8" s="4"/>
       <c r="BG8" s="7" t="s">
@@ -20266,34 +20523,34 @@
         <v>788</v>
       </c>
       <c r="AV9" s="4" t="s">
-        <v>2033</v>
+        <v>2030</v>
       </c>
       <c r="AW9" s="1" t="s">
         <v>864</v>
       </c>
       <c r="AY9" s="4" t="s">
+        <v>2043</v>
+      </c>
+      <c r="AZ9" s="13" t="s">
+        <v>2042</v>
+      </c>
+      <c r="BA9" s="4" t="s">
         <v>2046</v>
       </c>
-      <c r="AZ9" s="13" t="s">
-        <v>2045</v>
-      </c>
-      <c r="BA9" s="4" t="s">
+      <c r="BB9" s="4" t="s">
+        <v>2047</v>
+      </c>
+      <c r="BC9" s="4" t="s">
+        <v>2048</v>
+      </c>
+      <c r="BD9" s="4" t="s">
         <v>2049</v>
       </c>
-      <c r="BB9" s="4" t="s">
+      <c r="BE9" s="4" t="s">
         <v>2050</v>
       </c>
-      <c r="BC9" s="4" t="s">
-        <v>2051</v>
-      </c>
-      <c r="BD9" s="4" t="s">
-        <v>2052</v>
-      </c>
-      <c r="BE9" s="4" t="s">
-        <v>2053</v>
-      </c>
       <c r="BF9" s="4" t="s">
-        <v>2044</v>
+        <v>2041</v>
       </c>
       <c r="BG9" s="7" t="s">
         <v>847</v>
@@ -20304,13 +20561,13 @@
         <v>821</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>1777</v>
+        <v>1776</v>
       </c>
       <c r="C10" s="4" t="s">
+        <v>1686</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>1687</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>1688</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>1161</v>
@@ -20430,28 +20687,28 @@
         <v>404</v>
       </c>
       <c r="AS10" s="4" t="s">
+        <v>1688</v>
+      </c>
+      <c r="AV10" s="4" t="s">
+        <v>1690</v>
+      </c>
+      <c r="AW10" s="4" t="s">
         <v>1689</v>
       </c>
-      <c r="AV10" s="4" t="s">
-        <v>1691</v>
-      </c>
-      <c r="AW10" s="4" t="s">
-        <v>1690</v>
-      </c>
       <c r="AY10" s="4" t="s">
+        <v>2044</v>
+      </c>
+      <c r="AZ10" s="13" t="s">
+        <v>2045</v>
+      </c>
+      <c r="BA10" s="4" t="s">
+        <v>2046</v>
+      </c>
+      <c r="BB10" s="4" t="s">
         <v>2047</v>
       </c>
-      <c r="AZ10" s="13" t="s">
+      <c r="BC10" s="4" t="s">
         <v>2048</v>
-      </c>
-      <c r="BA10" s="4" t="s">
-        <v>2049</v>
-      </c>
-      <c r="BB10" s="4" t="s">
-        <v>2050</v>
-      </c>
-      <c r="BC10" s="4" t="s">
-        <v>2051</v>
       </c>
       <c r="BG10" s="7" t="s">
         <v>847</v>
@@ -20594,25 +20851,25 @@
         <v>404</v>
       </c>
       <c r="AV11" s="4" t="s">
-        <v>2054</v>
+        <v>2051</v>
       </c>
       <c r="AW11" s="1" t="s">
         <v>856</v>
       </c>
       <c r="AY11" s="1" t="s">
+        <v>2052</v>
+      </c>
+      <c r="AZ11" s="12" t="s">
+        <v>2053</v>
+      </c>
+      <c r="BA11" s="4" t="s">
+        <v>2057</v>
+      </c>
+      <c r="BB11" s="4" t="s">
         <v>2055</v>
       </c>
-      <c r="AZ11" s="12" t="s">
-        <v>2056</v>
-      </c>
-      <c r="BA11" s="4" t="s">
-        <v>2060</v>
-      </c>
-      <c r="BB11" s="4" t="s">
-        <v>2058</v>
-      </c>
       <c r="BC11" s="4" t="s">
-        <v>2057</v>
+        <v>2054</v>
       </c>
       <c r="BE11" s="4"/>
       <c r="BG11" s="7" t="s">
@@ -20621,7 +20878,7 @@
     </row>
     <row r="12" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>747</v>
@@ -20774,7 +21031,7 @@
         <v>1629</v>
       </c>
       <c r="AZ12" s="12" t="s">
-        <v>1763</v>
+        <v>1762</v>
       </c>
       <c r="BE12" s="4"/>
       <c r="BG12" s="7" t="s">
@@ -20921,13 +21178,13 @@
         <v>1229</v>
       </c>
       <c r="AW13" s="4" t="s">
+        <v>1712</v>
+      </c>
+      <c r="AY13" s="1" t="s">
         <v>1713</v>
       </c>
-      <c r="AY13" s="1" t="s">
+      <c r="AZ13" s="12" t="s">
         <v>1714</v>
-      </c>
-      <c r="AZ13" s="12" t="s">
-        <v>1715</v>
       </c>
       <c r="BE13" s="4"/>
       <c r="BG13" s="7" t="s">
@@ -21080,7 +21337,7 @@
         <v>1629</v>
       </c>
       <c r="AZ14" s="13" t="s">
-        <v>1740</v>
+        <v>1739</v>
       </c>
       <c r="BG14" s="7" t="s">
         <v>847</v>
@@ -21091,7 +21348,7 @@
         <v>822</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>1777</v>
+        <v>1776</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>709</v>
@@ -21226,13 +21483,13 @@
         <v>1230</v>
       </c>
       <c r="AW15" s="4" t="s">
-        <v>1692</v>
+        <v>1691</v>
       </c>
       <c r="AY15" s="1" t="s">
         <v>1677</v>
       </c>
       <c r="AZ15" s="13" t="s">
-        <v>1693</v>
+        <v>1692</v>
       </c>
       <c r="BG15" s="7" t="s">
         <v>847</v>
@@ -21243,7 +21500,7 @@
         <v>735</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>1773</v>
+        <v>1772</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>709</v>
@@ -21378,14 +21635,14 @@
         <v>1231</v>
       </c>
       <c r="AW16" s="4" t="s">
-        <v>1721</v>
+        <v>1720</v>
       </c>
       <c r="AX16" s="4"/>
       <c r="AY16" s="1" t="s">
         <v>1677</v>
       </c>
       <c r="AZ16" s="12" t="s">
-        <v>1722</v>
+        <v>1721</v>
       </c>
       <c r="BE16" s="4"/>
       <c r="BG16" s="7" t="s">
@@ -21394,7 +21651,7 @@
     </row>
     <row r="17" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>1767</v>
+        <v>1766</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>747</v>
@@ -21539,7 +21796,7 @@
         <v>1635</v>
       </c>
       <c r="AZ17" s="12" t="s">
-        <v>1744</v>
+        <v>1743</v>
       </c>
       <c r="BA17" s="1" t="s">
         <v>1462</v>
@@ -21568,7 +21825,7 @@
         <v>725</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>1774</v>
+        <v>1773</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>711</v>
@@ -21700,13 +21957,13 @@
         <v>1233</v>
       </c>
       <c r="AW18" s="4" t="s">
-        <v>1716</v>
+        <v>1715</v>
       </c>
       <c r="AY18" s="1" t="s">
         <v>1677</v>
       </c>
       <c r="AZ18" s="13" t="s">
-        <v>1764</v>
+        <v>1763</v>
       </c>
       <c r="BG18" s="7" t="s">
         <v>847</v>
@@ -21717,7 +21974,7 @@
         <v>737</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>1774</v>
+        <v>1773</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>711</v>
@@ -21849,13 +22106,13 @@
         <v>1234</v>
       </c>
       <c r="AW19" s="4" t="s">
-        <v>1717</v>
+        <v>1716</v>
       </c>
       <c r="AY19" s="1" t="s">
         <v>1677</v>
       </c>
       <c r="AZ19" s="13" t="s">
-        <v>1741</v>
+        <v>1740</v>
       </c>
       <c r="BG19" s="7" t="s">
         <v>847</v>
@@ -22013,7 +22270,7 @@
         <v>1629</v>
       </c>
       <c r="AZ20" s="13" t="s">
-        <v>1742</v>
+        <v>1741</v>
       </c>
       <c r="BG20" s="7" t="s">
         <v>847</v>
@@ -22162,7 +22419,7 @@
         <v>1629</v>
       </c>
       <c r="AZ21" s="12" t="s">
-        <v>1743</v>
+        <v>1742</v>
       </c>
       <c r="BE21" s="4"/>
       <c r="BG21" s="7" t="s">
@@ -22319,7 +22576,7 @@
         <v>1630</v>
       </c>
       <c r="AZ22" s="12" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
       <c r="BE22" s="4"/>
       <c r="BG22" s="7" t="s">
@@ -22331,7 +22588,7 @@
         <v>823</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>1775</v>
+        <v>1774</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>707</v>
@@ -22471,7 +22728,7 @@
         <v>1677</v>
       </c>
       <c r="AZ23" s="12" t="s">
-        <v>1746</v>
+        <v>1745</v>
       </c>
       <c r="BA23" s="1" t="s">
         <v>1675</v>
@@ -22492,7 +22749,7 @@
         <v>818</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>1773</v>
+        <v>1772</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>707</v>
@@ -22627,13 +22884,13 @@
         <v>1238</v>
       </c>
       <c r="AW24" s="4" t="s">
-        <v>1723</v>
+        <v>1722</v>
       </c>
       <c r="AY24" s="1" t="s">
         <v>1677</v>
       </c>
       <c r="AZ24" s="13" t="s">
-        <v>1747</v>
+        <v>1746</v>
       </c>
       <c r="BG24" s="7" t="s">
         <v>847</v>
@@ -22788,7 +23045,7 @@
         <v>1629</v>
       </c>
       <c r="AZ25" s="12" t="s">
-        <v>1748</v>
+        <v>1747</v>
       </c>
       <c r="BE25" s="4"/>
       <c r="BG25" s="7" t="s">
@@ -22944,7 +23201,7 @@
         <v>1636</v>
       </c>
       <c r="AZ26" s="12" t="s">
-        <v>1749</v>
+        <v>1748</v>
       </c>
       <c r="BA26" s="1" t="s">
         <v>1461</v>
@@ -22967,7 +23224,7 @@
         <v>723</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>1773</v>
+        <v>1772</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>709</v>
@@ -23105,13 +23362,13 @@
         <v>1241</v>
       </c>
       <c r="AW27" s="4" t="s">
-        <v>1724</v>
+        <v>1723</v>
       </c>
       <c r="AY27" s="1" t="s">
         <v>1677</v>
       </c>
       <c r="AZ27" s="13" t="s">
-        <v>1733</v>
+        <v>1732</v>
       </c>
       <c r="BG27" s="7" t="s">
         <v>847</v>
@@ -23122,7 +23379,7 @@
         <v>733</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>1773</v>
+        <v>1772</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>711</v>
@@ -23257,14 +23514,14 @@
         <v>1242</v>
       </c>
       <c r="AW28" s="4" t="s">
-        <v>1725</v>
+        <v>1724</v>
       </c>
       <c r="AX28" s="4"/>
       <c r="AY28" s="1" t="s">
         <v>1677</v>
       </c>
       <c r="AZ28" s="12" t="s">
-        <v>1734</v>
+        <v>1733</v>
       </c>
       <c r="BE28" s="4"/>
       <c r="BG28" s="7" t="s">
@@ -23273,7 +23530,7 @@
     </row>
     <row r="29" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>1769</v>
+        <v>1768</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>747</v>
@@ -23418,7 +23675,7 @@
         <v>1637</v>
       </c>
       <c r="AZ29" s="12" t="s">
-        <v>1750</v>
+        <v>1749</v>
       </c>
       <c r="BA29" s="1" t="s">
         <v>1460</v>
@@ -23441,7 +23698,7 @@
         <v>740</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>1774</v>
+        <v>1773</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>711</v>
@@ -23573,13 +23830,13 @@
         <v>1244</v>
       </c>
       <c r="AW30" s="4" t="s">
-        <v>1718</v>
+        <v>1717</v>
       </c>
       <c r="AY30" s="1" t="s">
         <v>1677</v>
       </c>
       <c r="AZ30" s="12" t="s">
-        <v>1735</v>
+        <v>1734</v>
       </c>
       <c r="BE30" s="4"/>
       <c r="BG30" s="7" t="s">
@@ -23733,7 +23990,7 @@
         <v>1629</v>
       </c>
       <c r="AZ31" s="12" t="s">
-        <v>1751</v>
+        <v>1750</v>
       </c>
       <c r="BE31" s="4"/>
       <c r="BG31" s="7" t="s">
@@ -23887,7 +24144,7 @@
         <v>1629</v>
       </c>
       <c r="AZ32" s="12" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
       <c r="BE32" s="4"/>
       <c r="BG32" s="7" t="s">
@@ -24040,7 +24297,7 @@
         <v>1629</v>
       </c>
       <c r="AZ33" s="13" t="s">
-        <v>1753</v>
+        <v>1752</v>
       </c>
       <c r="BG33" s="7" t="s">
         <v>847</v>
@@ -24189,7 +24446,7 @@
         <v>1629</v>
       </c>
       <c r="AZ34" s="13" t="s">
-        <v>1754</v>
+        <v>1753</v>
       </c>
       <c r="BG34" s="7" t="s">
         <v>847</v>
@@ -24200,7 +24457,7 @@
         <v>824</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>1776</v>
+        <v>1775</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>704</v>
@@ -24326,25 +24583,25 @@
         <v>404</v>
       </c>
       <c r="AS35" s="4" t="s">
+        <v>1706</v>
+      </c>
+      <c r="AV35" s="4" t="s">
         <v>1707</v>
-      </c>
-      <c r="AV35" s="4" t="s">
-        <v>1708</v>
       </c>
       <c r="AY35" s="1" t="s">
         <v>1677</v>
       </c>
       <c r="AZ35" s="13" t="s">
+        <v>1708</v>
+      </c>
+      <c r="BA35" s="4" t="s">
         <v>1709</v>
       </c>
-      <c r="BA35" s="4" t="s">
+      <c r="BB35" s="4" t="s">
         <v>1710</v>
       </c>
-      <c r="BB35" s="4" t="s">
+      <c r="BC35" s="4" t="s">
         <v>1711</v>
-      </c>
-      <c r="BC35" s="4" t="s">
-        <v>1712</v>
       </c>
       <c r="BG35" s="7" t="s">
         <v>847</v>
@@ -24355,7 +24612,7 @@
         <v>739</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>1783</v>
+        <v>1782</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>704</v>
@@ -24493,7 +24750,7 @@
         <v>1629</v>
       </c>
       <c r="AZ36" s="13" t="s">
-        <v>1755</v>
+        <v>1754</v>
       </c>
       <c r="BE36" s="4"/>
       <c r="BG36" s="7" t="s">
@@ -24505,7 +24762,7 @@
         <v>828</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>1775</v>
+        <v>1774</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>706</v>
@@ -24631,7 +24888,7 @@
         <v>404</v>
       </c>
       <c r="AS37" s="4" t="s">
-        <v>1732</v>
+        <v>1731</v>
       </c>
       <c r="AV37" s="4" t="s">
         <v>404</v>
@@ -24643,7 +24900,7 @@
         <v>1677</v>
       </c>
       <c r="AZ37" s="13" t="s">
-        <v>1756</v>
+        <v>1755</v>
       </c>
       <c r="BE37" s="4"/>
       <c r="BG37" s="7" t="s">
@@ -24793,7 +25050,7 @@
         <v>1629</v>
       </c>
       <c r="AZ38" s="13" t="s">
-        <v>1757</v>
+        <v>1756</v>
       </c>
       <c r="BG38" s="7" t="s">
         <v>847</v>
@@ -24943,10 +25200,10 @@
         <v>1631</v>
       </c>
       <c r="AZ39" s="12" t="s">
-        <v>1758</v>
+        <v>1757</v>
       </c>
       <c r="BA39" s="1" t="s">
-        <v>1727</v>
+        <v>1726</v>
       </c>
       <c r="BB39" s="1" t="s">
         <v>1213</v>
@@ -24964,7 +25221,7 @@
         <v>829</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>1775</v>
+        <v>1774</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>704</v>
@@ -25103,7 +25360,7 @@
         <v>1677</v>
       </c>
       <c r="AZ40" s="12" t="s">
-        <v>1759</v>
+        <v>1758</v>
       </c>
       <c r="BE40" s="4"/>
       <c r="BG40" s="7" t="s">
@@ -25115,7 +25372,7 @@
         <v>722</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>1774</v>
+        <v>1773</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>704</v>
@@ -25250,16 +25507,16 @@
         <v>1677</v>
       </c>
       <c r="AZ41" s="13" t="s">
-        <v>1760</v>
+        <v>1759</v>
       </c>
       <c r="BA41" s="4" t="s">
-        <v>1726</v>
+        <v>1725</v>
       </c>
       <c r="BB41" s="1" t="s">
+        <v>1727</v>
+      </c>
+      <c r="BC41" s="4" t="s">
         <v>1728</v>
-      </c>
-      <c r="BC41" s="4" t="s">
-        <v>1729</v>
       </c>
       <c r="BG41" s="7" t="s">
         <v>847</v>
@@ -25411,7 +25668,7 @@
         <v>1638</v>
       </c>
       <c r="AZ42" s="12" t="s">
-        <v>1761</v>
+        <v>1760</v>
       </c>
       <c r="BA42" s="1" t="s">
         <v>1459</v>
@@ -25573,7 +25830,7 @@
         <v>1632</v>
       </c>
       <c r="AZ43" s="12" t="s">
-        <v>1762</v>
+        <v>1761</v>
       </c>
       <c r="BA43" s="1" t="s">
         <v>1457</v>
@@ -25594,7 +25851,7 @@
         <v>825</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>1686</v>
+        <v>1685</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>704</v>
@@ -25726,13 +25983,13 @@
         <v>404</v>
       </c>
       <c r="AW44" s="1" t="s">
-        <v>1730</v>
+        <v>1729</v>
       </c>
       <c r="AY44" s="1" t="s">
         <v>1629</v>
       </c>
       <c r="AZ44" s="12" t="s">
-        <v>1731</v>
+        <v>1730</v>
       </c>
       <c r="BE44" s="4"/>
       <c r="BG44" s="7" t="s">
@@ -25744,7 +26001,7 @@
         <v>726</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>1774</v>
+        <v>1773</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>704</v>
@@ -25876,13 +26133,13 @@
         <v>1254</v>
       </c>
       <c r="AW45" s="4" t="s">
-        <v>1719</v>
+        <v>1718</v>
       </c>
       <c r="AY45" s="1" t="s">
         <v>1677</v>
       </c>
       <c r="AZ45" s="13" t="s">
-        <v>1720</v>
+        <v>1719</v>
       </c>
       <c r="BG45" s="7" t="s">
         <v>847</v>
@@ -25893,7 +26150,7 @@
         <v>826</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>1776</v>
+        <v>1775</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>704</v>
@@ -26019,25 +26276,25 @@
         <v>1228</v>
       </c>
       <c r="AV46" s="4" t="s">
-        <v>1705</v>
+        <v>1704</v>
       </c>
       <c r="AW46" s="4" t="s">
-        <v>1701</v>
+        <v>1700</v>
       </c>
       <c r="AY46" s="1" t="s">
         <v>1677</v>
       </c>
       <c r="AZ46" s="13" t="s">
-        <v>1704</v>
+        <v>1703</v>
       </c>
       <c r="BA46" s="4" t="s">
+        <v>1701</v>
+      </c>
+      <c r="BB46" s="4" t="s">
         <v>1702</v>
       </c>
-      <c r="BB46" s="4" t="s">
-        <v>1703</v>
-      </c>
       <c r="BC46" s="4" t="s">
-        <v>1706</v>
+        <v>1705</v>
       </c>
       <c r="BG46" s="7" t="s">
         <v>847</v>
@@ -26048,7 +26305,7 @@
         <v>827</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>1777</v>
+        <v>1776</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>704</v>
@@ -26174,25 +26431,25 @@
         <v>1228</v>
       </c>
       <c r="AV47" s="4" t="s">
-        <v>1696</v>
+        <v>1695</v>
       </c>
       <c r="AW47" s="4" t="s">
-        <v>1694</v>
+        <v>1693</v>
       </c>
       <c r="AY47" s="1" t="s">
         <v>1677</v>
       </c>
       <c r="AZ47" s="13" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="BA47" s="4" t="s">
+        <v>1696</v>
+      </c>
+      <c r="BB47" s="4" t="s">
         <v>1697</v>
       </c>
-      <c r="BB47" s="4" t="s">
+      <c r="BC47" s="4" t="s">
         <v>1698</v>
-      </c>
-      <c r="BC47" s="4" t="s">
-        <v>1699</v>
       </c>
       <c r="BG47" s="7" t="s">
         <v>847</v>
@@ -26366,7 +26623,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -26908,7 +27170,10 @@
   <dimension ref="A1:H86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>